<commit_message>
code and worktyple table adjust
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnpc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnpc/locale/locale-en.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="language" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1686" uniqueCount="1183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1668" uniqueCount="1172">
   <si>
     <t>myself</t>
   </si>
@@ -4035,15 +4035,9 @@
     <t>APPLICATIONSCENARIOS</t>
   </si>
   <si>
-    <t>煤层气井</t>
-  </si>
-  <si>
     <t>应用场景</t>
   </si>
   <si>
-    <t>油井</t>
-  </si>
-  <si>
     <t>正常</t>
   </si>
   <si>
@@ -4132,9 +4126,6 @@
     <t>ru</t>
   </si>
   <si>
-    <t>其他</t>
-  </si>
-  <si>
     <t>MD_TYPE</t>
   </si>
   <si>
@@ -4162,36 +4153,6 @@
     <t>TXBJYSTMD</t>
   </si>
   <si>
-    <t>USER_TITLE</t>
-  </si>
-  <si>
-    <t>中控室</t>
-  </si>
-  <si>
-    <t>工况巡检一组</t>
-  </si>
-  <si>
-    <t>工况巡检二组</t>
-  </si>
-  <si>
-    <t>工况巡检三组</t>
-  </si>
-  <si>
-    <t>工况巡检四组</t>
-  </si>
-  <si>
-    <t>USER_TYPE</t>
-  </si>
-  <si>
-    <t>数据分析员</t>
-  </si>
-  <si>
-    <t>系统管理员</t>
-  </si>
-  <si>
-    <t>数据管理员</t>
-  </si>
-  <si>
     <t>YXBJQJYS</t>
   </si>
   <si>
@@ -4201,9 +4162,6 @@
     <t>YXBJYSTMD</t>
   </si>
   <si>
-    <t>alarmType</t>
-  </si>
-  <si>
     <t>开关量报警</t>
   </si>
   <si>
@@ -4224,10 +4182,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>RESULENAME</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>RESULTDESCRIPTION</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4533,6 +4487,22 @@
   </si>
   <si>
     <t>data export</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALARMTYPE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cbm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>oil</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RESULTNAME</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5481,7 +5451,7 @@
         <v>5</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1169</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -9268,7 +9238,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>1167</v>
+        <v>1152</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>428</v>
@@ -15222,10 +15192,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G86"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -15243,7 +15213,7 @@
         <v>1016</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1164</v>
+        <v>1149</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1017</v>
@@ -15269,7 +15239,7 @@
         <v>1022</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>1170</v>
+        <v>1155</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -15286,7 +15256,7 @@
         <v>1022</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>1171</v>
+        <v>1156</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -15303,7 +15273,7 @@
         <v>1022</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>1172</v>
+        <v>1157</v>
       </c>
       <c r="D4" s="1">
         <v>2</v>
@@ -15320,7 +15290,7 @@
         <v>1022</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>1173</v>
+        <v>1158</v>
       </c>
       <c r="D5" s="1">
         <v>3</v>
@@ -15337,7 +15307,7 @@
         <v>1023</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>1024</v>
+        <v>1169</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -15345,7 +15315,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -15356,7 +15326,7 @@
         <v>1023</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>1026</v>
+        <v>1170</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -15364,7 +15334,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -15372,10 +15342,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1165</v>
+        <v>1150</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>1166</v>
+        <v>1151</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
@@ -15389,7 +15359,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>1165</v>
+        <v>1150</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>235</v>
@@ -15406,7 +15376,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>1165</v>
+        <v>1150</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>236</v>
@@ -15423,7 +15393,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>1165</v>
+        <v>1150</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>237</v>
@@ -15440,10 +15410,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>1165</v>
+        <v>1150</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>1168</v>
+        <v>1153</v>
       </c>
       <c r="D12" s="1">
         <v>400</v>
@@ -15457,10 +15427,10 @@
         <v>27</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
@@ -15474,10 +15444,10 @@
         <v>28</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>1030</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>1032</v>
       </c>
       <c r="D14" s="1">
         <v>100</v>
@@ -15491,10 +15461,10 @@
         <v>29</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="D15" s="1">
         <v>200</v>
@@ -15508,10 +15478,10 @@
         <v>30</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="D16" s="1">
         <v>300</v>
@@ -15525,10 +15495,10 @@
         <v>31</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
@@ -15542,10 +15512,10 @@
         <v>32</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="D18" s="1">
         <v>100</v>
@@ -15559,10 +15529,10 @@
         <v>33</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="D19" s="1">
         <v>200</v>
@@ -15576,10 +15546,10 @@
         <v>34</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="D20" s="1">
         <v>300</v>
@@ -15593,10 +15563,10 @@
         <v>35</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>1035</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>1037</v>
       </c>
       <c r="D21" s="1">
         <v>400</v>
@@ -15610,7 +15580,7 @@
         <v>36</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="C22" s="5">
         <v>0</v>
@@ -15627,7 +15597,7 @@
         <v>37</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="C23" s="5">
         <v>0</v>
@@ -15644,7 +15614,7 @@
         <v>38</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="C24" s="5">
         <v>0</v>
@@ -15661,7 +15631,7 @@
         <v>39</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="C25" s="5">
         <v>0</v>
@@ -15678,7 +15648,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="C26" s="5">
         <v>0</v>
@@ -15695,7 +15665,7 @@
         <v>41</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="C27" s="5">
         <v>0</v>
@@ -15712,7 +15682,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="C28" s="5">
         <v>0</v>
@@ -15729,7 +15699,7 @@
         <v>43</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="C29" s="5">
         <v>0</v>
@@ -15746,10 +15716,10 @@
         <v>46</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="D30" s="1">
         <v>101</v>
@@ -15763,10 +15733,10 @@
         <v>47</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>1040</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>1042</v>
       </c>
       <c r="D31" s="1">
         <v>201</v>
@@ -15780,10 +15750,10 @@
         <v>48</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="D32" s="1">
         <v>300</v>
@@ -15797,10 +15767,10 @@
         <v>49</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>1174</v>
+        <v>1159</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="D33" s="1">
         <v>-44</v>
@@ -15814,10 +15784,10 @@
         <v>50</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>1174</v>
+        <v>1159</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="D34" s="1">
         <v>-55</v>
@@ -15831,10 +15801,10 @@
         <v>51</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>1174</v>
+        <v>1159</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="D35" s="1">
         <v>-66</v>
@@ -15848,10 +15818,10 @@
         <v>52</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>1174</v>
+        <v>1159</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="D36" s="1">
         <v>-77</v>
@@ -15865,10 +15835,10 @@
         <v>53</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>1174</v>
+        <v>1159</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="D37" s="1">
         <v>-88</v>
@@ -15882,10 +15852,10 @@
         <v>54</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>1174</v>
+        <v>1159</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="D38" s="1">
         <v>-99</v>
@@ -15899,10 +15869,10 @@
         <v>55</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>1174</v>
+        <v>1159</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="D39" s="1">
         <v>0</v>
@@ -15916,10 +15886,10 @@
         <v>56</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>1174</v>
+        <v>1159</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="D40" s="1">
         <v>1</v>
@@ -15933,10 +15903,10 @@
         <v>57</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="D41" s="1">
         <v>1</v>
@@ -15950,10 +15920,10 @@
         <v>58</v>
       </c>
       <c r="B42" s="5" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>1052</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>1054</v>
       </c>
       <c r="D42" s="1">
         <v>2</v>
@@ -15967,10 +15937,10 @@
         <v>59</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="D43" s="1">
         <v>3</v>
@@ -15984,10 +15954,10 @@
         <v>80</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>1175</v>
+        <v>1160</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>1176</v>
+        <v>1161</v>
       </c>
       <c r="D44" s="1">
         <v>0</v>
@@ -16001,10 +15971,10 @@
         <v>81</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>1177</v>
+        <v>1162</v>
       </c>
       <c r="D45" s="1">
         <v>2</v>
@@ -16018,10 +15988,10 @@
         <v>90</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
       <c r="D46" s="1">
         <v>1</v>
@@ -16035,10 +16005,10 @@
         <v>91</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
       <c r="D47" s="1">
         <v>2</v>
@@ -16052,10 +16022,10 @@
         <v>94</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>1178</v>
+        <v>1163</v>
       </c>
       <c r="D48" s="1">
         <v>0</v>
@@ -16069,10 +16039,10 @@
         <v>95</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>1179</v>
+        <v>1164</v>
       </c>
       <c r="D49" s="1">
         <v>1</v>
@@ -16086,10 +16056,10 @@
         <v>96</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>1180</v>
+        <v>1165</v>
       </c>
       <c r="D50" s="1">
         <v>2</v>
@@ -16103,10 +16073,10 @@
         <v>97</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>1181</v>
+        <v>1166</v>
       </c>
       <c r="D51" s="1">
         <v>3</v>
@@ -16120,10 +16090,10 @@
         <v>98</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>1182</v>
+        <v>1167</v>
       </c>
       <c r="D52" s="1">
         <v>4</v>
@@ -16137,10 +16107,10 @@
         <v>99</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>1063</v>
+        <v>1060</v>
       </c>
       <c r="D53" s="1">
         <v>0</v>
@@ -16154,10 +16124,10 @@
         <v>100</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="D54" s="1">
         <v>1</v>
@@ -16171,10 +16141,10 @@
         <v>101</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="D55" s="1">
         <v>2</v>
@@ -16188,10 +16158,10 @@
         <v>102</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>1063</v>
+        <v>1060</v>
       </c>
       <c r="D56" s="1">
         <v>0</v>
@@ -16205,10 +16175,10 @@
         <v>103</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="D57" s="1">
         <v>1</v>
@@ -16222,10 +16192,10 @@
         <v>104</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="D58" s="1">
         <v>2</v>
@@ -16239,7 +16209,7 @@
         <v>105</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="C59" s="5">
         <v>0</v>
@@ -16256,7 +16226,7 @@
         <v>106</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="C60" s="5">
         <v>0</v>
@@ -16273,7 +16243,7 @@
         <v>107</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="C61" s="5">
         <v>0</v>
@@ -16287,13 +16257,13 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>1067</v>
+        <v>1030</v>
       </c>
       <c r="D62" s="1">
         <v>0</v>
@@ -16304,13 +16274,13 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>1068</v>
+        <v>1034</v>
       </c>
       <c r="D63" s="1">
         <v>1</v>
@@ -16321,13 +16291,13 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>1069</v>
+        <v>1031</v>
       </c>
       <c r="D64" s="1">
         <v>2</v>
@@ -16338,16 +16308,16 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>1070</v>
+        <v>1030</v>
       </c>
       <c r="D65" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
@@ -16355,16 +16325,16 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>1071</v>
+        <v>1034</v>
       </c>
       <c r="D66" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
@@ -16372,16 +16342,16 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>1056</v>
+        <v>1031</v>
       </c>
       <c r="D67" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
@@ -16389,13 +16359,13 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>1072</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>1073</v>
+        <v>1065</v>
+      </c>
+      <c r="C68" s="5">
+        <v>0</v>
       </c>
       <c r="D68" s="1">
         <v>0</v>
@@ -16406,13 +16376,13 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>1072</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>1074</v>
+        <v>1065</v>
+      </c>
+      <c r="C69" s="5">
+        <v>0</v>
       </c>
       <c r="D69" s="1">
         <v>1</v>
@@ -16423,13 +16393,13 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>1072</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>1075</v>
+        <v>1065</v>
+      </c>
+      <c r="C70" s="5">
+        <v>0</v>
       </c>
       <c r="D70" s="1">
         <v>2</v>
@@ -16440,13 +16410,13 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>1076</v>
+        <v>1168</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>1032</v>
+        <v>1066</v>
       </c>
       <c r="D71" s="1">
         <v>0</v>
@@ -16457,13 +16427,13 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>1076</v>
+        <v>1168</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>1036</v>
+        <v>1067</v>
       </c>
       <c r="D72" s="1">
         <v>1</v>
@@ -16474,13 +16444,13 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>1076</v>
+        <v>1168</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>1033</v>
+        <v>1068</v>
       </c>
       <c r="D73" s="1">
         <v>2</v>
@@ -16491,16 +16461,16 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>1077</v>
+        <v>1168</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>1032</v>
+        <v>1069</v>
       </c>
       <c r="D74" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
@@ -16508,16 +16478,16 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>1077</v>
+        <v>1168</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>1036</v>
+        <v>1026</v>
       </c>
       <c r="D75" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
@@ -16525,16 +16495,16 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>1077</v>
+        <v>1168</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>1033</v>
+        <v>1068</v>
       </c>
       <c r="D76" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
@@ -16542,173 +16512,20 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>1078</v>
-      </c>
-      <c r="C77" s="5">
-        <v>0</v>
+        <v>1168</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>1027</v>
       </c>
       <c r="D77" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
-        <v>124</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>1078</v>
-      </c>
-      <c r="C78" s="5">
-        <v>0</v>
-      </c>
-      <c r="D78" s="1">
-        <v>1</v>
-      </c>
-      <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
-      <c r="G78" s="1"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
-        <v>125</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>1078</v>
-      </c>
-      <c r="C79" s="5">
-        <v>0</v>
-      </c>
-      <c r="D79" s="1">
-        <v>2</v>
-      </c>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
-      <c r="G79" s="1"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
-        <v>126</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>1079</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>1080</v>
-      </c>
-      <c r="D80" s="1">
-        <v>0</v>
-      </c>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
-        <v>127</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>1079</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>1081</v>
-      </c>
-      <c r="D81" s="1">
-        <v>1</v>
-      </c>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
-        <v>128</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>1079</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>1082</v>
-      </c>
-      <c r="D82" s="1">
-        <v>2</v>
-      </c>
-      <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
-        <v>129</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>1079</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>1083</v>
-      </c>
-      <c r="D83" s="1">
-        <v>3</v>
-      </c>
-      <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
-        <v>130</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>1079</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>1028</v>
-      </c>
-      <c r="D84" s="1">
-        <v>4</v>
-      </c>
-      <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
-        <v>131</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>1079</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>1082</v>
-      </c>
-      <c r="D85" s="1">
-        <v>5</v>
-      </c>
-      <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
-      <c r="G85" s="1"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
-        <v>132</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>1079</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>1029</v>
-      </c>
-      <c r="D86" s="1">
-        <v>6</v>
-      </c>
-      <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
-      <c r="G86" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -16720,12 +16537,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="26.77734375" customWidth="1"/>
     <col min="4" max="4" width="93.109375" customWidth="1"/>
     <col min="5" max="5" width="19.109375" customWidth="1"/>
@@ -16735,25 +16553,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>1084</v>
+        <v>1070</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1085</v>
+        <v>1071</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1086</v>
+        <v>1171</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1087</v>
+        <v>1072</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1088</v>
+        <v>1073</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>1089</v>
+        <v>1074</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>1090</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -16764,14 +16582,14 @@
         <v>1201</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1091</v>
+        <v>1076</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1092</v>
+        <v>1077</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>1093</v>
+        <v>1078</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -16783,14 +16601,14 @@
         <v>1202</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1094</v>
+        <v>1079</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>1093</v>
+        <v>1078</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -16802,14 +16620,14 @@
         <v>1203</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1095</v>
+        <v>1080</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1096</v>
+        <v>1081</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>1093</v>
+        <v>1078</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -16821,14 +16639,14 @@
         <v>1204</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1097</v>
+        <v>1082</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1098</v>
+        <v>1083</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>1099</v>
+        <v>1084</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -16840,14 +16658,14 @@
         <v>1205</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1100</v>
+        <v>1085</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>1101</v>
+        <v>1086</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>1099</v>
+        <v>1084</v>
       </c>
       <c r="G6" s="1"/>
     </row>
@@ -16859,14 +16677,14 @@
         <v>1206</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1102</v>
+        <v>1087</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1103</v>
+        <v>1088</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>1099</v>
+        <v>1084</v>
       </c>
       <c r="G7" s="1"/>
     </row>
@@ -16878,14 +16696,14 @@
         <v>1207</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1104</v>
+        <v>1089</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>1105</v>
+        <v>1090</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>1106</v>
+        <v>1091</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -16897,14 +16715,14 @@
         <v>1208</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1107</v>
+        <v>1092</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1108</v>
+        <v>1093</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>1109</v>
+        <v>1094</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -16916,14 +16734,14 @@
         <v>1209</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1110</v>
+        <v>1095</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>1111</v>
+        <v>1096</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>1109</v>
+        <v>1094</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -16935,14 +16753,14 @@
         <v>1210</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1112</v>
+        <v>1097</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>1113</v>
+        <v>1098</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>1114</v>
+        <v>1099</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -16954,14 +16772,14 @@
         <v>1211</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1115</v>
+        <v>1100</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>1116</v>
+        <v>1101</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>1117</v>
+        <v>1102</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -16973,14 +16791,14 @@
         <v>1212</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1118</v>
+        <v>1103</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>1119</v>
+        <v>1104</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>1120</v>
+        <v>1105</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -16992,14 +16810,14 @@
         <v>1213</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1121</v>
+        <v>1106</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>1122</v>
+        <v>1107</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>1120</v>
+        <v>1105</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -17011,14 +16829,14 @@
         <v>1214</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1123</v>
+        <v>1108</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>1124</v>
+        <v>1109</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>1120</v>
+        <v>1105</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -17030,14 +16848,14 @@
         <v>1215</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1125</v>
+        <v>1110</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>1126</v>
+        <v>1111</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>1127</v>
+        <v>1112</v>
       </c>
       <c r="G16" s="1"/>
     </row>
@@ -17049,14 +16867,14 @@
         <v>1216</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1128</v>
+        <v>1113</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>1129</v>
+        <v>1114</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>1120</v>
+        <v>1105</v>
       </c>
       <c r="G17" s="1"/>
     </row>
@@ -17068,14 +16886,14 @@
         <v>1217</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1130</v>
+        <v>1115</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>1131</v>
+        <v>1116</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
-        <v>1120</v>
+        <v>1105</v>
       </c>
       <c r="G18" s="1"/>
     </row>
@@ -17087,14 +16905,14 @@
         <v>1218</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1132</v>
+        <v>1117</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>1133</v>
+        <v>1118</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
-        <v>1134</v>
+        <v>1119</v>
       </c>
       <c r="G19" s="1"/>
     </row>
@@ -17106,14 +16924,14 @@
         <v>1219</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1135</v>
+        <v>1120</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>1136</v>
+        <v>1121</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
-        <v>1137</v>
+        <v>1122</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -17125,14 +16943,14 @@
         <v>1220</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1138</v>
+        <v>1123</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>1126</v>
+        <v>1111</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>1139</v>
+        <v>1124</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -17144,14 +16962,14 @@
         <v>1221</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1140</v>
+        <v>1125</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>1141</v>
+        <v>1126</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>1142</v>
+        <v>1127</v>
       </c>
       <c r="G22" s="1"/>
     </row>
@@ -17163,14 +16981,14 @@
         <v>1222</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1143</v>
+        <v>1128</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>1144</v>
+        <v>1129</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>1145</v>
+        <v>1130</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -17182,14 +17000,14 @@
         <v>1223</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>1146</v>
+        <v>1131</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>1147</v>
+        <v>1132</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>1148</v>
+        <v>1133</v>
       </c>
       <c r="G24" s="1"/>
     </row>
@@ -17201,14 +17019,14 @@
         <v>1224</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>1149</v>
+        <v>1134</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>1150</v>
+        <v>1135</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>1106</v>
+        <v>1091</v>
       </c>
       <c r="G25" s="1"/>
     </row>
@@ -17220,12 +17038,12 @@
         <v>1225</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>1151</v>
+        <v>1136</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>1106</v>
+        <v>1091</v>
       </c>
       <c r="G26" s="1"/>
     </row>
@@ -17237,14 +17055,14 @@
         <v>1226</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>1152</v>
+        <v>1137</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>1153</v>
+        <v>1138</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>1154</v>
+        <v>1139</v>
       </c>
       <c r="G27" s="1"/>
     </row>
@@ -17256,12 +17074,12 @@
         <v>1227</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>1155</v>
+        <v>1140</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
-        <v>1154</v>
+        <v>1139</v>
       </c>
       <c r="G28" s="1"/>
     </row>
@@ -17273,14 +17091,14 @@
         <v>1230</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>1156</v>
+        <v>1141</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>1157</v>
+        <v>1142</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
-        <v>1158</v>
+        <v>1143</v>
       </c>
       <c r="G29" s="1"/>
     </row>
@@ -17292,12 +17110,12 @@
         <v>1231</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>1159</v>
+        <v>1144</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1" t="s">
-        <v>1160</v>
+        <v>1145</v>
       </c>
       <c r="G30" s="1"/>
     </row>
@@ -17309,12 +17127,12 @@
         <v>1232</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>1161</v>
+        <v>1146</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>1162</v>
+        <v>1147</v>
       </c>
       <c r="G31" s="1"/>
     </row>
@@ -17326,7 +17144,7 @@
         <v>1302</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>1163</v>
+        <v>1148</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>

</xml_diff>

<commit_message>
RPC was changed to SRP
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnpc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnpc/locale/locale-en.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="language" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="module" sheetId="4" r:id="rId4"/>
     <sheet name="tbl_code" sheetId="5" r:id="rId5"/>
     <sheet name="worktype" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1668" uniqueCount="1172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1614" uniqueCount="1174">
   <si>
     <t>myself</t>
   </si>
@@ -4044,37 +4045,6 @@
     <t>运行状态报警</t>
   </si>
   <si>
-    <t>BJQJYS</t>
-  </si>
-  <si>
-    <t>000000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dc2828</t>
-  </si>
-  <si>
-    <t>f09614</t>
-  </si>
-  <si>
-    <t>fae600</t>
-  </si>
-  <si>
-    <t>BJYS</t>
-  </si>
-  <si>
-    <t>00ff00</t>
-  </si>
-  <si>
-    <t>#808080</t>
-  </si>
-  <si>
-    <t>BJYSTMD</t>
-  </si>
-  <si>
-    <t>BJYSTMD3</t>
-  </si>
-  <si>
     <t>DEVICETYPE</t>
   </si>
   <si>
@@ -4126,39 +4096,9 @@
     <t>MD_TYPE</t>
   </si>
   <si>
-    <t>PROTOCOL</t>
-  </si>
-  <si>
-    <t>modbus-tcp</t>
-  </si>
-  <si>
-    <t>modbus-rtu</t>
-  </si>
-  <si>
     <t>SYSTEMACTION</t>
   </si>
   <si>
-    <t>TXBJQJYS</t>
-  </si>
-  <si>
-    <t>6c6262</t>
-  </si>
-  <si>
-    <t>TXBJYS</t>
-  </si>
-  <si>
-    <t>TXBJYSTMD</t>
-  </si>
-  <si>
-    <t>YXBJQJYS</t>
-  </si>
-  <si>
-    <t>YXBJYS</t>
-  </si>
-  <si>
-    <t>YXBJYSTMD</t>
-  </si>
-  <si>
     <t>开关量报警</t>
   </si>
   <si>
@@ -4187,328 +4127,405 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>REMARK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ITEMCODE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALARMLEVEL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>normal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>offline</t>
+  </si>
+  <si>
+    <t>offline</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>control</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RESULTSTATUS</t>
+  </si>
+  <si>
+    <t>MD_TYPE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>disable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user login</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user exit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>driver configuration</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>module access</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>data export</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALARMTYPE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cbm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>oil</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RESULTNAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>code1202</t>
+  </si>
+  <si>
+    <t>code1203</t>
+  </si>
+  <si>
+    <t>code1204</t>
+  </si>
+  <si>
+    <t>code1205</t>
+  </si>
+  <si>
+    <t>code1206</t>
+  </si>
+  <si>
+    <t>code1207</t>
+  </si>
+  <si>
+    <t>code1208</t>
+  </si>
+  <si>
+    <t>code1209</t>
+  </si>
+  <si>
+    <t>code1210</t>
+  </si>
+  <si>
+    <t>code1211</t>
+  </si>
+  <si>
+    <t>code1212</t>
+  </si>
+  <si>
+    <t>code1213</t>
+  </si>
+  <si>
+    <t>code1214</t>
+  </si>
+  <si>
+    <t>code1215</t>
+  </si>
+  <si>
+    <t>code1216</t>
+  </si>
+  <si>
+    <t>code1217</t>
+  </si>
+  <si>
+    <t>code1218</t>
+  </si>
+  <si>
+    <t>code1219</t>
+  </si>
+  <si>
+    <t>code1220</t>
+  </si>
+  <si>
+    <t>code1221</t>
+  </si>
+  <si>
+    <t>code1222</t>
+  </si>
+  <si>
+    <t>code1223</t>
+  </si>
+  <si>
+    <t>code1224</t>
+  </si>
+  <si>
+    <t>code1225</t>
+  </si>
+  <si>
+    <t>code1226</t>
+  </si>
+  <si>
+    <t>code1227</t>
+  </si>
+  <si>
+    <t>code1230</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>code1231</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>code1232</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>code1201</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>suggestion1201</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>OPTIMIZATIONSUGGESTION</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>REMARK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>图形在下理论载荷线附近，呈条带状；动液面接近于井口；产量较高，接近或大于理论排量。</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>图形呈平行四边形；充满系数≥0.6。</t>
-  </si>
-  <si>
-    <t>图形四角明显呈角度；增、卸载线平行；0.3≤充满系数﹤0.6。</t>
-  </si>
-  <si>
-    <t>图形四角明显呈角度；0.1≤充满系数﹤0.3；沉没度较低。</t>
-  </si>
-  <si>
-    <t>间抽或降低冲次</t>
-  </si>
-  <si>
-    <t>图形下面部分呈角度；充满系数﹤0.1。</t>
-  </si>
-  <si>
-    <t>图形呈条状；产量为零。</t>
-  </si>
-  <si>
-    <t>充满系数﹤0.3；沉没度较高。</t>
-  </si>
-  <si>
-    <t>洗井或加药</t>
-  </si>
-  <si>
-    <t>图形靠近上理论载荷线；增、卸载过程缓慢，卸载线平缓；产量为零。</t>
-  </si>
-  <si>
-    <t>合理控制气体</t>
-  </si>
-  <si>
-    <t>图形四角圆滑呈弧度，气油比越高，圆弧的曲率半径越大；增载缓慢，增、卸载线不明显。</t>
-  </si>
-  <si>
-    <t>图形上部分倾斜；图形上、下载荷线不平行。</t>
-  </si>
-  <si>
-    <t>检泵</t>
-  </si>
-  <si>
-    <t>图形呈条带状；图形在下理论载荷线附近；产量下降。</t>
-  </si>
-  <si>
-    <t>油管打压试验</t>
-  </si>
-  <si>
-    <t>图形上部分圆滑、缺损；上载荷线低于上理论载荷线；增载过程缓慢，卸载提前。</t>
-  </si>
-  <si>
-    <t>洗井、碰泵或检泵</t>
-  </si>
-  <si>
-    <t>图形下部分圆滑、缺损；下载荷线高于下理论载荷线；增载提前，卸载过程缓慢。</t>
-  </si>
-  <si>
-    <t>图形呈椭圆状；图形在上、下理论载荷线之间；漏失严重时，油井不出油。</t>
-  </si>
-  <si>
-    <t>图形呈条带状；图形在下理论载荷线附近；产量为零。</t>
-  </si>
-  <si>
-    <t>洗井、碰泵或检泵/打压、更换油管</t>
-  </si>
-  <si>
-    <t>图形呈条带状；图形在上理论载荷线附近；产量为零。</t>
-  </si>
-  <si>
-    <t>图形呈条带状；图形在上、下理论载荷线之间；产量为零。</t>
-  </si>
-  <si>
-    <t>图形右上角凸起。</t>
-  </si>
-  <si>
-    <t>校正井口设备</t>
-  </si>
-  <si>
-    <t>图形左下角拖尾。</t>
-  </si>
-  <si>
-    <t>上提（增大）防冲距</t>
-  </si>
-  <si>
-    <t>检泵/下放（缩小）防冲距</t>
-  </si>
-  <si>
-    <t>图形右边缺损；右下角拖尾；增载过程中突然卸载。</t>
-  </si>
-  <si>
-    <t>下放（缩小）防冲距</t>
-  </si>
-  <si>
-    <t>图形呈条带状，两端尖；图形在下理论载荷线下方，断杆位置距井口越近图形越下移；产量突然为零。</t>
-  </si>
-  <si>
-    <t>替换抽油杆</t>
-  </si>
-  <si>
-    <t>图形呈斜条带状；可通过图形拐点找到被卡位置；油井不出油。</t>
-  </si>
-  <si>
-    <t>洗井或检泵</t>
-  </si>
-  <si>
-    <t>图形肥大；产量下降。</t>
-  </si>
-  <si>
-    <t>图形呈不规则、不重复的锯齿状；油井出油正常。</t>
-  </si>
-  <si>
-    <t>防砂</t>
-  </si>
-  <si>
-    <t>图形顺时针偏转。</t>
-  </si>
-  <si>
-    <t>降低冲次</t>
-  </si>
-  <si>
-    <t>优化抽油杆柱组合</t>
-  </si>
-  <si>
-    <t>检查采集仪表</t>
-  </si>
-  <si>
-    <t>ITEMCODE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALARMLEVEL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>normal</t>
-  </si>
-  <si>
-    <t>normal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>offline</t>
-  </si>
-  <si>
-    <t>offline</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>add</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>update</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>delete</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>control</t>
+    <t>suggestion1202</t>
+  </si>
+  <si>
+    <t>suggestion1203</t>
+  </si>
+  <si>
+    <t>suggestion1204</t>
+  </si>
+  <si>
+    <t>suggestion1205</t>
+  </si>
+  <si>
+    <t>suggestion1206</t>
+  </si>
+  <si>
+    <t>suggestion1207</t>
+  </si>
+  <si>
+    <t>suggestion1208</t>
+  </si>
+  <si>
+    <t>suggestion1209</t>
+  </si>
+  <si>
+    <t>suggestion1210</t>
+  </si>
+  <si>
+    <t>suggestion1211</t>
+  </si>
+  <si>
+    <t>suggestion1212</t>
+  </si>
+  <si>
+    <t>suggestion1213</t>
+  </si>
+  <si>
+    <t>suggestion1214</t>
+  </si>
+  <si>
+    <t>suggestion1215</t>
+  </si>
+  <si>
+    <t>suggestion1216</t>
+  </si>
+  <si>
+    <t>suggestion1217</t>
+  </si>
+  <si>
+    <t>suggestion1218</t>
+  </si>
+  <si>
+    <t>suggestion1219</t>
+  </si>
+  <si>
+    <t>suggestion1220</t>
+  </si>
+  <si>
+    <t>suggestion1221</t>
+  </si>
+  <si>
+    <t>suggestion1222</t>
+  </si>
+  <si>
+    <t>suggestion1223</t>
+  </si>
+  <si>
+    <t>suggestion1224</t>
+  </si>
+  <si>
+    <t>suggestion1225</t>
+  </si>
+  <si>
+    <t>suggestion1226</t>
+  </si>
+  <si>
+    <t>suggestion1227</t>
+  </si>
+  <si>
+    <t>suggestion1230</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>suggestion1231</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>suggestion1232</t>
+  </si>
+  <si>
+    <t>code1302</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>suggestion1302</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>description1201</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>description1202</t>
+  </si>
+  <si>
+    <t>description1203</t>
+  </si>
+  <si>
+    <t>description1204</t>
+  </si>
+  <si>
+    <t>description1205</t>
+  </si>
+  <si>
+    <t>description1206</t>
+  </si>
+  <si>
+    <t>description1207</t>
+  </si>
+  <si>
+    <t>description1208</t>
+  </si>
+  <si>
+    <t>description1209</t>
+  </si>
+  <si>
+    <t>description1210</t>
+  </si>
+  <si>
+    <t>description1211</t>
+  </si>
+  <si>
+    <t>description1212</t>
+  </si>
+  <si>
+    <t>description1213</t>
+  </si>
+  <si>
+    <t>description1214</t>
+  </si>
+  <si>
+    <t>description1215</t>
+  </si>
+  <si>
+    <t>description1216</t>
+  </si>
+  <si>
+    <t>description1217</t>
+  </si>
+  <si>
+    <t>description1218</t>
+  </si>
+  <si>
+    <t>description1219</t>
+  </si>
+  <si>
+    <t>description1220</t>
+  </si>
+  <si>
+    <t>description1221</t>
+  </si>
+  <si>
+    <t>description1222</t>
+  </si>
+  <si>
+    <t>description1223</t>
+  </si>
+  <si>
+    <t>description1224</t>
+  </si>
+  <si>
+    <t>description1225</t>
+  </si>
+  <si>
+    <t>description1226</t>
+  </si>
+  <si>
+    <t>description1227</t>
+  </si>
+  <si>
+    <t>description1230</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>description1231</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>description1232</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>description1302</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LANGUAGE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>RESULTSTATUS</t>
-  </si>
-  <si>
-    <t>MD_TYPE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>enable</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>disable</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>user login</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>user exit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>driver configuration</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>module access</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>data export</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALARMTYPE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cbm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>oil</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RESULTNAME</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>code1201</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>code1202</t>
-  </si>
-  <si>
-    <t>code1203</t>
-  </si>
-  <si>
-    <t>code1204</t>
-  </si>
-  <si>
-    <t>code1205</t>
-  </si>
-  <si>
-    <t>code1206</t>
-  </si>
-  <si>
-    <t>code1207</t>
-  </si>
-  <si>
-    <t>code1208</t>
-  </si>
-  <si>
-    <t>code1209</t>
-  </si>
-  <si>
-    <t>code1210</t>
-  </si>
-  <si>
-    <t>code1211</t>
-  </si>
-  <si>
-    <t>code1212</t>
-  </si>
-  <si>
-    <t>code1213</t>
-  </si>
-  <si>
-    <t>code1214</t>
-  </si>
-  <si>
-    <t>code1215</t>
-  </si>
-  <si>
-    <t>code1216</t>
-  </si>
-  <si>
-    <t>code1217</t>
-  </si>
-  <si>
-    <t>code1218</t>
-  </si>
-  <si>
-    <t>code1219</t>
-  </si>
-  <si>
-    <t>code1220</t>
-  </si>
-  <si>
-    <t>code1221</t>
-  </si>
-  <si>
-    <t>code1222</t>
-  </si>
-  <si>
-    <t>code1223</t>
-  </si>
-  <si>
-    <t>code1224</t>
-  </si>
-  <si>
-    <t>code1225</t>
-  </si>
-  <si>
-    <t>code1226</t>
-  </si>
-  <si>
-    <t>code1227</t>
-  </si>
-  <si>
-    <t>code1230</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>code1231</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>code1232</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>code1233</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRPCalculate</t>
   </si>
 </sst>
 </file>
@@ -5456,7 +5473,7 @@
         <v>5</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1123</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -8249,8 +8266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C865"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="F88" sqref="F88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -9243,7 +9260,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>1121</v>
+        <v>1057</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>428</v>
@@ -9331,7 +9348,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>258</v>
+        <v>1173</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>258</v>
@@ -15197,10 +15214,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G77"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33:D40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -15218,7 +15235,7 @@
         <v>1016</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1118</v>
+        <v>1054</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1017</v>
@@ -15244,7 +15261,7 @@
         <v>1022</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>1124</v>
+        <v>1060</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -15261,7 +15278,7 @@
         <v>1022</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>1125</v>
+        <v>1061</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -15278,7 +15295,7 @@
         <v>1022</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>1126</v>
+        <v>1062</v>
       </c>
       <c r="D4" s="1">
         <v>2</v>
@@ -15295,7 +15312,7 @@
         <v>1022</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>1127</v>
+        <v>1063</v>
       </c>
       <c r="D5" s="1">
         <v>3</v>
@@ -15312,7 +15329,7 @@
         <v>1023</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>1138</v>
+        <v>1074</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -15331,7 +15348,7 @@
         <v>1023</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>1139</v>
+        <v>1075</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -15347,10 +15364,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1119</v>
+        <v>1055</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>1120</v>
+        <v>1056</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
@@ -15364,7 +15381,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>1119</v>
+        <v>1055</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>235</v>
@@ -15381,7 +15398,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>1119</v>
+        <v>1055</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>236</v>
@@ -15398,7 +15415,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>1119</v>
+        <v>1055</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>237</v>
@@ -15415,10 +15432,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>1119</v>
+        <v>1055</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>1122</v>
+        <v>1058</v>
       </c>
       <c r="D12" s="1">
         <v>400</v>
@@ -15429,7 +15446,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>1027</v>
@@ -15438,7 +15455,7 @@
         <v>1028</v>
       </c>
       <c r="D13" s="1">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -15446,7 +15463,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>1027</v>
@@ -15455,7 +15472,7 @@
         <v>1029</v>
       </c>
       <c r="D14" s="1">
-        <v>100</v>
+        <v>201</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -15463,7 +15480,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>1027</v>
@@ -15472,7 +15489,7 @@
         <v>1030</v>
       </c>
       <c r="D15" s="1">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -15480,16 +15497,16 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>1027</v>
+        <v>1172</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>1031</v>
       </c>
       <c r="D16" s="1">
-        <v>300</v>
+        <v>-44</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -15497,16 +15514,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>1032</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>1033</v>
-      </c>
       <c r="D17" s="1">
-        <v>0</v>
+        <v>-55</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -15514,16 +15531,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>1032</v>
+        <v>1064</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>1029</v>
+        <v>1033</v>
       </c>
       <c r="D18" s="1">
-        <v>100</v>
+        <v>-66</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -15531,16 +15548,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>1032</v>
+        <v>1064</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>1030</v>
+        <v>1034</v>
       </c>
       <c r="D19" s="1">
-        <v>200</v>
+        <v>-77</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -15548,16 +15565,16 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>1032</v>
+        <v>1064</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>1031</v>
+        <v>1035</v>
       </c>
       <c r="D20" s="1">
-        <v>300</v>
+        <v>-88</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -15565,16 +15582,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>1032</v>
+        <v>1064</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>1034</v>
+        <v>1036</v>
       </c>
       <c r="D21" s="1">
-        <v>400</v>
+        <v>-99</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -15582,13 +15599,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>1035</v>
-      </c>
-      <c r="C22" s="5">
-        <v>0</v>
+        <v>1064</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>1037</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
@@ -15599,16 +15616,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>1035</v>
-      </c>
-      <c r="C23" s="5">
-        <v>0</v>
+        <v>1064</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>1038</v>
       </c>
       <c r="D23" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -15616,16 +15633,16 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>1035</v>
-      </c>
-      <c r="C24" s="5">
-        <v>0</v>
+        <v>1171</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>1040</v>
       </c>
       <c r="D24" s="1">
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -15633,16 +15650,16 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>1035</v>
-      </c>
-      <c r="C25" s="5">
-        <v>0</v>
+        <v>1039</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>1041</v>
       </c>
       <c r="D25" s="1">
-        <v>300</v>
+        <v>2</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -15650,16 +15667,16 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>1036</v>
-      </c>
-      <c r="C26" s="5">
-        <v>0</v>
+        <v>1039</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>1042</v>
       </c>
       <c r="D26" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -15667,16 +15684,16 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>1036</v>
-      </c>
-      <c r="C27" s="5">
+        <v>1065</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D27" s="1">
         <v>0</v>
-      </c>
-      <c r="D27" s="1">
-        <v>100</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -15684,16 +15701,16 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>1036</v>
-      </c>
-      <c r="C28" s="5">
-        <v>0</v>
+        <v>1043</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>1067</v>
       </c>
       <c r="D28" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -15701,16 +15718,16 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>1036</v>
-      </c>
-      <c r="C29" s="5">
+        <v>1044</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D29" s="1">
         <v>0</v>
-      </c>
-      <c r="D29" s="1">
-        <v>300</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -15718,16 +15735,16 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>1037</v>
+        <v>1044</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>1038</v>
+        <v>1069</v>
       </c>
       <c r="D30" s="1">
-        <v>101</v>
+        <v>1</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -15735,16 +15752,16 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>1037</v>
+        <v>1044</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>1039</v>
+        <v>1070</v>
       </c>
       <c r="D31" s="1">
-        <v>201</v>
+        <v>2</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -15752,16 +15769,16 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>1037</v>
+        <v>1044</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>1040</v>
+        <v>1071</v>
       </c>
       <c r="D32" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -15769,16 +15786,16 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>1128</v>
+        <v>1044</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>1041</v>
+        <v>1072</v>
       </c>
       <c r="D33" s="1">
-        <v>-44</v>
+        <v>4</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -15786,16 +15803,16 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>1128</v>
+        <v>1073</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>1042</v>
+        <v>1045</v>
       </c>
       <c r="D34" s="1">
-        <v>-55</v>
+        <v>0</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -15803,16 +15820,16 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>1128</v>
+        <v>1073</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>1043</v>
+        <v>1046</v>
       </c>
       <c r="D35" s="1">
-        <v>-66</v>
+        <v>1</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -15820,16 +15837,16 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>1128</v>
+        <v>1073</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>1044</v>
+        <v>1047</v>
       </c>
       <c r="D36" s="1">
-        <v>-77</v>
+        <v>2</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -15837,16 +15854,16 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>1128</v>
+        <v>1073</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>1045</v>
+        <v>1048</v>
       </c>
       <c r="D37" s="1">
-        <v>-88</v>
+        <v>3</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -15854,16 +15871,16 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>1128</v>
+        <v>1073</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>1046</v>
+        <v>1025</v>
       </c>
       <c r="D38" s="1">
-        <v>-99</v>
+        <v>4</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -15871,16 +15888,16 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>1128</v>
+        <v>1073</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>1047</v>
       </c>
       <c r="D39" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -15888,649 +15905,20 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>1128</v>
+        <v>1073</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>1048</v>
+        <v>1026</v>
       </c>
       <c r="D40" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>57</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>1049</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>1050</v>
-      </c>
-      <c r="D41" s="1">
-        <v>1</v>
-      </c>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>58</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>1049</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>1051</v>
-      </c>
-      <c r="D42" s="1">
-        <v>2</v>
-      </c>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>59</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>1049</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>1052</v>
-      </c>
-      <c r="D43" s="1">
-        <v>3</v>
-      </c>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>80</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>1129</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>1130</v>
-      </c>
-      <c r="D44" s="1">
-        <v>0</v>
-      </c>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>81</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>1053</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>1131</v>
-      </c>
-      <c r="D45" s="1">
-        <v>2</v>
-      </c>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>90</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>1054</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>1055</v>
-      </c>
-      <c r="D46" s="1">
-        <v>1</v>
-      </c>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>91</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>1054</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>1056</v>
-      </c>
-      <c r="D47" s="1">
-        <v>2</v>
-      </c>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>94</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>1057</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>1132</v>
-      </c>
-      <c r="D48" s="1">
-        <v>0</v>
-      </c>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>95</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>1057</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>1133</v>
-      </c>
-      <c r="D49" s="1">
-        <v>1</v>
-      </c>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>96</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>1057</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>1134</v>
-      </c>
-      <c r="D50" s="1">
-        <v>2</v>
-      </c>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <v>97</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>1057</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>1135</v>
-      </c>
-      <c r="D51" s="1">
-        <v>3</v>
-      </c>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
-        <v>98</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>1057</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>1136</v>
-      </c>
-      <c r="D52" s="1">
-        <v>4</v>
-      </c>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>99</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>1058</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>1059</v>
-      </c>
-      <c r="D53" s="1">
-        <v>0</v>
-      </c>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <v>100</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>1058</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>1033</v>
-      </c>
-      <c r="D54" s="1">
-        <v>1</v>
-      </c>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
-        <v>101</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>1058</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>1030</v>
-      </c>
-      <c r="D55" s="1">
-        <v>2</v>
-      </c>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
-        <v>102</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>1060</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>1059</v>
-      </c>
-      <c r="D56" s="1">
-        <v>0</v>
-      </c>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
-        <v>103</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>1060</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>1033</v>
-      </c>
-      <c r="D57" s="1">
-        <v>1</v>
-      </c>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
-        <v>104</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>1060</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>1030</v>
-      </c>
-      <c r="D58" s="1">
-        <v>2</v>
-      </c>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
-        <v>105</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>1061</v>
-      </c>
-      <c r="C59" s="5">
-        <v>0</v>
-      </c>
-      <c r="D59" s="1">
-        <v>0</v>
-      </c>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
-        <v>106</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>1061</v>
-      </c>
-      <c r="C60" s="5">
-        <v>0</v>
-      </c>
-      <c r="D60" s="1">
-        <v>1</v>
-      </c>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
-        <v>107</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>1061</v>
-      </c>
-      <c r="C61" s="5">
-        <v>0</v>
-      </c>
-      <c r="D61" s="1">
-        <v>2</v>
-      </c>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
-        <v>117</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>1062</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>1029</v>
-      </c>
-      <c r="D62" s="1">
-        <v>0</v>
-      </c>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
-        <v>118</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>1062</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>1033</v>
-      </c>
-      <c r="D63" s="1">
-        <v>1</v>
-      </c>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
-        <v>119</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>1062</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>1030</v>
-      </c>
-      <c r="D64" s="1">
-        <v>2</v>
-      </c>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
-        <v>120</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>1063</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>1029</v>
-      </c>
-      <c r="D65" s="1">
-        <v>0</v>
-      </c>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
-        <v>121</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>1063</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>1033</v>
-      </c>
-      <c r="D66" s="1">
-        <v>1</v>
-      </c>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
-        <v>122</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>1063</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>1030</v>
-      </c>
-      <c r="D67" s="1">
-        <v>2</v>
-      </c>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
-        <v>123</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>1064</v>
-      </c>
-      <c r="C68" s="5">
-        <v>0</v>
-      </c>
-      <c r="D68" s="1">
-        <v>0</v>
-      </c>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
-        <v>124</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>1064</v>
-      </c>
-      <c r="C69" s="5">
-        <v>0</v>
-      </c>
-      <c r="D69" s="1">
-        <v>1</v>
-      </c>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
-        <v>125</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>1064</v>
-      </c>
-      <c r="C70" s="5">
-        <v>0</v>
-      </c>
-      <c r="D70" s="1">
-        <v>2</v>
-      </c>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
-        <v>126</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>1137</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>1065</v>
-      </c>
-      <c r="D71" s="1">
-        <v>0</v>
-      </c>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
-        <v>127</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>1137</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>1066</v>
-      </c>
-      <c r="D72" s="1">
-        <v>1</v>
-      </c>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
-        <v>128</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>1137</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>1067</v>
-      </c>
-      <c r="D73" s="1">
-        <v>2</v>
-      </c>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
-        <v>129</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>1137</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>1068</v>
-      </c>
-      <c r="D74" s="1">
-        <v>3</v>
-      </c>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
-        <v>130</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>1137</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>1025</v>
-      </c>
-      <c r="D75" s="1">
-        <v>4</v>
-      </c>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
-        <v>131</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>1137</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>1067</v>
-      </c>
-      <c r="D76" s="1">
-        <v>5</v>
-      </c>
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
-        <v>132</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>1137</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>1026</v>
-      </c>
-      <c r="D77" s="1">
-        <v>6</v>
-      </c>
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
-      <c r="G77" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -16542,8 +15930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -16558,25 +15946,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>1069</v>
+        <v>1049</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1070</v>
+        <v>1050</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1140</v>
+        <v>1076</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1071</v>
+        <v>1051</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1072</v>
+        <v>1052</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>1073</v>
+        <v>1108</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>1074</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -16587,14 +15975,14 @@
         <v>1201</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1141</v>
+        <v>1106</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1075</v>
+        <v>1140</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>1076</v>
+        <v>1107</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -16606,14 +15994,14 @@
         <v>1202</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1142</v>
+        <v>1077</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1077</v>
+        <v>1141</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>1076</v>
+        <v>1109</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -16625,14 +16013,14 @@
         <v>1203</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1143</v>
+        <v>1078</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1078</v>
+        <v>1142</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>1076</v>
+        <v>1110</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -16644,14 +16032,14 @@
         <v>1204</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1144</v>
+        <v>1079</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1079</v>
+        <v>1143</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>1080</v>
+        <v>1111</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -16663,14 +16051,14 @@
         <v>1205</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1145</v>
+        <v>1080</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>1081</v>
+        <v>1144</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>1080</v>
+        <v>1112</v>
       </c>
       <c r="G6" s="1"/>
     </row>
@@ -16682,14 +16070,14 @@
         <v>1206</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1146</v>
+        <v>1081</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1082</v>
+        <v>1145</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>1080</v>
+        <v>1113</v>
       </c>
       <c r="G7" s="1"/>
     </row>
@@ -16701,14 +16089,14 @@
         <v>1207</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1147</v>
+        <v>1082</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>1083</v>
+        <v>1146</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>1084</v>
+        <v>1114</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -16720,14 +16108,14 @@
         <v>1208</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1148</v>
+        <v>1083</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1085</v>
+        <v>1147</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>1086</v>
+        <v>1115</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -16739,14 +16127,14 @@
         <v>1209</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1149</v>
+        <v>1084</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>1087</v>
+        <v>1148</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>1086</v>
+        <v>1116</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -16758,14 +16146,14 @@
         <v>1210</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1150</v>
+        <v>1085</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>1088</v>
+        <v>1149</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>1089</v>
+        <v>1117</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -16777,14 +16165,14 @@
         <v>1211</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1151</v>
+        <v>1086</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>1090</v>
+        <v>1150</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>1091</v>
+        <v>1118</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -16796,14 +16184,14 @@
         <v>1212</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1152</v>
+        <v>1087</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>1092</v>
+        <v>1151</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>1093</v>
+        <v>1119</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -16815,14 +16203,14 @@
         <v>1213</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1153</v>
+        <v>1088</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>1094</v>
+        <v>1152</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>1093</v>
+        <v>1120</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -16834,14 +16222,14 @@
         <v>1214</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1154</v>
+        <v>1089</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>1095</v>
+        <v>1153</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>1093</v>
+        <v>1121</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -16853,14 +16241,14 @@
         <v>1215</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1155</v>
+        <v>1090</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>1096</v>
+        <v>1154</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>1097</v>
+        <v>1122</v>
       </c>
       <c r="G16" s="1"/>
     </row>
@@ -16872,14 +16260,14 @@
         <v>1216</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1156</v>
+        <v>1091</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>1098</v>
+        <v>1155</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>1093</v>
+        <v>1123</v>
       </c>
       <c r="G17" s="1"/>
     </row>
@@ -16891,14 +16279,14 @@
         <v>1217</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1157</v>
+        <v>1092</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>1099</v>
+        <v>1156</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
-        <v>1093</v>
+        <v>1124</v>
       </c>
       <c r="G18" s="1"/>
     </row>
@@ -16910,14 +16298,14 @@
         <v>1218</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1158</v>
+        <v>1093</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>1100</v>
+        <v>1157</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
-        <v>1101</v>
+        <v>1125</v>
       </c>
       <c r="G19" s="1"/>
     </row>
@@ -16929,14 +16317,14 @@
         <v>1219</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1159</v>
+        <v>1094</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>1102</v>
+        <v>1158</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
-        <v>1103</v>
+        <v>1126</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -16948,14 +16336,14 @@
         <v>1220</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1160</v>
+        <v>1095</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>1096</v>
+        <v>1159</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>1104</v>
+        <v>1127</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -16967,14 +16355,14 @@
         <v>1221</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1161</v>
+        <v>1096</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>1105</v>
+        <v>1160</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>1106</v>
+        <v>1128</v>
       </c>
       <c r="G22" s="1"/>
     </row>
@@ -16986,14 +16374,14 @@
         <v>1222</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1162</v>
+        <v>1097</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>1107</v>
+        <v>1161</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>1108</v>
+        <v>1129</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -17005,14 +16393,14 @@
         <v>1223</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>1163</v>
+        <v>1098</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>1109</v>
+        <v>1162</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>1110</v>
+        <v>1130</v>
       </c>
       <c r="G24" s="1"/>
     </row>
@@ -17024,14 +16412,14 @@
         <v>1224</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>1164</v>
+        <v>1099</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>1111</v>
+        <v>1163</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>1084</v>
+        <v>1131</v>
       </c>
       <c r="G25" s="1"/>
     </row>
@@ -17043,12 +16431,14 @@
         <v>1225</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>1165</v>
-      </c>
-      <c r="D26" s="1"/>
+        <v>1100</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>1164</v>
+      </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>1084</v>
+        <v>1132</v>
       </c>
       <c r="G26" s="1"/>
     </row>
@@ -17060,14 +16450,14 @@
         <v>1226</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>1166</v>
+        <v>1101</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>1112</v>
+        <v>1165</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>1113</v>
+        <v>1133</v>
       </c>
       <c r="G27" s="1"/>
     </row>
@@ -17079,12 +16469,14 @@
         <v>1227</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>1167</v>
-      </c>
-      <c r="D28" s="1"/>
+        <v>1102</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>1166</v>
+      </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
-        <v>1113</v>
+        <v>1134</v>
       </c>
       <c r="G28" s="1"/>
     </row>
@@ -17096,14 +16488,14 @@
         <v>1230</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>1168</v>
+        <v>1103</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>1114</v>
+        <v>1167</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
-        <v>1115</v>
+        <v>1135</v>
       </c>
       <c r="G29" s="1"/>
     </row>
@@ -17115,12 +16507,14 @@
         <v>1231</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>1169</v>
-      </c>
-      <c r="D30" s="1"/>
+        <v>1104</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>1168</v>
+      </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1" t="s">
-        <v>1116</v>
+        <v>1136</v>
       </c>
       <c r="G30" s="1"/>
     </row>
@@ -17132,12 +16526,14 @@
         <v>1232</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>1170</v>
-      </c>
-      <c r="D31" s="1"/>
+        <v>1105</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>1169</v>
+      </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>1117</v>
+        <v>1137</v>
       </c>
       <c r="G31" s="1"/>
     </row>
@@ -17149,15 +16545,35 @@
         <v>1302</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>1171</v>
-      </c>
-      <c r="D32" s="1"/>
+        <v>1138</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>1170</v>
+      </c>
       <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
+      <c r="F32" s="1" t="s">
+        <v>1139</v>
+      </c>
       <c r="G32" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Organization and module adjustment
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnpc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnpc/locale/locale-en.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="1175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1618" uniqueCount="1176">
   <si>
     <t>myself</t>
   </si>
@@ -4524,11 +4524,15 @@
     <t>SRPCalculate</t>
   </si>
   <si>
+    <t>language edit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>roleLanguageEdit</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>language edit</t>
+    <t>unnamed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -8268,10 +8272,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C866"/>
+  <dimension ref="A1:C867"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A310" workbookViewId="0">
-      <selection activeCell="C317" sqref="C317"/>
+    <sheetView tabSelected="1" topLeftCell="A253" workbookViewId="0">
+      <selection activeCell="C273" sqref="C273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -11277,10 +11281,10 @@
         <v>272</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>492</v>
+        <v>1175</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>492</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
@@ -11288,10 +11292,10 @@
         <v>273</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
@@ -11299,10 +11303,10 @@
         <v>274</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
@@ -11310,10 +11314,10 @@
         <v>275</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
@@ -11321,10 +11325,10 @@
         <v>276</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
@@ -11332,10 +11336,10 @@
         <v>277</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
@@ -11343,10 +11347,10 @@
         <v>278</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
@@ -11354,10 +11358,10 @@
         <v>279</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
@@ -11365,10 +11369,10 @@
         <v>280</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C281" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
@@ -11376,10 +11380,10 @@
         <v>281</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C282" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
@@ -11387,10 +11391,10 @@
         <v>282</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C283" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
@@ -11398,10 +11402,10 @@
         <v>283</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C284" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
@@ -11409,10 +11413,10 @@
         <v>284</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C285" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
@@ -11420,10 +11424,10 @@
         <v>285</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
@@ -11431,10 +11435,10 @@
         <v>286</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
@@ -11442,10 +11446,10 @@
         <v>287</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C288" s="1" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
@@ -11453,10 +11457,10 @@
         <v>288</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C289" s="1" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
@@ -11464,10 +11468,10 @@
         <v>289</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C290" s="1" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
@@ -11475,10 +11479,10 @@
         <v>290</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C291" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
@@ -11486,10 +11490,10 @@
         <v>291</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C292" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
@@ -11497,10 +11501,10 @@
         <v>292</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C293" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
@@ -11508,10 +11512,10 @@
         <v>293</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
@@ -11519,10 +11523,10 @@
         <v>294</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C295" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
@@ -11530,10 +11534,10 @@
         <v>295</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>648</v>
+        <v>519</v>
       </c>
       <c r="C296" s="1" t="s">
-        <v>647</v>
+        <v>519</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
@@ -11541,10 +11545,10 @@
         <v>296</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>520</v>
+        <v>648</v>
       </c>
       <c r="C297" s="1" t="s">
-        <v>520</v>
+        <v>647</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
@@ -11552,10 +11556,10 @@
         <v>297</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>532</v>
+        <v>520</v>
       </c>
       <c r="C298" s="1" t="s">
-        <v>530</v>
+        <v>520</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
@@ -11563,10 +11567,10 @@
         <v>298</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="C299" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
@@ -11574,10 +11578,10 @@
         <v>299</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C300" s="1" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
@@ -11585,10 +11589,10 @@
         <v>300</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="C301" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
@@ -11596,10 +11600,10 @@
         <v>301</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>750</v>
+        <v>536</v>
       </c>
       <c r="C302" s="1" t="s">
-        <v>750</v>
+        <v>535</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
@@ -11607,10 +11611,10 @@
         <v>302</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="C303" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
@@ -11618,10 +11622,10 @@
         <v>303</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
@@ -11629,10 +11633,10 @@
         <v>304</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>537</v>
+        <v>752</v>
       </c>
       <c r="C305" s="1" t="s">
-        <v>545</v>
+        <v>752</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
@@ -11640,10 +11644,10 @@
         <v>305</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C306" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
@@ -11651,10 +11655,10 @@
         <v>306</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C307" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
@@ -11662,10 +11666,10 @@
         <v>307</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C308" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
@@ -11673,10 +11677,10 @@
         <v>308</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>549</v>
+        <v>540</v>
       </c>
       <c r="C309" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
@@ -11684,10 +11688,10 @@
         <v>309</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C310" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
@@ -11695,10 +11699,10 @@
         <v>310</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>541</v>
+        <v>551</v>
       </c>
       <c r="C311" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
@@ -11706,10 +11710,10 @@
         <v>311</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C312" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
@@ -11717,10 +11721,10 @@
         <v>312</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C313" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
@@ -11728,10 +11732,10 @@
         <v>313</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C314" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
@@ -11739,10 +11743,10 @@
         <v>314</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>557</v>
+        <v>544</v>
       </c>
       <c r="C315" s="1" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
@@ -11750,10 +11754,10 @@
         <v>315</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C316" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
@@ -11761,10 +11765,10 @@
         <v>316</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>1173</v>
+        <v>559</v>
       </c>
       <c r="C317" s="1" t="s">
-        <v>1174</v>
+        <v>560</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
@@ -11772,10 +11776,10 @@
         <v>317</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>561</v>
+        <v>1174</v>
       </c>
       <c r="C318" s="1" t="s">
-        <v>562</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
@@ -11783,10 +11787,10 @@
         <v>318</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="C319" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
@@ -11794,10 +11798,10 @@
         <v>319</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C320" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
@@ -11805,10 +11809,10 @@
         <v>320</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C321" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.25">
@@ -11816,10 +11820,10 @@
         <v>321</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C322" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.25">
@@ -11827,10 +11831,10 @@
         <v>322</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C323" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
@@ -11838,10 +11842,10 @@
         <v>323</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C324" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
@@ -11849,10 +11853,10 @@
         <v>324</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C325" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
@@ -11860,10 +11864,10 @@
         <v>325</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C326" s="1" t="s">
-        <v>586</v>
+        <v>570</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
@@ -11871,10 +11875,10 @@
         <v>326</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C327" s="1" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
@@ -11882,10 +11886,10 @@
         <v>327</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C328" s="1" t="s">
-        <v>573</v>
+        <v>585</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.25">
@@ -11893,10 +11897,10 @@
         <v>328</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C329" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.25">
@@ -11904,10 +11908,10 @@
         <v>329</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C330" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.25">
@@ -11915,10 +11919,10 @@
         <v>330</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C331" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.25">
@@ -11926,10 +11930,10 @@
         <v>331</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C332" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.25">
@@ -11937,10 +11941,10 @@
         <v>332</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.25">
@@ -11948,10 +11952,10 @@
         <v>333</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C334" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.25">
@@ -11959,10 +11963,10 @@
         <v>334</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C335" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.25">
@@ -11970,10 +11974,10 @@
         <v>335</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C336" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.25">
@@ -11981,10 +11985,10 @@
         <v>336</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C337" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.25">
@@ -11992,10 +11996,10 @@
         <v>337</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C338" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.25">
@@ -12003,10 +12007,10 @@
         <v>338</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C339" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.25">
@@ -12014,10 +12018,10 @@
         <v>339</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="C340" s="1" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.25">
@@ -12025,10 +12029,10 @@
         <v>340</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="C341" s="1" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.25">
@@ -12036,10 +12040,10 @@
         <v>341</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C342" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.25">
@@ -12047,10 +12051,10 @@
         <v>342</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="C343" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.25">
@@ -12058,10 +12062,10 @@
         <v>343</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C344" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.25">
@@ -12069,10 +12073,10 @@
         <v>344</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C345" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.25">
@@ -12080,10 +12084,10 @@
         <v>345</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>754</v>
+        <v>595</v>
       </c>
       <c r="C346" s="1" t="s">
-        <v>753</v>
+        <v>595</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.25">
@@ -12091,10 +12095,10 @@
         <v>346</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>616</v>
+        <v>754</v>
       </c>
       <c r="C347" s="1" t="s">
-        <v>617</v>
+        <v>753</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.25">
@@ -12102,10 +12106,10 @@
         <v>347</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C348" s="1" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.25">
@@ -12113,10 +12117,10 @@
         <v>348</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>596</v>
+        <v>618</v>
       </c>
       <c r="C349" s="1" t="s">
-        <v>605</v>
+        <v>619</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.25">
@@ -12124,10 +12128,10 @@
         <v>349</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C350" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.25">
@@ -12135,10 +12139,10 @@
         <v>350</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C351" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.25">
@@ -12146,10 +12150,10 @@
         <v>351</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C352" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.25">
@@ -12157,10 +12161,10 @@
         <v>352</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C353" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.25">
@@ -12168,10 +12172,10 @@
         <v>353</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C354" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.25">
@@ -12179,10 +12183,10 @@
         <v>354</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>615</v>
+        <v>601</v>
       </c>
       <c r="C355" s="1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.25">
@@ -12190,10 +12194,10 @@
         <v>355</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>602</v>
+        <v>615</v>
       </c>
       <c r="C356" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.25">
@@ -12201,10 +12205,10 @@
         <v>356</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C357" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.25">
@@ -12212,10 +12216,10 @@
         <v>357</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C358" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.25">
@@ -12223,10 +12227,10 @@
         <v>358</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>620</v>
+        <v>604</v>
       </c>
       <c r="C359" s="1" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.25">
@@ -12234,10 +12238,10 @@
         <v>359</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>632</v>
+        <v>620</v>
       </c>
       <c r="C360" s="1" t="s">
-        <v>632</v>
+        <v>620</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.25">
@@ -12245,10 +12249,10 @@
         <v>360</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>621</v>
+        <v>632</v>
       </c>
       <c r="C361" s="1" t="s">
-        <v>627</v>
+        <v>632</v>
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.25">
@@ -12256,10 +12260,10 @@
         <v>361</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C362" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.25">
@@ -12267,10 +12271,10 @@
         <v>362</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C363" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.25">
@@ -12278,10 +12282,10 @@
         <v>363</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C364" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.25">
@@ -12289,10 +12293,10 @@
         <v>364</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C365" s="1" t="s">
-        <v>611</v>
+        <v>630</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.25">
@@ -12300,10 +12304,10 @@
         <v>365</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C366" s="1" t="s">
-        <v>631</v>
+        <v>611</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.25">
@@ -12311,10 +12315,10 @@
         <v>366</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>633</v>
+        <v>626</v>
       </c>
       <c r="C367" s="1" t="s">
-        <v>640</v>
+        <v>631</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.25">
@@ -12322,10 +12326,10 @@
         <v>367</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C368" s="1" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
@@ -12333,10 +12337,10 @@
         <v>368</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>679</v>
+        <v>634</v>
       </c>
       <c r="C369" s="1" t="s">
-        <v>680</v>
+        <v>639</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
@@ -12344,10 +12348,10 @@
         <v>369</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>635</v>
+        <v>679</v>
       </c>
       <c r="C370" s="1" t="s">
-        <v>637</v>
+        <v>680</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
@@ -12355,10 +12359,10 @@
         <v>370</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C371" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.25">
@@ -12366,10 +12370,10 @@
         <v>371</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="C372" s="1" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
@@ -12377,10 +12381,10 @@
         <v>372</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C373" s="1" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.25">
@@ -12388,10 +12392,10 @@
         <v>373</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C374" s="1" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.25">
@@ -12399,10 +12403,10 @@
         <v>374</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>681</v>
+        <v>645</v>
       </c>
       <c r="C375" s="1" t="s">
-        <v>695</v>
+        <v>646</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
@@ -12410,10 +12414,10 @@
         <v>375</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C376" s="1" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.25">
@@ -12421,10 +12425,10 @@
         <v>376</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C377" s="1" t="s">
-        <v>683</v>
+        <v>696</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.25">
@@ -12432,10 +12436,10 @@
         <v>377</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="C378" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.25">
@@ -12443,10 +12447,10 @@
         <v>378</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C379" s="1" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.25">
@@ -12454,10 +12458,10 @@
         <v>379</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C380" s="1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.25">
@@ -12465,10 +12469,10 @@
         <v>380</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C381" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.25">
@@ -12476,10 +12480,10 @@
         <v>381</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C382" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.25">
@@ -12487,10 +12491,10 @@
         <v>382</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C383" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.25">
@@ -12498,10 +12502,10 @@
         <v>383</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C384" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.25">
@@ -12509,10 +12513,10 @@
         <v>384</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C385" s="1" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.25">
@@ -12520,10 +12524,10 @@
         <v>385</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C386" s="1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.25">
@@ -12531,10 +12535,10 @@
         <v>386</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C387" s="1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.25">
@@ -12542,10 +12546,10 @@
         <v>387</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="C388" s="1" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.25">
@@ -12553,10 +12557,10 @@
         <v>388</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="C389" s="1" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.25">
@@ -12564,10 +12568,10 @@
         <v>389</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="C390" s="1" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.25">
@@ -12575,10 +12579,10 @@
         <v>390</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C391" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.25">
@@ -12586,10 +12590,10 @@
         <v>391</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="C392" s="1" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.25">
@@ -12597,10 +12601,10 @@
         <v>392</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="C393" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.25">
@@ -12608,10 +12612,10 @@
         <v>393</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C394" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.25">
@@ -12619,10 +12623,10 @@
         <v>394</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C395" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.25">
@@ -12630,10 +12634,10 @@
         <v>395</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C396" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.25">
@@ -12641,10 +12645,10 @@
         <v>396</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C397" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.25">
@@ -12652,10 +12656,10 @@
         <v>397</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="C398" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.25">
@@ -12663,10 +12667,10 @@
         <v>398</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="C399" s="1" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.25">
@@ -12674,10 +12678,10 @@
         <v>399</v>
       </c>
       <c r="B400" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C400" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.25">
@@ -12685,10 +12689,10 @@
         <v>400</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C401" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.25">
@@ -12696,10 +12700,10 @@
         <v>401</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C402" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.25">
@@ -12707,10 +12711,10 @@
         <v>402</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C403" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.25">
@@ -12718,10 +12722,10 @@
         <v>403</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C404" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.25">
@@ -12729,10 +12733,10 @@
         <v>404</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C405" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.25">
@@ -12740,10 +12744,10 @@
         <v>405</v>
       </c>
       <c r="B406" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C406" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.25">
@@ -12751,10 +12755,10 @@
         <v>406</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C407" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.25">
@@ -12762,10 +12766,10 @@
         <v>407</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="C408" s="1" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.25">
@@ -12773,10 +12777,10 @@
         <v>408</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="C409" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.25">
@@ -12784,10 +12788,10 @@
         <v>409</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C410" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.25">
@@ -12795,10 +12799,10 @@
         <v>410</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C411" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.25">
@@ -12806,10 +12810,10 @@
         <v>411</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C412" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.25">
@@ -12817,10 +12821,10 @@
         <v>412</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C413" s="1" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.25">
@@ -12828,10 +12832,10 @@
         <v>413</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>781</v>
+        <v>728</v>
       </c>
       <c r="C414" s="1" t="s">
-        <v>782</v>
+        <v>728</v>
       </c>
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.25">
@@ -12839,10 +12843,10 @@
         <v>414</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C415" s="1" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.25">
@@ -12850,10 +12854,10 @@
         <v>415</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C416" s="1" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.25">
@@ -12861,10 +12865,10 @@
         <v>416</v>
       </c>
       <c r="B417" s="1" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="C417" s="1" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.25">
@@ -12872,10 +12876,10 @@
         <v>417</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="C418" s="1" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.25">
@@ -12883,10 +12887,10 @@
         <v>418</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C419" s="1" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.25">
@@ -12894,10 +12898,10 @@
         <v>419</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="C420" s="1" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.25">
@@ -12905,10 +12909,10 @@
         <v>420</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C421" s="1" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.25">
@@ -12916,10 +12920,10 @@
         <v>421</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>833</v>
+        <v>793</v>
       </c>
       <c r="C422" s="1" t="s">
-        <v>829</v>
+        <v>793</v>
       </c>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.25">
@@ -12927,10 +12931,10 @@
         <v>422</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>830</v>
+        <v>833</v>
       </c>
       <c r="C423" s="1" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.25">
@@ -12938,10 +12942,10 @@
         <v>423</v>
       </c>
       <c r="B424" s="1" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C424" s="1" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.25">
@@ -12949,10 +12953,10 @@
         <v>424</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C425" s="1" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.25">
@@ -12960,10 +12964,10 @@
         <v>425</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="C426" s="1" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.25">
@@ -12971,10 +12975,10 @@
         <v>426</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="C427" s="1" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.25">
@@ -12982,10 +12986,10 @@
         <v>427</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C428" s="1" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.25">
@@ -12993,10 +12997,10 @@
         <v>428</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C429" s="1" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.25">
@@ -13004,10 +13008,10 @@
         <v>429</v>
       </c>
       <c r="B430" s="1" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="C430" s="1" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.25">
@@ -13015,10 +13019,10 @@
         <v>430</v>
       </c>
       <c r="B431" s="1" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C431" s="1" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.25">
@@ -13026,10 +13030,10 @@
         <v>431</v>
       </c>
       <c r="B432" s="1" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="C432" s="1" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.25">
@@ -13037,10 +13041,10 @@
         <v>432</v>
       </c>
       <c r="B433" s="1" t="s">
-        <v>1008</v>
+        <v>841</v>
       </c>
       <c r="C433" s="1" t="s">
-        <v>1008</v>
+        <v>841</v>
       </c>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.25">
@@ -13048,10 +13052,10 @@
         <v>433</v>
       </c>
       <c r="B434" s="1" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="C434" s="1" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.25">
@@ -13059,16 +13063,22 @@
         <v>434</v>
       </c>
       <c r="B435" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C435" s="1" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="436" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A436" s="1">
+        <v>435</v>
+      </c>
+      <c r="B436" s="1" t="s">
         <v>1011</v>
       </c>
-      <c r="C435" s="1" t="s">
+      <c r="C436" s="1" t="s">
         <v>1010</v>
       </c>
-    </row>
-    <row r="436" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A436" s="1"/>
-      <c r="B436" s="1"/>
-      <c r="C436" s="1"/>
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A437" s="1"/>
@@ -15219,6 +15229,11 @@
       <c r="A866" s="1"/>
       <c r="B866" s="1"/>
       <c r="C866" s="1"/>
+    </row>
+    <row r="867" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A867" s="1"/>
+      <c r="B867" s="1"/>
+      <c r="C867" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Function adjustment optimization and database document update
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnpc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnpc/locale/locale-en.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB156DE-BD4B-4862-8E0B-68EB88414A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AE8FE1-E1F5-4356-A45C-D6502BCA8D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3781" uniqueCount="3587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3787" uniqueCount="3592">
   <si>
     <t>myself</t>
   </si>
@@ -13381,6 +13381,26 @@
   </si>
   <si>
     <t>自定义</t>
+  </si>
+  <si>
+    <t>driverConfig_Unit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单元</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>driverConfig_Group</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -20415,10 +20435,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FBAC76-7507-496A-9947-9F636F0BCBC6}">
-  <dimension ref="A1:D634"/>
+  <dimension ref="A1:D636"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A556" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B569" sqref="B569"/>
+    <sheetView tabSelected="1" topLeftCell="A613" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D636" sqref="D636"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -29302,6 +29322,34 @@
       </c>
       <c r="D634" s="1" t="s">
         <v>3570</v>
+      </c>
+    </row>
+    <row r="635" spans="1:4">
+      <c r="A635" s="15">
+        <v>634</v>
+      </c>
+      <c r="B635" s="5" t="s">
+        <v>3587</v>
+      </c>
+      <c r="C635" s="18" t="s">
+        <v>3588</v>
+      </c>
+      <c r="D635" s="9" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="636" spans="1:4">
+      <c r="A636" s="15">
+        <v>635</v>
+      </c>
+      <c r="B636" s="5" t="s">
+        <v>3589</v>
+      </c>
+      <c r="C636" s="18" t="s">
+        <v>3590</v>
+      </c>
+      <c r="D636" s="9" t="s">
+        <v>3591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Instance optimization and adjustment
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnpc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnpc/locale/locale-en.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC64EE42-A7EB-4263-8536-ED943A32B27C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A6F37D-8BA6-4619-8E17-3D3F8DD5092D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3790" uniqueCount="3595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3793" uniqueCount="3598">
   <si>
     <t>myself</t>
   </si>
@@ -13412,6 +13412,18 @@
   </si>
   <si>
     <t>Not uplinked</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>primaryDeviceCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主设备数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of primary devices</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -20448,10 +20460,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FBAC76-7507-496A-9947-9F636F0BCBC6}">
-  <dimension ref="A1:D637"/>
+  <dimension ref="A1:D638"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A433" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D449" sqref="D449"/>
+    <sheetView tabSelected="1" topLeftCell="A619" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D638" sqref="D638"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -26733,7 +26745,7 @@
         <v>2249</v>
       </c>
     </row>
-    <row r="449" spans="1:4" customFormat="1">
+    <row r="449" spans="1:4">
       <c r="A449" s="15">
         <v>448</v>
       </c>
@@ -26747,7 +26759,7 @@
         <v>3594</v>
       </c>
     </row>
-    <row r="450" spans="1:4" customFormat="1">
+    <row r="450" spans="1:4">
       <c r="A450" s="15">
         <v>449</v>
       </c>
@@ -26761,7 +26773,7 @@
         <v>3124</v>
       </c>
     </row>
-    <row r="451" spans="1:4" customFormat="1">
+    <row r="451" spans="1:4">
       <c r="A451" s="15">
         <v>450</v>
       </c>
@@ -26775,7 +26787,7 @@
         <v>3125</v>
       </c>
     </row>
-    <row r="452" spans="1:4" customFormat="1">
+    <row r="452" spans="1:4">
       <c r="A452" s="15">
         <v>451</v>
       </c>
@@ -26789,7 +26801,7 @@
         <v>3126</v>
       </c>
     </row>
-    <row r="453" spans="1:4" customFormat="1">
+    <row r="453" spans="1:4">
       <c r="A453" s="15">
         <v>452</v>
       </c>
@@ -26803,7 +26815,7 @@
         <v>3298</v>
       </c>
     </row>
-    <row r="454" spans="1:4" customFormat="1">
+    <row r="454" spans="1:4">
       <c r="A454" s="15">
         <v>453</v>
       </c>
@@ -26817,7 +26829,7 @@
         <v>3299</v>
       </c>
     </row>
-    <row r="455" spans="1:4" customFormat="1">
+    <row r="455" spans="1:4">
       <c r="A455" s="15">
         <v>454</v>
       </c>
@@ -26831,7 +26843,7 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="456" spans="1:4" customFormat="1">
+    <row r="456" spans="1:4">
       <c r="A456" s="15">
         <v>455</v>
       </c>
@@ -26845,7 +26857,7 @@
         <v>3301</v>
       </c>
     </row>
-    <row r="457" spans="1:4" customFormat="1">
+    <row r="457" spans="1:4">
       <c r="A457" s="15">
         <v>456</v>
       </c>
@@ -26859,7 +26871,7 @@
         <v>3127</v>
       </c>
     </row>
-    <row r="458" spans="1:4" customFormat="1">
+    <row r="458" spans="1:4">
       <c r="A458" s="15">
         <v>457</v>
       </c>
@@ -26873,7 +26885,7 @@
         <v>3471</v>
       </c>
     </row>
-    <row r="459" spans="1:4" customFormat="1">
+    <row r="459" spans="1:4">
       <c r="A459" s="15">
         <v>458</v>
       </c>
@@ -26887,7 +26899,7 @@
         <v>3303</v>
       </c>
     </row>
-    <row r="460" spans="1:4" customFormat="1">
+    <row r="460" spans="1:4">
       <c r="A460" s="15">
         <v>459</v>
       </c>
@@ -26901,7 +26913,7 @@
         <v>3129</v>
       </c>
     </row>
-    <row r="461" spans="1:4" customFormat="1">
+    <row r="461" spans="1:4">
       <c r="A461" s="15">
         <v>460</v>
       </c>
@@ -26915,7 +26927,7 @@
         <v>3472</v>
       </c>
     </row>
-    <row r="462" spans="1:4" customFormat="1">
+    <row r="462" spans="1:4">
       <c r="A462" s="15">
         <v>461</v>
       </c>
@@ -26929,7 +26941,7 @@
         <v>3473</v>
       </c>
     </row>
-    <row r="463" spans="1:4" customFormat="1">
+    <row r="463" spans="1:4">
       <c r="A463" s="15">
         <v>462</v>
       </c>
@@ -26943,7 +26955,7 @@
         <v>3474</v>
       </c>
     </row>
-    <row r="464" spans="1:4" customFormat="1">
+    <row r="464" spans="1:4">
       <c r="A464" s="15">
         <v>463</v>
       </c>
@@ -29377,6 +29389,20 @@
       </c>
       <c r="D637" s="9" t="s">
         <v>3591</v>
+      </c>
+    </row>
+    <row r="638" spans="1:4">
+      <c r="A638" s="15">
+        <v>637</v>
+      </c>
+      <c r="B638" s="5" t="s">
+        <v>3595</v>
+      </c>
+      <c r="C638" s="18" t="s">
+        <v>3596</v>
+      </c>
+      <c r="D638" s="9" t="s">
+        <v>3597</v>
       </c>
     </row>
   </sheetData>
@@ -31262,7 +31288,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Data dictionary module adjustment
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnpc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnpc/locale/locale-en.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2F2878-B79B-4A8B-8934-ACC5C4842A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E13EB0A-A95E-4F8C-8744-E5D27003E706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3820" uniqueCount="3620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3829" uniqueCount="3622">
   <si>
     <t>myself</t>
   </si>
@@ -12058,9 +12058,6 @@
     <t>Customize</t>
   </si>
   <si>
-    <t>Configuration</t>
-  </si>
-  <si>
     <t>open</t>
   </si>
   <si>
@@ -13518,6 +13515,18 @@
   </si>
   <si>
     <t>Enabled</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DICTDATASOURCE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字典</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dictionary</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -15393,7 +15402,7 @@
         <v>766</v>
       </c>
       <c r="C98" s="23" t="s">
-        <v>3348</v>
+        <v>3347</v>
       </c>
       <c r="D98" s="19" t="s">
         <v>769</v>
@@ -15407,7 +15416,7 @@
         <v>767</v>
       </c>
       <c r="C99" s="23" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="D99" s="19" t="s">
         <v>770</v>
@@ -15507,7 +15516,7 @@
         <v>735</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>3389</v>
+        <v>3388</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -15551,7 +15560,7 @@
         <v>992</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>3390</v>
+        <v>3389</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -15573,7 +15582,7 @@
         <v>994</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>3391</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -15595,7 +15604,7 @@
         <v>996</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>3392</v>
+        <v>3391</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -15606,7 +15615,7 @@
         <v>997</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>3393</v>
+        <v>3392</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -15661,7 +15670,7 @@
         <v>1002</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>3394</v>
+        <v>3393</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -16923,7 +16932,7 @@
         <v>2352</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>3432</v>
+        <v>3431</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -16937,7 +16946,7 @@
         <v>2353</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>3436</v>
+        <v>3435</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -16951,7 +16960,7 @@
         <v>2354</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>3440</v>
+        <v>3439</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -16965,7 +16974,7 @@
         <v>2355</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>3444</v>
+        <v>3443</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -16979,7 +16988,7 @@
         <v>2356</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>3448</v>
+        <v>3447</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -16993,7 +17002,7 @@
         <v>2357</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>3433</v>
+        <v>3432</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -17007,7 +17016,7 @@
         <v>2358</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>3437</v>
+        <v>3436</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -17021,7 +17030,7 @@
         <v>2359</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>3441</v>
+        <v>3440</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -17035,7 +17044,7 @@
         <v>2360</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>3445</v>
+        <v>3444</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -17049,7 +17058,7 @@
         <v>2361</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>3449</v>
+        <v>3448</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -17063,7 +17072,7 @@
         <v>2362</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>3434</v>
+        <v>3433</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -17077,7 +17086,7 @@
         <v>2363</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>3438</v>
+        <v>3437</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -17091,7 +17100,7 @@
         <v>2364</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>3442</v>
+        <v>3441</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -17105,7 +17114,7 @@
         <v>2365</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>3446</v>
+        <v>3445</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -17119,7 +17128,7 @@
         <v>2366</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>3450</v>
+        <v>3449</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -17133,7 +17142,7 @@
         <v>2367</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>3435</v>
+        <v>3434</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -17147,7 +17156,7 @@
         <v>2368</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>3439</v>
+        <v>3438</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -17161,7 +17170,7 @@
         <v>2369</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>3443</v>
+        <v>3442</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -17175,7 +17184,7 @@
         <v>2370</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>3447</v>
+        <v>3446</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -17189,7 +17198,7 @@
         <v>2371</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>3451</v>
+        <v>3450</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -17917,7 +17926,7 @@
         <v>2444</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>3412</v>
+        <v>3411</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -17931,7 +17940,7 @@
         <v>2445</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>3413</v>
+        <v>3412</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -18015,7 +18024,7 @@
         <v>1256</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>3414</v>
+        <v>3413</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -18029,7 +18038,7 @@
         <v>1257</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>3415</v>
+        <v>3414</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -18043,7 +18052,7 @@
         <v>1258</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>3416</v>
+        <v>3415</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -18225,7 +18234,7 @@
         <v>1259</v>
       </c>
       <c r="D165" s="19" t="s">
-        <v>3330</v>
+        <v>3329</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -18253,7 +18262,7 @@
         <v>1261</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>3417</v>
+        <v>3416</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -18267,7 +18276,7 @@
         <v>1262</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>3418</v>
+        <v>3417</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -18281,7 +18290,7 @@
         <v>1263</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>3419</v>
+        <v>3418</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -18306,10 +18315,10 @@
         <v>649</v>
       </c>
       <c r="C171" s="9" t="s">
+        <v>3542</v>
+      </c>
+      <c r="D171" s="1" t="s">
         <v>3543</v>
-      </c>
-      <c r="D171" s="1" t="s">
-        <v>3544</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -18631,7 +18640,7 @@
         <v>2488</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>3421</v>
+        <v>3420</v>
       </c>
     </row>
     <row r="195" spans="1:4">
@@ -18645,7 +18654,7 @@
         <v>2489</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>3422</v>
+        <v>3421</v>
       </c>
     </row>
     <row r="196" spans="1:4">
@@ -18659,7 +18668,7 @@
         <v>1277</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>3420</v>
+        <v>3419</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -18673,7 +18682,7 @@
         <v>1278</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>3423</v>
+        <v>3422</v>
       </c>
     </row>
     <row r="198" spans="1:4">
@@ -18947,7 +18956,7 @@
         <v>216</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>3607</v>
+        <v>3606</v>
       </c>
       <c r="C217" s="9" t="s">
         <v>2514</v>
@@ -18961,13 +18970,13 @@
         <v>217</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>3608</v>
+        <v>3607</v>
       </c>
       <c r="C218" s="9" t="s">
+        <v>3604</v>
+      </c>
+      <c r="D218" s="1" t="s">
         <v>3605</v>
-      </c>
-      <c r="D218" s="1" t="s">
-        <v>3606</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -20563,8 +20572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FBAC76-7507-496A-9947-9F636F0BCBC6}">
   <dimension ref="A1:D646"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A397" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D406" sqref="D406"/>
+    <sheetView tabSelected="1" topLeftCell="A628" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C653" sqref="C653"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -20610,7 +20619,7 @@
         <v>22</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>3332</v>
+        <v>3331</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>821</v>
@@ -20638,7 +20647,7 @@
         <v>24</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>3333</v>
+        <v>3332</v>
       </c>
       <c r="D5" s="19" t="s">
         <v>822</v>
@@ -20666,7 +20675,7 @@
         <v>26</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>3334</v>
+        <v>3333</v>
       </c>
       <c r="D7" s="19" t="s">
         <v>823</v>
@@ -21100,10 +21109,10 @@
         <v>46</v>
       </c>
       <c r="C38" s="9" t="s">
+        <v>3403</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>3404</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>3405</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -21615,13 +21624,13 @@
         <v>74</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>3594</v>
+        <v>3593</v>
       </c>
       <c r="C75" s="9" t="s">
+        <v>3589</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>3590</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>3591</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -21629,13 +21638,13 @@
         <v>75</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>3595</v>
+        <v>3594</v>
       </c>
       <c r="C76" s="9" t="s">
+        <v>3591</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>3592</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>3593</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -21643,13 +21652,13 @@
         <v>76</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>3600</v>
+        <v>3599</v>
       </c>
       <c r="C77" s="9" t="s">
+        <v>3595</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>3596</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>3597</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -21657,13 +21666,13 @@
         <v>77</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>3601</v>
+        <v>3600</v>
       </c>
       <c r="C78" s="9" t="s">
+        <v>3597</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>3598</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>3599</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -21671,13 +21680,13 @@
         <v>78</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>3604</v>
+        <v>3603</v>
       </c>
       <c r="C79" s="9" t="s">
+        <v>3601</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>3602</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>3603</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -21943,7 +21952,7 @@
         <v>1993</v>
       </c>
       <c r="D98" s="19" t="s">
-        <v>3335</v>
+        <v>3334</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -22609,13 +22618,13 @@
         <v>145</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>3611</v>
+        <v>3610</v>
       </c>
       <c r="C146" s="9" t="s">
+        <v>3608</v>
+      </c>
+      <c r="D146" s="1" t="s">
         <v>3609</v>
-      </c>
-      <c r="D146" s="1" t="s">
-        <v>3610</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -22825,7 +22834,7 @@
         <v>2005</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>3395</v>
+        <v>3394</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -22948,7 +22957,7 @@
         <v>1096</v>
       </c>
       <c r="C170" s="23" t="s">
-        <v>3331</v>
+        <v>3330</v>
       </c>
       <c r="D170" s="19" t="s">
         <v>2864</v>
@@ -23119,7 +23128,7 @@
         <v>2882</v>
       </c>
       <c r="D182" s="19" t="s">
-        <v>3461</v>
+        <v>3460</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -23147,7 +23156,7 @@
         <v>1391</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>3463</v>
+        <v>3462</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -23161,7 +23170,7 @@
         <v>1392</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>3462</v>
+        <v>3461</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -23200,7 +23209,7 @@
         <v>182</v>
       </c>
       <c r="C188" s="23" t="s">
-        <v>3338</v>
+        <v>3337</v>
       </c>
       <c r="D188" s="19" t="s">
         <v>2883</v>
@@ -23214,7 +23223,7 @@
         <v>940</v>
       </c>
       <c r="C189" s="23" t="s">
-        <v>3339</v>
+        <v>3338</v>
       </c>
       <c r="D189" s="19" t="s">
         <v>2884</v>
@@ -23270,7 +23279,7 @@
         <v>186</v>
       </c>
       <c r="C193" s="23" t="s">
-        <v>3340</v>
+        <v>3339</v>
       </c>
       <c r="D193" s="19" t="s">
         <v>2889</v>
@@ -23326,7 +23335,7 @@
         <v>190</v>
       </c>
       <c r="C197" s="23" t="s">
-        <v>3341</v>
+        <v>3340</v>
       </c>
       <c r="D197" s="19" t="s">
         <v>2895</v>
@@ -23354,7 +23363,7 @@
         <v>192</v>
       </c>
       <c r="C199" s="23" t="s">
-        <v>3342</v>
+        <v>3341</v>
       </c>
       <c r="D199" s="19" t="s">
         <v>2896</v>
@@ -23480,10 +23489,10 @@
         <v>209</v>
       </c>
       <c r="C208" s="9" t="s">
+        <v>3395</v>
+      </c>
+      <c r="D208" s="1" t="s">
         <v>3396</v>
-      </c>
-      <c r="D208" s="1" t="s">
-        <v>3397</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -23494,7 +23503,7 @@
         <v>529</v>
       </c>
       <c r="C209" s="23" t="s">
-        <v>3343</v>
+        <v>3342</v>
       </c>
       <c r="D209" s="19" t="s">
         <v>2905</v>
@@ -23511,7 +23520,7 @@
         <v>1406</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>3336</v>
+        <v>3335</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -23525,7 +23534,7 @@
         <v>1407</v>
       </c>
       <c r="D211" s="19" t="s">
-        <v>3337</v>
+        <v>3336</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -24614,10 +24623,10 @@
         <v>287</v>
       </c>
       <c r="C289" s="9" t="s">
+        <v>3268</v>
+      </c>
+      <c r="D289" s="1" t="s">
         <v>3269</v>
-      </c>
-      <c r="D289" s="1" t="s">
-        <v>3270</v>
       </c>
     </row>
     <row r="290" spans="1:4">
@@ -24796,10 +24805,10 @@
         <v>295</v>
       </c>
       <c r="C302" s="9" t="s">
+        <v>3270</v>
+      </c>
+      <c r="D302" s="1" t="s">
         <v>3271</v>
-      </c>
-      <c r="D302" s="1" t="s">
-        <v>3272</v>
       </c>
     </row>
     <row r="303" spans="1:4">
@@ -25216,10 +25225,10 @@
         <v>542</v>
       </c>
       <c r="C332" s="9" t="s">
+        <v>3272</v>
+      </c>
+      <c r="D332" s="1" t="s">
         <v>3273</v>
-      </c>
-      <c r="D332" s="1" t="s">
-        <v>3274</v>
       </c>
     </row>
     <row r="333" spans="1:4">
@@ -25314,10 +25323,10 @@
         <v>335</v>
       </c>
       <c r="C339" s="23" t="s">
-        <v>3344</v>
+        <v>3343</v>
       </c>
       <c r="D339" s="19" t="s">
-        <v>3275</v>
+        <v>3274</v>
       </c>
     </row>
     <row r="340" spans="1:4">
@@ -25510,10 +25519,10 @@
         <v>962</v>
       </c>
       <c r="C353" s="23" t="s">
-        <v>3345</v>
+        <v>3344</v>
       </c>
       <c r="D353" s="19" t="s">
-        <v>3276</v>
+        <v>3275</v>
       </c>
     </row>
     <row r="354" spans="1:4">
@@ -25566,10 +25575,10 @@
         <v>964</v>
       </c>
       <c r="C357" s="23" t="s">
-        <v>3346</v>
+        <v>3345</v>
       </c>
       <c r="D357" s="19" t="s">
-        <v>3277</v>
+        <v>3276</v>
       </c>
     </row>
     <row r="358" spans="1:4">
@@ -25846,10 +25855,10 @@
         <v>1079</v>
       </c>
       <c r="C377" s="23" t="s">
-        <v>3347</v>
+        <v>3346</v>
       </c>
       <c r="D377" s="19" t="s">
-        <v>3278</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="378" spans="1:4">
@@ -25947,7 +25956,7 @@
         <v>1563</v>
       </c>
       <c r="D384" s="1" t="s">
-        <v>3452</v>
+        <v>3451</v>
       </c>
     </row>
     <row r="385" spans="1:4">
@@ -25989,7 +25998,7 @@
         <v>1565</v>
       </c>
       <c r="D387" s="1" t="s">
-        <v>3429</v>
+        <v>3428</v>
       </c>
     </row>
     <row r="388" spans="1:4">
@@ -26017,7 +26026,7 @@
         <v>1566</v>
       </c>
       <c r="D389" s="1" t="s">
-        <v>3453</v>
+        <v>3452</v>
       </c>
     </row>
     <row r="390" spans="1:4">
@@ -26129,7 +26138,7 @@
         <v>1573</v>
       </c>
       <c r="D397" s="1" t="s">
-        <v>3454</v>
+        <v>3453</v>
       </c>
     </row>
     <row r="398" spans="1:4">
@@ -26157,7 +26166,7 @@
         <v>1575</v>
       </c>
       <c r="D399" s="1" t="s">
-        <v>3455</v>
+        <v>3454</v>
       </c>
     </row>
     <row r="400" spans="1:4">
@@ -26185,7 +26194,7 @@
         <v>1577</v>
       </c>
       <c r="D401" s="1" t="s">
-        <v>3456</v>
+        <v>3455</v>
       </c>
     </row>
     <row r="402" spans="1:4">
@@ -26199,7 +26208,7 @@
         <v>1578</v>
       </c>
       <c r="D402" s="1" t="s">
-        <v>3457</v>
+        <v>3456</v>
       </c>
     </row>
     <row r="403" spans="1:4">
@@ -26213,7 +26222,7 @@
         <v>1579</v>
       </c>
       <c r="D403" s="1" t="s">
-        <v>3458</v>
+        <v>3457</v>
       </c>
     </row>
     <row r="404" spans="1:4">
@@ -26252,10 +26261,10 @@
         <v>359</v>
       </c>
       <c r="C406" s="9" t="s">
+        <v>3617</v>
+      </c>
+      <c r="D406" s="1" t="s">
         <v>3618</v>
-      </c>
-      <c r="D406" s="1" t="s">
-        <v>3619</v>
       </c>
     </row>
     <row r="407" spans="1:4">
@@ -26280,7 +26289,7 @@
         <v>361</v>
       </c>
       <c r="C408" s="9" t="s">
-        <v>3279</v>
+        <v>3278</v>
       </c>
       <c r="D408" s="1" t="s">
         <v>861</v>
@@ -26423,7 +26432,7 @@
         <v>1113</v>
       </c>
       <c r="D418" s="1" t="s">
-        <v>3459</v>
+        <v>3458</v>
       </c>
     </row>
     <row r="419" spans="1:4">
@@ -26490,7 +26499,7 @@
         <v>375</v>
       </c>
       <c r="C423" s="9" t="s">
-        <v>3280</v>
+        <v>3279</v>
       </c>
       <c r="D423" s="1" t="s">
         <v>862</v>
@@ -26574,10 +26583,10 @@
         <v>378</v>
       </c>
       <c r="C429" s="9" t="s">
+        <v>3280</v>
+      </c>
+      <c r="D429" s="1" t="s">
         <v>3281</v>
-      </c>
-      <c r="D429" s="1" t="s">
-        <v>3282</v>
       </c>
     </row>
     <row r="430" spans="1:4">
@@ -26588,7 +26597,7 @@
         <v>379</v>
       </c>
       <c r="C430" s="9" t="s">
-        <v>3283</v>
+        <v>3282</v>
       </c>
       <c r="D430" s="1" t="s">
         <v>863</v>
@@ -26658,7 +26667,7 @@
         <v>1027</v>
       </c>
       <c r="C435" s="9" t="s">
-        <v>3284</v>
+        <v>3283</v>
       </c>
       <c r="D435" s="1" t="s">
         <v>1028</v>
@@ -26686,10 +26695,10 @@
         <v>1055</v>
       </c>
       <c r="C437" s="9" t="s">
+        <v>3284</v>
+      </c>
+      <c r="D437" s="1" t="s">
         <v>3285</v>
-      </c>
-      <c r="D437" s="1" t="s">
-        <v>3286</v>
       </c>
     </row>
     <row r="438" spans="1:4">
@@ -26781,13 +26790,13 @@
         <v>443</v>
       </c>
       <c r="B444" s="5" t="s">
-        <v>3400</v>
+        <v>3399</v>
       </c>
       <c r="C444" s="9" t="s">
-        <v>3398</v>
+        <v>3397</v>
       </c>
       <c r="D444" s="1" t="s">
-        <v>3402</v>
+        <v>3401</v>
       </c>
     </row>
     <row r="445" spans="1:4">
@@ -26795,13 +26804,13 @@
         <v>444</v>
       </c>
       <c r="B445" s="5" t="s">
-        <v>3401</v>
+        <v>3400</v>
       </c>
       <c r="C445" s="9" t="s">
-        <v>3399</v>
+        <v>3398</v>
       </c>
       <c r="D445" s="1" t="s">
-        <v>3403</v>
+        <v>3402</v>
       </c>
     </row>
     <row r="446" spans="1:4">
@@ -26935,13 +26944,13 @@
         <v>454</v>
       </c>
       <c r="B455" s="5" t="s">
+        <v>3583</v>
+      </c>
+      <c r="C455" s="25" t="s">
         <v>3584</v>
       </c>
-      <c r="C455" s="25" t="s">
+      <c r="D455" s="25" t="s">
         <v>3585</v>
-      </c>
-      <c r="D455" s="25" t="s">
-        <v>3586</v>
       </c>
     </row>
     <row r="456" spans="1:4">
@@ -26994,10 +27003,10 @@
         <v>393</v>
       </c>
       <c r="C459" s="9" t="s">
-        <v>3287</v>
+        <v>3286</v>
       </c>
       <c r="D459" s="1" t="s">
-        <v>3292</v>
+        <v>3291</v>
       </c>
     </row>
     <row r="460" spans="1:4">
@@ -27008,10 +27017,10 @@
         <v>394</v>
       </c>
       <c r="C460" s="9" t="s">
-        <v>3288</v>
+        <v>3287</v>
       </c>
       <c r="D460" s="1" t="s">
-        <v>3293</v>
+        <v>3292</v>
       </c>
     </row>
     <row r="461" spans="1:4">
@@ -27022,10 +27031,10 @@
         <v>395</v>
       </c>
       <c r="C461" s="9" t="s">
-        <v>3289</v>
+        <v>3288</v>
       </c>
       <c r="D461" s="1" t="s">
-        <v>3294</v>
+        <v>3293</v>
       </c>
     </row>
     <row r="462" spans="1:4">
@@ -27036,10 +27045,10 @@
         <v>396</v>
       </c>
       <c r="C462" s="9" t="s">
-        <v>3290</v>
+        <v>3289</v>
       </c>
       <c r="D462" s="1" t="s">
-        <v>3295</v>
+        <v>3294</v>
       </c>
     </row>
     <row r="463" spans="1:4">
@@ -27050,7 +27059,7 @@
         <v>397</v>
       </c>
       <c r="C463" s="9" t="s">
-        <v>3291</v>
+        <v>3290</v>
       </c>
       <c r="D463" s="1" t="s">
         <v>3123</v>
@@ -27067,7 +27076,7 @@
         <v>1117</v>
       </c>
       <c r="D464" s="1" t="s">
-        <v>3464</v>
+        <v>3463</v>
       </c>
     </row>
     <row r="465" spans="1:4">
@@ -27078,10 +27087,10 @@
         <v>399</v>
       </c>
       <c r="C465" s="9" t="s">
+        <v>3295</v>
+      </c>
+      <c r="D465" s="1" t="s">
         <v>3296</v>
-      </c>
-      <c r="D465" s="1" t="s">
-        <v>3297</v>
       </c>
     </row>
     <row r="466" spans="1:4">
@@ -27109,7 +27118,7 @@
         <v>2012</v>
       </c>
       <c r="D467" s="1" t="s">
-        <v>3465</v>
+        <v>3464</v>
       </c>
     </row>
     <row r="468" spans="1:4">
@@ -27123,7 +27132,7 @@
         <v>2013</v>
       </c>
       <c r="D468" s="1" t="s">
-        <v>3466</v>
+        <v>3465</v>
       </c>
     </row>
     <row r="469" spans="1:4">
@@ -27137,7 +27146,7 @@
         <v>1611</v>
       </c>
       <c r="D469" s="1" t="s">
-        <v>3467</v>
+        <v>3466</v>
       </c>
     </row>
     <row r="470" spans="1:4">
@@ -27145,13 +27154,13 @@
         <v>469</v>
       </c>
       <c r="B470" s="5" t="s">
+        <v>3611</v>
+      </c>
+      <c r="C470" s="9" t="s">
         <v>3612</v>
       </c>
-      <c r="C470" s="9" t="s">
-        <v>3613</v>
-      </c>
       <c r="D470" s="9" t="s">
-        <v>3616</v>
+        <v>3615</v>
       </c>
     </row>
     <row r="471" spans="1:4">
@@ -27159,13 +27168,13 @@
         <v>470</v>
       </c>
       <c r="B471" s="5" t="s">
+        <v>3613</v>
+      </c>
+      <c r="C471" s="9" t="s">
         <v>3614</v>
       </c>
-      <c r="C471" s="9" t="s">
-        <v>3615</v>
-      </c>
       <c r="D471" s="9" t="s">
-        <v>3617</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="472" spans="1:4">
@@ -27358,7 +27367,7 @@
         <v>409</v>
       </c>
       <c r="C485" s="9" t="s">
-        <v>3298</v>
+        <v>3297</v>
       </c>
       <c r="D485" s="1" t="s">
         <v>864</v>
@@ -27372,7 +27381,7 @@
         <v>410</v>
       </c>
       <c r="C486" s="9" t="s">
-        <v>3299</v>
+        <v>3298</v>
       </c>
       <c r="D486" s="1" t="s">
         <v>865</v>
@@ -27473,7 +27482,7 @@
         <v>1122</v>
       </c>
       <c r="D493" s="1" t="s">
-        <v>3478</v>
+        <v>3477</v>
       </c>
     </row>
     <row r="494" spans="1:4">
@@ -27484,10 +27493,10 @@
         <v>412</v>
       </c>
       <c r="C494" s="9" t="s">
+        <v>3299</v>
+      </c>
+      <c r="D494" s="1" t="s">
         <v>3300</v>
-      </c>
-      <c r="D494" s="1" t="s">
-        <v>3301</v>
       </c>
     </row>
     <row r="495" spans="1:4">
@@ -27529,7 +27538,7 @@
         <v>1623</v>
       </c>
       <c r="D497" s="1" t="s">
-        <v>3479</v>
+        <v>3478</v>
       </c>
     </row>
     <row r="498" spans="1:4">
@@ -27540,10 +27549,10 @@
         <v>416</v>
       </c>
       <c r="C498" s="9" t="s">
+        <v>3301</v>
+      </c>
+      <c r="D498" s="1" t="s">
         <v>3302</v>
-      </c>
-      <c r="D498" s="1" t="s">
-        <v>3303</v>
       </c>
     </row>
     <row r="499" spans="1:4">
@@ -27554,10 +27563,10 @@
         <v>420</v>
       </c>
       <c r="C499" s="9" t="s">
-        <v>3304</v>
+        <v>3303</v>
       </c>
       <c r="D499" s="1" t="s">
-        <v>3307</v>
+        <v>3306</v>
       </c>
     </row>
     <row r="500" spans="1:4">
@@ -27568,10 +27577,10 @@
         <v>417</v>
       </c>
       <c r="C500" s="9" t="s">
+        <v>3304</v>
+      </c>
+      <c r="D500" s="1" t="s">
         <v>3305</v>
-      </c>
-      <c r="D500" s="1" t="s">
-        <v>3306</v>
       </c>
     </row>
     <row r="501" spans="1:4">
@@ -28271,7 +28280,7 @@
         <v>1672</v>
       </c>
       <c r="D550" s="1" t="s">
-        <v>3494</v>
+        <v>3493</v>
       </c>
     </row>
     <row r="551" spans="1:4">
@@ -28366,7 +28375,7 @@
         <v>507</v>
       </c>
       <c r="C557" s="9" t="s">
-        <v>3308</v>
+        <v>3307</v>
       </c>
       <c r="D557" s="1" t="s">
         <v>866</v>
@@ -28677,7 +28686,7 @@
         <v>1697</v>
       </c>
       <c r="D579" s="1" t="s">
-        <v>3411</v>
+        <v>3410</v>
       </c>
     </row>
     <row r="580" spans="1:4">
@@ -28691,7 +28700,7 @@
         <v>1698</v>
       </c>
       <c r="D580" s="1" t="s">
-        <v>3225</v>
+        <v>3224</v>
       </c>
     </row>
     <row r="581" spans="1:4">
@@ -28705,7 +28714,7 @@
         <v>1699</v>
       </c>
       <c r="D581" s="1" t="s">
-        <v>3226</v>
+        <v>3225</v>
       </c>
     </row>
     <row r="582" spans="1:4">
@@ -28716,10 +28725,10 @@
         <v>756</v>
       </c>
       <c r="C582" s="13" t="s">
-        <v>3407</v>
+        <v>3406</v>
       </c>
       <c r="D582" s="4" t="s">
-        <v>3409</v>
+        <v>3408</v>
       </c>
     </row>
     <row r="583" spans="1:4">
@@ -28730,10 +28739,10 @@
         <v>757</v>
       </c>
       <c r="C583" s="13" t="s">
-        <v>3406</v>
+        <v>3405</v>
       </c>
       <c r="D583" s="4" t="s">
-        <v>3408</v>
+        <v>3407</v>
       </c>
     </row>
     <row r="584" spans="1:4">
@@ -28747,7 +28756,7 @@
         <v>1700</v>
       </c>
       <c r="D584" s="1" t="s">
-        <v>3227</v>
+        <v>3226</v>
       </c>
     </row>
     <row r="585" spans="1:4">
@@ -28761,7 +28770,7 @@
         <v>1701</v>
       </c>
       <c r="D585" s="1" t="s">
-        <v>3228</v>
+        <v>3227</v>
       </c>
     </row>
     <row r="586" spans="1:4">
@@ -28775,7 +28784,7 @@
         <v>1702</v>
       </c>
       <c r="D586" s="1" t="s">
-        <v>3229</v>
+        <v>3228</v>
       </c>
     </row>
     <row r="587" spans="1:4">
@@ -28789,7 +28798,7 @@
         <v>1703</v>
       </c>
       <c r="D587" s="1" t="s">
-        <v>3230</v>
+        <v>3229</v>
       </c>
     </row>
     <row r="588" spans="1:4">
@@ -28803,7 +28812,7 @@
         <v>1704</v>
       </c>
       <c r="D588" s="1" t="s">
-        <v>3231</v>
+        <v>3230</v>
       </c>
     </row>
     <row r="589" spans="1:4">
@@ -28817,7 +28826,7 @@
         <v>1705</v>
       </c>
       <c r="D589" s="1" t="s">
-        <v>3232</v>
+        <v>3231</v>
       </c>
     </row>
     <row r="590" spans="1:4">
@@ -28831,7 +28840,7 @@
         <v>1706</v>
       </c>
       <c r="D590" s="1" t="s">
-        <v>3233</v>
+        <v>3232</v>
       </c>
     </row>
     <row r="591" spans="1:4">
@@ -28845,7 +28854,7 @@
         <v>1707</v>
       </c>
       <c r="D591" s="1" t="s">
-        <v>3234</v>
+        <v>3233</v>
       </c>
     </row>
     <row r="592" spans="1:4">
@@ -28859,7 +28868,7 @@
         <v>1708</v>
       </c>
       <c r="D592" s="1" t="s">
-        <v>3235</v>
+        <v>3234</v>
       </c>
     </row>
     <row r="593" spans="1:4">
@@ -28873,7 +28882,7 @@
         <v>1709</v>
       </c>
       <c r="D593" s="1" t="s">
-        <v>3236</v>
+        <v>3235</v>
       </c>
     </row>
     <row r="594" spans="1:4">
@@ -28887,7 +28896,7 @@
         <v>1710</v>
       </c>
       <c r="D594" s="1" t="s">
-        <v>3237</v>
+        <v>3236</v>
       </c>
     </row>
     <row r="595" spans="1:4">
@@ -28901,7 +28910,7 @@
         <v>1711</v>
       </c>
       <c r="D595" s="1" t="s">
-        <v>3238</v>
+        <v>3237</v>
       </c>
     </row>
     <row r="596" spans="1:4">
@@ -28915,7 +28924,7 @@
         <v>1712</v>
       </c>
       <c r="D596" s="1" t="s">
-        <v>3239</v>
+        <v>3238</v>
       </c>
     </row>
     <row r="597" spans="1:4">
@@ -28929,7 +28938,7 @@
         <v>1713</v>
       </c>
       <c r="D597" s="1" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="598" spans="1:4">
@@ -28943,7 +28952,7 @@
         <v>1714</v>
       </c>
       <c r="D598" s="1" t="s">
-        <v>3241</v>
+        <v>3240</v>
       </c>
     </row>
     <row r="599" spans="1:4">
@@ -28957,7 +28966,7 @@
         <v>1715</v>
       </c>
       <c r="D599" s="1" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="600" spans="1:4">
@@ -28971,7 +28980,7 @@
         <v>1716</v>
       </c>
       <c r="D600" s="1" t="s">
-        <v>3243</v>
+        <v>3242</v>
       </c>
     </row>
     <row r="601" spans="1:4">
@@ -28985,7 +28994,7 @@
         <v>1717</v>
       </c>
       <c r="D601" s="1" t="s">
-        <v>3244</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="602" spans="1:4">
@@ -28999,7 +29008,7 @@
         <v>1718</v>
       </c>
       <c r="D602" s="1" t="s">
-        <v>3245</v>
+        <v>3244</v>
       </c>
     </row>
     <row r="603" spans="1:4">
@@ -29013,7 +29022,7 @@
         <v>1719</v>
       </c>
       <c r="D603" s="1" t="s">
-        <v>3246</v>
+        <v>3245</v>
       </c>
     </row>
     <row r="604" spans="1:4">
@@ -29027,7 +29036,7 @@
         <v>1720</v>
       </c>
       <c r="D604" s="1" t="s">
-        <v>3247</v>
+        <v>3246</v>
       </c>
     </row>
     <row r="605" spans="1:4">
@@ -29041,7 +29050,7 @@
         <v>1721</v>
       </c>
       <c r="D605" s="1" t="s">
-        <v>3248</v>
+        <v>3247</v>
       </c>
     </row>
     <row r="606" spans="1:4">
@@ -29055,7 +29064,7 @@
         <v>1722</v>
       </c>
       <c r="D606" s="1" t="s">
-        <v>3249</v>
+        <v>3248</v>
       </c>
     </row>
     <row r="607" spans="1:4">
@@ -29069,7 +29078,7 @@
         <v>1723</v>
       </c>
       <c r="D607" s="1" t="s">
-        <v>3250</v>
+        <v>3249</v>
       </c>
     </row>
     <row r="608" spans="1:4">
@@ -29083,7 +29092,7 @@
         <v>1724</v>
       </c>
       <c r="D608" s="1" t="s">
-        <v>3251</v>
+        <v>3250</v>
       </c>
     </row>
     <row r="609" spans="1:4">
@@ -29097,7 +29106,7 @@
         <v>1725</v>
       </c>
       <c r="D609" s="1" t="s">
-        <v>3252</v>
+        <v>3251</v>
       </c>
     </row>
     <row r="610" spans="1:4">
@@ -29111,7 +29120,7 @@
         <v>1726</v>
       </c>
       <c r="D610" s="1" t="s">
-        <v>3253</v>
+        <v>3252</v>
       </c>
     </row>
     <row r="611" spans="1:4">
@@ -29125,7 +29134,7 @@
         <v>1727</v>
       </c>
       <c r="D611" s="4" t="s">
-        <v>3254</v>
+        <v>3253</v>
       </c>
     </row>
     <row r="612" spans="1:4">
@@ -29139,7 +29148,7 @@
         <v>1728</v>
       </c>
       <c r="D612" s="4" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
     </row>
     <row r="613" spans="1:4">
@@ -29153,7 +29162,7 @@
         <v>1729</v>
       </c>
       <c r="D613" s="1" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
     </row>
     <row r="614" spans="1:4">
@@ -29164,10 +29173,10 @@
         <v>933</v>
       </c>
       <c r="C614" s="9" t="s">
+        <v>3308</v>
+      </c>
+      <c r="D614" s="1" t="s">
         <v>3309</v>
-      </c>
-      <c r="D614" s="1" t="s">
-        <v>3310</v>
       </c>
     </row>
     <row r="615" spans="1:4">
@@ -29181,7 +29190,7 @@
         <v>1730</v>
       </c>
       <c r="D615" s="1" t="s">
-        <v>3257</v>
+        <v>3256</v>
       </c>
     </row>
     <row r="616" spans="1:4">
@@ -29195,7 +29204,7 @@
         <v>1731</v>
       </c>
       <c r="D616" s="1" t="s">
-        <v>3258</v>
+        <v>3257</v>
       </c>
     </row>
     <row r="617" spans="1:4">
@@ -29209,7 +29218,7 @@
         <v>1732</v>
       </c>
       <c r="D617" s="1" t="s">
-        <v>3259</v>
+        <v>3258</v>
       </c>
     </row>
     <row r="618" spans="1:4">
@@ -29223,7 +29232,7 @@
         <v>1733</v>
       </c>
       <c r="D618" s="1" t="s">
-        <v>3260</v>
+        <v>3259</v>
       </c>
     </row>
     <row r="619" spans="1:4">
@@ -29237,7 +29246,7 @@
         <v>1734</v>
       </c>
       <c r="D619" s="1" t="s">
-        <v>3261</v>
+        <v>3260</v>
       </c>
     </row>
     <row r="620" spans="1:4">
@@ -29251,7 +29260,7 @@
         <v>1735</v>
       </c>
       <c r="D620" s="1" t="s">
-        <v>3262</v>
+        <v>3261</v>
       </c>
     </row>
     <row r="621" spans="1:4">
@@ -29265,7 +29274,7 @@
         <v>1736</v>
       </c>
       <c r="D621" s="1" t="s">
-        <v>3263</v>
+        <v>3262</v>
       </c>
     </row>
     <row r="622" spans="1:4">
@@ -29279,7 +29288,7 @@
         <v>1737</v>
       </c>
       <c r="D622" s="1" t="s">
-        <v>3264</v>
+        <v>3263</v>
       </c>
     </row>
     <row r="623" spans="1:4">
@@ -29293,7 +29302,7 @@
         <v>1738</v>
       </c>
       <c r="D623" s="1" t="s">
-        <v>3265</v>
+        <v>3264</v>
       </c>
     </row>
     <row r="624" spans="1:4">
@@ -29307,7 +29316,7 @@
         <v>1739</v>
       </c>
       <c r="D624" s="1" t="s">
-        <v>3266</v>
+        <v>3265</v>
       </c>
     </row>
     <row r="625" spans="1:4">
@@ -29321,7 +29330,7 @@
         <v>1740</v>
       </c>
       <c r="D625" s="1" t="s">
-        <v>3267</v>
+        <v>3266</v>
       </c>
     </row>
     <row r="626" spans="1:4">
@@ -29335,7 +29344,7 @@
         <v>1741</v>
       </c>
       <c r="D626" s="1" t="s">
-        <v>3268</v>
+        <v>3267</v>
       </c>
     </row>
     <row r="627" spans="1:4" ht="15">
@@ -29343,13 +29352,13 @@
         <v>626</v>
       </c>
       <c r="B627" s="24" t="s">
-        <v>3565</v>
+        <v>3564</v>
       </c>
       <c r="C627" s="18" t="s">
+        <v>3528</v>
+      </c>
+      <c r="D627" s="24" t="s">
         <v>3529</v>
-      </c>
-      <c r="D627" s="24" t="s">
-        <v>3530</v>
       </c>
     </row>
     <row r="628" spans="1:4">
@@ -29357,13 +29366,13 @@
         <v>627</v>
       </c>
       <c r="B628" s="1" t="s">
-        <v>3566</v>
+        <v>3565</v>
       </c>
       <c r="C628" s="9" t="s">
+        <v>3530</v>
+      </c>
+      <c r="D628" s="1" t="s">
         <v>3531</v>
-      </c>
-      <c r="D628" s="1" t="s">
-        <v>3532</v>
       </c>
     </row>
     <row r="629" spans="1:4">
@@ -29371,13 +29380,13 @@
         <v>628</v>
       </c>
       <c r="B629" s="1" t="s">
-        <v>3536</v>
+        <v>3535</v>
       </c>
       <c r="C629" s="9" t="s">
-        <v>3533</v>
+        <v>3532</v>
       </c>
       <c r="D629" s="1" t="s">
-        <v>3536</v>
+        <v>3535</v>
       </c>
     </row>
     <row r="630" spans="1:4">
@@ -29385,13 +29394,13 @@
         <v>629</v>
       </c>
       <c r="B630" s="1" t="s">
-        <v>3535</v>
+        <v>3534</v>
       </c>
       <c r="C630" s="9" t="s">
+        <v>3533</v>
+      </c>
+      <c r="D630" s="1" t="s">
         <v>3534</v>
-      </c>
-      <c r="D630" s="1" t="s">
-        <v>3535</v>
       </c>
     </row>
     <row r="631" spans="1:4">
@@ -29399,13 +29408,13 @@
         <v>630</v>
       </c>
       <c r="B631" s="1" t="s">
-        <v>3540</v>
+        <v>3539</v>
       </c>
       <c r="C631" s="1" t="s">
-        <v>3537</v>
+        <v>3536</v>
       </c>
       <c r="D631" s="1" t="s">
-        <v>3540</v>
+        <v>3539</v>
       </c>
     </row>
     <row r="632" spans="1:4">
@@ -29413,13 +29422,13 @@
         <v>631</v>
       </c>
       <c r="B632" s="1" t="s">
-        <v>3541</v>
+        <v>3540</v>
       </c>
       <c r="C632" s="1" t="s">
-        <v>3538</v>
+        <v>3537</v>
       </c>
       <c r="D632" s="1" t="s">
-        <v>3541</v>
+        <v>3540</v>
       </c>
     </row>
     <row r="633" spans="1:4">
@@ -29427,13 +29436,13 @@
         <v>632</v>
       </c>
       <c r="B633" s="1" t="s">
-        <v>3542</v>
+        <v>3541</v>
       </c>
       <c r="C633" s="1" t="s">
-        <v>3539</v>
+        <v>3538</v>
       </c>
       <c r="D633" s="1" t="s">
-        <v>3542</v>
+        <v>3541</v>
       </c>
     </row>
     <row r="634" spans="1:4">
@@ -29441,13 +29450,13 @@
         <v>633</v>
       </c>
       <c r="B634" s="1" t="s">
-        <v>3564</v>
+        <v>3563</v>
       </c>
       <c r="C634" s="1" t="s">
+        <v>3562</v>
+      </c>
+      <c r="D634" s="1" t="s">
         <v>3563</v>
-      </c>
-      <c r="D634" s="1" t="s">
-        <v>3564</v>
       </c>
     </row>
     <row r="635" spans="1:4">
@@ -29455,13 +29464,13 @@
         <v>634</v>
       </c>
       <c r="B635" s="1" t="s">
-        <v>3567</v>
+        <v>3566</v>
       </c>
       <c r="C635" s="1" t="s">
+        <v>3544</v>
+      </c>
+      <c r="D635" s="1" t="s">
         <v>3545</v>
-      </c>
-      <c r="D635" s="1" t="s">
-        <v>3546</v>
       </c>
     </row>
     <row r="636" spans="1:4">
@@ -29469,13 +29478,13 @@
         <v>635</v>
       </c>
       <c r="B636" s="1" t="s">
-        <v>3568</v>
+        <v>3567</v>
       </c>
       <c r="C636" s="1" t="s">
+        <v>3546</v>
+      </c>
+      <c r="D636" s="1" t="s">
         <v>3547</v>
-      </c>
-      <c r="D636" s="1" t="s">
-        <v>3548</v>
       </c>
     </row>
     <row r="637" spans="1:4">
@@ -29483,13 +29492,13 @@
         <v>636</v>
       </c>
       <c r="B637" s="1" t="s">
-        <v>3569</v>
+        <v>3568</v>
       </c>
       <c r="C637" s="1" t="s">
+        <v>3548</v>
+      </c>
+      <c r="D637" s="1" t="s">
         <v>3549</v>
-      </c>
-      <c r="D637" s="1" t="s">
-        <v>3550</v>
       </c>
     </row>
     <row r="638" spans="1:4">
@@ -29497,13 +29506,13 @@
         <v>637</v>
       </c>
       <c r="B638" s="1" t="s">
-        <v>3570</v>
+        <v>3569</v>
       </c>
       <c r="C638" s="1" t="s">
+        <v>3550</v>
+      </c>
+      <c r="D638" s="1" t="s">
         <v>3551</v>
-      </c>
-      <c r="D638" s="1" t="s">
-        <v>3552</v>
       </c>
     </row>
     <row r="639" spans="1:4">
@@ -29511,13 +29520,13 @@
         <v>638</v>
       </c>
       <c r="B639" s="1" t="s">
-        <v>3554</v>
+        <v>3553</v>
       </c>
       <c r="C639" s="18" t="s">
+        <v>3552</v>
+      </c>
+      <c r="D639" s="1" t="s">
         <v>3553</v>
-      </c>
-      <c r="D639" s="1" t="s">
-        <v>3554</v>
       </c>
     </row>
     <row r="640" spans="1:4">
@@ -29525,13 +29534,13 @@
         <v>639</v>
       </c>
       <c r="B640" s="1" t="s">
-        <v>3571</v>
+        <v>3570</v>
       </c>
       <c r="C640" s="1" t="s">
+        <v>3554</v>
+      </c>
+      <c r="D640" s="1" t="s">
         <v>3555</v>
-      </c>
-      <c r="D640" s="1" t="s">
-        <v>3556</v>
       </c>
     </row>
     <row r="641" spans="1:4">
@@ -29539,13 +29548,13 @@
         <v>640</v>
       </c>
       <c r="B641" s="1" t="s">
-        <v>3572</v>
+        <v>3571</v>
       </c>
       <c r="C641" s="1" t="s">
+        <v>3556</v>
+      </c>
+      <c r="D641" s="1" t="s">
         <v>3557</v>
-      </c>
-      <c r="D641" s="1" t="s">
-        <v>3558</v>
       </c>
     </row>
     <row r="642" spans="1:4">
@@ -29553,13 +29562,13 @@
         <v>641</v>
       </c>
       <c r="B642" s="1" t="s">
-        <v>3573</v>
+        <v>3572</v>
       </c>
       <c r="C642" s="1" t="s">
+        <v>3558</v>
+      </c>
+      <c r="D642" s="1" t="s">
         <v>3559</v>
-      </c>
-      <c r="D642" s="1" t="s">
-        <v>3560</v>
       </c>
     </row>
     <row r="643" spans="1:4">
@@ -29567,13 +29576,13 @@
         <v>642</v>
       </c>
       <c r="B643" s="1" t="s">
-        <v>3574</v>
+        <v>3573</v>
       </c>
       <c r="C643" s="1" t="s">
+        <v>3560</v>
+      </c>
+      <c r="D643" s="1" t="s">
         <v>3561</v>
-      </c>
-      <c r="D643" s="1" t="s">
-        <v>3562</v>
       </c>
     </row>
     <row r="644" spans="1:4">
@@ -29581,10 +29590,10 @@
         <v>643</v>
       </c>
       <c r="B644" s="5" t="s">
+        <v>3578</v>
+      </c>
+      <c r="C644" s="18" t="s">
         <v>3579</v>
-      </c>
-      <c r="C644" s="18" t="s">
-        <v>3580</v>
       </c>
       <c r="D644" s="9" t="s">
         <v>480</v>
@@ -29595,13 +29604,13 @@
         <v>644</v>
       </c>
       <c r="B645" s="5" t="s">
+        <v>3580</v>
+      </c>
+      <c r="C645" s="18" t="s">
         <v>3581</v>
       </c>
-      <c r="C645" s="18" t="s">
+      <c r="D645" s="9" t="s">
         <v>3582</v>
-      </c>
-      <c r="D645" s="9" t="s">
-        <v>3583</v>
       </c>
     </row>
     <row r="646" spans="1:4">
@@ -29609,13 +29618,13 @@
         <v>645</v>
       </c>
       <c r="B646" s="5" t="s">
+        <v>3586</v>
+      </c>
+      <c r="C646" s="18" t="s">
         <v>3587</v>
       </c>
-      <c r="C646" s="18" t="s">
+      <c r="D646" s="9" t="s">
         <v>3588</v>
-      </c>
-      <c r="D646" s="9" t="s">
-        <v>3589</v>
       </c>
     </row>
   </sheetData>
@@ -29627,10 +29636,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:D7"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -29702,7 +29711,7 @@
         <v>1964</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>3311</v>
+        <v>3310</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -29742,7 +29751,7 @@
         <v>1966</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>3312</v>
+        <v>3311</v>
       </c>
       <c r="E5" s="1">
         <v>3</v>
@@ -29759,10 +29768,10 @@
         <v>688</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>3407</v>
+        <v>3406</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>3409</v>
+        <v>3408</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
@@ -29779,10 +29788,10 @@
         <v>688</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>3406</v>
+        <v>3405</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>3408</v>
+        <v>3407</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
@@ -29819,10 +29828,10 @@
         <v>702</v>
       </c>
       <c r="C9" s="13" t="s">
+        <v>3312</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>3313</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>3314</v>
       </c>
       <c r="E9" s="1">
         <v>100</v>
@@ -29842,7 +29851,7 @@
         <v>1967</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>3315</v>
+        <v>3314</v>
       </c>
       <c r="E10" s="1">
         <v>200</v>
@@ -29859,10 +29868,10 @@
         <v>702</v>
       </c>
       <c r="C11" s="13" t="s">
+        <v>3315</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>3316</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>3317</v>
       </c>
       <c r="E11" s="1">
         <v>300</v>
@@ -29962,7 +29971,7 @@
         <v>1971</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>3318</v>
+        <v>3317</v>
       </c>
       <c r="E16" s="1">
         <v>-44</v>
@@ -29982,7 +29991,7 @@
         <v>1972</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>3319</v>
+        <v>3318</v>
       </c>
       <c r="E17" s="1">
         <v>-55</v>
@@ -30002,7 +30011,7 @@
         <v>1973</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>3320</v>
+        <v>3319</v>
       </c>
       <c r="E18" s="1">
         <v>-66</v>
@@ -30022,7 +30031,7 @@
         <v>1974</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>3321</v>
+        <v>3320</v>
       </c>
       <c r="E19" s="1">
         <v>-77</v>
@@ -30042,7 +30051,7 @@
         <v>1975</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>3322</v>
+        <v>3321</v>
       </c>
       <c r="E20" s="1">
         <v>-88</v>
@@ -30062,7 +30071,7 @@
         <v>1976</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>3323</v>
+        <v>3322</v>
       </c>
       <c r="E21" s="1">
         <v>-99</v>
@@ -30082,7 +30091,7 @@
         <v>1977</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>3254</v>
+        <v>3253</v>
       </c>
       <c r="E22" s="1">
         <v>0</v>
@@ -30102,7 +30111,7 @@
         <v>1978</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="E23" s="1">
         <v>1</v>
@@ -30242,7 +30251,7 @@
         <v>1985</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>3324</v>
+        <v>3323</v>
       </c>
       <c r="E30" s="1">
         <v>1</v>
@@ -30262,7 +30271,7 @@
         <v>726</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>3326</v>
+        <v>3325</v>
       </c>
       <c r="E31" s="1">
         <v>2</v>
@@ -30282,7 +30291,7 @@
         <v>1986</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>3327</v>
+        <v>3326</v>
       </c>
       <c r="E32" s="1">
         <v>3</v>
@@ -30302,7 +30311,7 @@
         <v>1987</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>3328</v>
+        <v>3327</v>
       </c>
       <c r="E33" s="1">
         <v>4</v>
@@ -30322,7 +30331,7 @@
         <v>1358</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>3329</v>
+        <v>3328</v>
       </c>
       <c r="E34" s="1">
         <v>0</v>
@@ -30496,13 +30505,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>3575</v>
+        <v>3574</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>1516</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
       <c r="E43" s="1">
         <v>0</v>
@@ -30516,7 +30525,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>3575</v>
+        <v>3574</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>1515</v>
@@ -30536,13 +30545,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>3575</v>
+        <v>3574</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>1514</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>3577</v>
+        <v>3576</v>
       </c>
       <c r="E45" s="1">
         <v>2</v>
@@ -30556,10 +30565,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>3575</v>
+        <v>3574</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>3578</v>
+        <v>3577</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>3223</v>
@@ -30576,13 +30585,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>3575</v>
+        <v>3574</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>1696</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>3224</v>
+        <v>867</v>
       </c>
       <c r="E47" s="1">
         <v>4</v>
@@ -30590,6 +30599,66 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="15">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>3619</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>3620</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>3621</v>
+      </c>
+      <c r="E48" s="1">
+        <v>0</v>
+      </c>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="15">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>3619</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>1696</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>867</v>
+      </c>
+      <c r="E49" s="1">
+        <v>1</v>
+      </c>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="15">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>3619</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>1300</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>826</v>
+      </c>
+      <c r="E50" s="1">
+        <v>2</v>
+      </c>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -31531,7 +31600,7 @@
         <v>719</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3350</v>
+        <v>3349</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -31564,7 +31633,7 @@
         <v>722</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>3351</v>
+        <v>3350</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -31572,10 +31641,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>3363</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>3364</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>3365</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -31586,7 +31655,7 @@
         <v>723</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>3352</v>
+        <v>3351</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -31597,7 +31666,7 @@
         <v>724</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -31608,7 +31677,7 @@
         <v>725</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>3354</v>
+        <v>3353</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -31619,7 +31688,7 @@
         <v>726</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>3325</v>
+        <v>3324</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -31630,7 +31699,7 @@
         <v>727</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>3355</v>
+        <v>3354</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -31641,7 +31710,7 @@
         <v>728</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>3356</v>
+        <v>3355</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -31652,7 +31721,7 @@
         <v>729</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>3357</v>
+        <v>3356</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -31663,7 +31732,7 @@
         <v>730</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>3358</v>
+        <v>3357</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -31671,10 +31740,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>3365</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>3366</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>3367</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -31685,7 +31754,7 @@
         <v>1301</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>3359</v>
+        <v>3358</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -31696,7 +31765,7 @@
         <v>690</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>3360</v>
+        <v>3359</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -31707,7 +31776,7 @@
         <v>731</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>3361</v>
+        <v>3360</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -31718,7 +31787,7 @@
         <v>732</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>3362</v>
+        <v>3361</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -31729,7 +31798,7 @@
         <v>733</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>3363</v>
+        <v>3362</v>
       </c>
     </row>
   </sheetData>
@@ -31769,10 +31838,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3505</v>
+        <v>3504</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3499</v>
+        <v>3498</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -31780,10 +31849,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3495</v>
+        <v>3494</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>3500</v>
+        <v>3499</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -31791,10 +31860,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3496</v>
+        <v>3495</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>3501</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -31802,10 +31871,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3506</v>
+        <v>3505</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>3518</v>
+        <v>3517</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -31813,7 +31882,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>3507</v>
+        <v>3506</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>2808</v>
@@ -31838,7 +31907,7 @@
         <v>1358</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>3329</v>
+        <v>3328</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -31849,7 +31918,7 @@
         <v>1369</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>3519</v>
+        <v>3518</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -31860,7 +31929,7 @@
         <v>724</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>3353</v>
+        <v>3352</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -31868,10 +31937,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>3508</v>
+        <v>3507</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>3520</v>
+        <v>3519</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -31879,10 +31948,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>3509</v>
+        <v>3508</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>3521</v>
+        <v>3520</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -31890,10 +31959,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>3510</v>
+        <v>3509</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>3522</v>
+        <v>3521</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -31901,10 +31970,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>3511</v>
+        <v>3510</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>3523</v>
+        <v>3522</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -31912,10 +31981,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>3512</v>
+        <v>3511</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>3502</v>
+        <v>3501</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -31923,10 +31992,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>3497</v>
+        <v>3496</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>3503</v>
+        <v>3502</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -31934,10 +32003,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>3498</v>
+        <v>3497</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>3504</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -31945,10 +32014,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>3513</v>
+        <v>3512</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>3524</v>
+        <v>3523</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -31956,10 +32025,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>3514</v>
+        <v>3513</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>3525</v>
+        <v>3524</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -31970,7 +32039,7 @@
         <v>1106</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>3410</v>
+        <v>3409</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -31978,10 +32047,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>3515</v>
+        <v>3514</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>3526</v>
+        <v>3525</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -31989,10 +32058,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>3516</v>
+        <v>3515</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>3527</v>
+        <v>3526</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -32000,10 +32069,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>3517</v>
+        <v>3516</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>3528</v>
+        <v>3527</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -32014,7 +32083,7 @@
         <v>1107</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>3371</v>
+        <v>3370</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -32025,7 +32094,7 @@
         <v>1108</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>3473</v>
+        <v>3472</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -32036,7 +32105,7 @@
         <v>1109</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>3474</v>
+        <v>3473</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -32047,7 +32116,7 @@
         <v>1110</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>3475</v>
+        <v>3474</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -32058,7 +32127,7 @@
         <v>1111</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>3492</v>
+        <v>3491</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -32069,7 +32138,7 @@
         <v>1112</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>3493</v>
+        <v>3492</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -32077,10 +32146,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>3371</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>3372</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>3373</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -32088,10 +32157,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>3373</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>3374</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>3375</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -32102,7 +32171,7 @@
         <v>736</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>3424</v>
+        <v>3423</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -32113,7 +32182,7 @@
         <v>737</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>3425</v>
+        <v>3424</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -32121,10 +32190,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>3470</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>3471</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>3472</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -32146,7 +32215,7 @@
         <v>1114</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>3426</v>
+        <v>3425</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -32154,7 +32223,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>3283</v>
+        <v>3282</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>863</v>
@@ -32168,7 +32237,7 @@
         <v>1115</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>3427</v>
+        <v>3426</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -32179,7 +32248,7 @@
         <v>738</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>3428</v>
+        <v>3427</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -32190,7 +32259,7 @@
         <v>1116</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>3460</v>
+        <v>3459</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -32212,7 +32281,7 @@
         <v>2011</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>3431</v>
+        <v>3430</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -32245,7 +32314,7 @@
         <v>739</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>3368</v>
+        <v>3367</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -32256,7 +32325,7 @@
         <v>1118</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>3468</v>
+        <v>3467</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -32264,10 +32333,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>3470</v>
+        <v>3469</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>3469</v>
+        <v>3468</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -32278,7 +32347,7 @@
         <v>746</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>3484</v>
+        <v>3483</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -32289,7 +32358,7 @@
         <v>747</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>3485</v>
+        <v>3484</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -32300,7 +32369,7 @@
         <v>748</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>3369</v>
+        <v>3368</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -32311,7 +32380,7 @@
         <v>749</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>3370</v>
+        <v>3369</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -32322,7 +32391,7 @@
         <v>750</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>3486</v>
+        <v>3485</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -32333,7 +32402,7 @@
         <v>751</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>3487</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -32352,10 +32421,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>3487</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>3488</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>3489</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -32363,10 +32432,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>3489</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>3490</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>3491</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -32377,7 +32446,7 @@
         <v>1119</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>3430</v>
+        <v>3429</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -32396,7 +32465,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>3298</v>
+        <v>3297</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>409</v>
@@ -32407,7 +32476,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>3299</v>
+        <v>3298</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>865</v>
@@ -32421,7 +32490,7 @@
         <v>1121</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -32451,10 +32520,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>3301</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>3302</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>3303</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -32462,10 +32531,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>3304</v>
+        <v>3303</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>3307</v>
+        <v>3306</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -32476,7 +32545,7 @@
         <v>741</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>3477</v>
+        <v>3476</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -32487,7 +32556,7 @@
         <v>742</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>3480</v>
+        <v>3479</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -32498,7 +32567,7 @@
         <v>743</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>3481</v>
+        <v>3480</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -32509,7 +32578,7 @@
         <v>744</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>3482</v>
+        <v>3481</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -32520,7 +32589,7 @@
         <v>745</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>3483</v>
+        <v>3482</v>
       </c>
     </row>
   </sheetData>
@@ -32552,13 +32621,13 @@
         <v>1746</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>3382</v>
+        <v>3381</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>929</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>3384</v>
+        <v>3383</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>686</v>
@@ -32569,16 +32638,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>3385</v>
+        <v>3384</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1031</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>3375</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>3376</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>3377</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -32586,16 +32655,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>3383</v>
+        <v>3382</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>3386</v>
+        <v>3385</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>3377</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>3378</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>3379</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -32603,16 +32672,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>3387</v>
+        <v>3386</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>927</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>3379</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>3380</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>3381</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -32620,16 +32689,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>3388</v>
+        <v>3387</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>928</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>3379</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>3380</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>3381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The data dictionary module is perfect
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnpc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnpc/locale/locale-en.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E13EB0A-A95E-4F8C-8744-E5D27003E706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E66ADA-E486-43BD-B819-8D995FD58D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3829" uniqueCount="3622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3832" uniqueCount="3626">
   <si>
     <t>myself</t>
   </si>
@@ -13522,11 +13522,26 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>字典</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dictionary</t>
+    <t>基础字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>驱动配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Base fields</t>
+  </si>
+  <si>
+    <t>字段来源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The source of the field</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>columnDataSource</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -20570,10 +20585,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FBAC76-7507-496A-9947-9F636F0BCBC6}">
-  <dimension ref="A1:D646"/>
+  <dimension ref="A1:D647"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A628" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C653" sqref="C653"/>
+    <sheetView tabSelected="1" topLeftCell="A535" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B556" sqref="B556"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -28358,13 +28373,13 @@
         <v>555</v>
       </c>
       <c r="B556" s="5" t="s">
-        <v>506</v>
-      </c>
-      <c r="C556" s="9" t="s">
-        <v>1678</v>
-      </c>
-      <c r="D556" s="1" t="s">
-        <v>3204</v>
+        <v>3625</v>
+      </c>
+      <c r="C556" s="18" t="s">
+        <v>3623</v>
+      </c>
+      <c r="D556" s="9" t="s">
+        <v>3624</v>
       </c>
     </row>
     <row r="557" spans="1:4">
@@ -28372,13 +28387,13 @@
         <v>556</v>
       </c>
       <c r="B557" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C557" s="9" t="s">
-        <v>3307</v>
+        <v>1678</v>
       </c>
       <c r="D557" s="1" t="s">
-        <v>866</v>
+        <v>3204</v>
       </c>
     </row>
     <row r="558" spans="1:4">
@@ -28386,13 +28401,13 @@
         <v>557</v>
       </c>
       <c r="B558" s="5" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C558" s="9" t="s">
-        <v>1680</v>
+        <v>3307</v>
       </c>
       <c r="D558" s="1" t="s">
-        <v>3205</v>
+        <v>866</v>
       </c>
     </row>
     <row r="559" spans="1:4">
@@ -28400,13 +28415,13 @@
         <v>558</v>
       </c>
       <c r="B559" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C559" s="9" t="s">
-        <v>1679</v>
+        <v>1680</v>
       </c>
       <c r="D559" s="1" t="s">
-        <v>3206</v>
+        <v>3205</v>
       </c>
     </row>
     <row r="560" spans="1:4">
@@ -28414,13 +28429,13 @@
         <v>559</v>
       </c>
       <c r="B560" s="5" t="s">
-        <v>548</v>
+        <v>509</v>
       </c>
       <c r="C560" s="9" t="s">
-        <v>1517</v>
+        <v>1679</v>
       </c>
       <c r="D560" s="1" t="s">
-        <v>3020</v>
+        <v>3206</v>
       </c>
     </row>
     <row r="561" spans="1:4">
@@ -28428,13 +28443,13 @@
         <v>560</v>
       </c>
       <c r="B561" s="5" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C561" s="9" t="s">
-        <v>1680</v>
+        <v>1517</v>
       </c>
       <c r="D561" s="1" t="s">
-        <v>3207</v>
+        <v>3020</v>
       </c>
     </row>
     <row r="562" spans="1:4">
@@ -28442,13 +28457,13 @@
         <v>561</v>
       </c>
       <c r="B562" s="5" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C562" s="9" t="s">
-        <v>1518</v>
+        <v>1680</v>
       </c>
       <c r="D562" s="1" t="s">
-        <v>2776</v>
+        <v>3207</v>
       </c>
     </row>
     <row r="563" spans="1:4">
@@ -28456,13 +28471,13 @@
         <v>562</v>
       </c>
       <c r="B563" s="5" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C563" s="9" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="D563" s="1" t="s">
-        <v>2777</v>
+        <v>2776</v>
       </c>
     </row>
     <row r="564" spans="1:4">
@@ -28470,13 +28485,13 @@
         <v>563</v>
       </c>
       <c r="B564" s="5" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C564" s="9" t="s">
-        <v>1681</v>
+        <v>1519</v>
       </c>
       <c r="D564" s="1" t="s">
-        <v>3208</v>
+        <v>2777</v>
       </c>
     </row>
     <row r="565" spans="1:4">
@@ -28484,13 +28499,13 @@
         <v>564</v>
       </c>
       <c r="B565" s="5" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C565" s="9" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="D565" s="1" t="s">
-        <v>3209</v>
+        <v>3208</v>
       </c>
     </row>
     <row r="566" spans="1:4">
@@ -28498,13 +28513,13 @@
         <v>565</v>
       </c>
       <c r="B566" s="5" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C566" s="9" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="D566" s="1" t="s">
-        <v>3210</v>
+        <v>3209</v>
       </c>
     </row>
     <row r="567" spans="1:4">
@@ -28512,13 +28527,13 @@
         <v>566</v>
       </c>
       <c r="B567" s="5" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C567" s="9" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="D567" s="1" t="s">
-        <v>3211</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="568" spans="1:4">
@@ -28526,13 +28541,13 @@
         <v>567</v>
       </c>
       <c r="B568" s="5" t="s">
-        <v>588</v>
+        <v>556</v>
       </c>
       <c r="C568" s="9" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="D568" s="1" t="s">
-        <v>3212</v>
+        <v>3211</v>
       </c>
     </row>
     <row r="569" spans="1:4">
@@ -28540,13 +28555,13 @@
         <v>568</v>
       </c>
       <c r="B569" s="5" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="C569" s="9" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="D569" s="1" t="s">
-        <v>3213</v>
+        <v>3212</v>
       </c>
     </row>
     <row r="570" spans="1:4">
@@ -28554,13 +28569,13 @@
         <v>569</v>
       </c>
       <c r="B570" s="5" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C570" s="9" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
       <c r="D570" s="1" t="s">
-        <v>3214</v>
+        <v>3213</v>
       </c>
     </row>
     <row r="571" spans="1:4">
@@ -28568,13 +28583,13 @@
         <v>570</v>
       </c>
       <c r="B571" s="5" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C571" s="9" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="D571" s="1" t="s">
-        <v>3215</v>
+        <v>3214</v>
       </c>
     </row>
     <row r="572" spans="1:4">
@@ -28582,13 +28597,13 @@
         <v>571</v>
       </c>
       <c r="B572" s="5" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="C572" s="9" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="D572" s="1" t="s">
-        <v>3216</v>
+        <v>3215</v>
       </c>
     </row>
     <row r="573" spans="1:4">
@@ -28596,13 +28611,13 @@
         <v>572</v>
       </c>
       <c r="B573" s="5" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C573" s="9" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="D573" s="1" t="s">
-        <v>3217</v>
+        <v>3216</v>
       </c>
     </row>
     <row r="574" spans="1:4">
@@ -28610,13 +28625,13 @@
         <v>573</v>
       </c>
       <c r="B574" s="5" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C574" s="9" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="D574" s="1" t="s">
-        <v>3218</v>
+        <v>3217</v>
       </c>
     </row>
     <row r="575" spans="1:4">
@@ -28624,13 +28639,13 @@
         <v>574</v>
       </c>
       <c r="B575" s="5" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C575" s="9" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="D575" s="1" t="s">
-        <v>3219</v>
+        <v>3218</v>
       </c>
     </row>
     <row r="576" spans="1:4">
@@ -28638,13 +28653,13 @@
         <v>575</v>
       </c>
       <c r="B576" s="5" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C576" s="9" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="D576" s="1" t="s">
-        <v>3220</v>
+        <v>3219</v>
       </c>
     </row>
     <row r="577" spans="1:4">
@@ -28652,13 +28667,13 @@
         <v>576</v>
       </c>
       <c r="B577" s="5" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C577" s="9" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="D577" s="1" t="s">
-        <v>3221</v>
+        <v>3220</v>
       </c>
     </row>
     <row r="578" spans="1:4">
@@ -28666,13 +28681,13 @@
         <v>577</v>
       </c>
       <c r="B578" s="5" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C578" s="9" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="D578" s="1" t="s">
-        <v>3222</v>
+        <v>3221</v>
       </c>
     </row>
     <row r="579" spans="1:4">
@@ -28680,13 +28695,13 @@
         <v>578</v>
       </c>
       <c r="B579" s="5" t="s">
-        <v>680</v>
+        <v>595</v>
       </c>
       <c r="C579" s="9" t="s">
-        <v>1697</v>
+        <v>1695</v>
       </c>
       <c r="D579" s="1" t="s">
-        <v>3410</v>
+        <v>3222</v>
       </c>
     </row>
     <row r="580" spans="1:4">
@@ -28694,13 +28709,13 @@
         <v>579</v>
       </c>
       <c r="B580" s="5" t="s">
-        <v>935</v>
+        <v>680</v>
       </c>
       <c r="C580" s="9" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="D580" s="1" t="s">
-        <v>3224</v>
+        <v>3410</v>
       </c>
     </row>
     <row r="581" spans="1:4">
@@ -28708,13 +28723,13 @@
         <v>580</v>
       </c>
       <c r="B581" s="5" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="C581" s="9" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="D581" s="1" t="s">
-        <v>3225</v>
+        <v>3224</v>
       </c>
     </row>
     <row r="582" spans="1:4">
@@ -28722,13 +28737,13 @@
         <v>581</v>
       </c>
       <c r="B582" s="5" t="s">
-        <v>756</v>
-      </c>
-      <c r="C582" s="13" t="s">
-        <v>3406</v>
-      </c>
-      <c r="D582" s="4" t="s">
-        <v>3408</v>
+        <v>934</v>
+      </c>
+      <c r="C582" s="9" t="s">
+        <v>1699</v>
+      </c>
+      <c r="D582" s="1" t="s">
+        <v>3225</v>
       </c>
     </row>
     <row r="583" spans="1:4">
@@ -28736,13 +28751,13 @@
         <v>582</v>
       </c>
       <c r="B583" s="5" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="C583" s="13" t="s">
-        <v>3405</v>
+        <v>3406</v>
       </c>
       <c r="D583" s="4" t="s">
-        <v>3407</v>
+        <v>3408</v>
       </c>
     </row>
     <row r="584" spans="1:4">
@@ -28750,13 +28765,13 @@
         <v>583</v>
       </c>
       <c r="B584" s="5" t="s">
-        <v>880</v>
-      </c>
-      <c r="C584" s="9" t="s">
-        <v>1700</v>
-      </c>
-      <c r="D584" s="1" t="s">
-        <v>3226</v>
+        <v>757</v>
+      </c>
+      <c r="C584" s="13" t="s">
+        <v>3405</v>
+      </c>
+      <c r="D584" s="4" t="s">
+        <v>3407</v>
       </c>
     </row>
     <row r="585" spans="1:4">
@@ -28764,13 +28779,13 @@
         <v>584</v>
       </c>
       <c r="B585" s="5" t="s">
-        <v>876</v>
+        <v>880</v>
       </c>
       <c r="C585" s="9" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="D585" s="1" t="s">
-        <v>3227</v>
+        <v>3226</v>
       </c>
     </row>
     <row r="586" spans="1:4">
@@ -28778,13 +28793,13 @@
         <v>585</v>
       </c>
       <c r="B586" s="5" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="C586" s="9" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="D586" s="1" t="s">
-        <v>3228</v>
+        <v>3227</v>
       </c>
     </row>
     <row r="587" spans="1:4">
@@ -28792,13 +28807,13 @@
         <v>586</v>
       </c>
       <c r="B587" s="5" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C587" s="9" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="D587" s="1" t="s">
-        <v>3229</v>
+        <v>3228</v>
       </c>
     </row>
     <row r="588" spans="1:4">
@@ -28806,13 +28821,13 @@
         <v>587</v>
       </c>
       <c r="B588" s="5" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="C588" s="9" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="D588" s="1" t="s">
-        <v>3230</v>
+        <v>3229</v>
       </c>
     </row>
     <row r="589" spans="1:4">
@@ -28820,13 +28835,13 @@
         <v>588</v>
       </c>
       <c r="B589" s="5" t="s">
-        <v>901</v>
+        <v>879</v>
       </c>
       <c r="C589" s="9" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="D589" s="1" t="s">
-        <v>3231</v>
+        <v>3230</v>
       </c>
     </row>
     <row r="590" spans="1:4">
@@ -28834,13 +28849,13 @@
         <v>589</v>
       </c>
       <c r="B590" s="5" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="C590" s="9" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="D590" s="1" t="s">
-        <v>3232</v>
+        <v>3231</v>
       </c>
     </row>
     <row r="591" spans="1:4">
@@ -28848,13 +28863,13 @@
         <v>590</v>
       </c>
       <c r="B591" s="5" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="C591" s="9" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="D591" s="1" t="s">
-        <v>3233</v>
+        <v>3232</v>
       </c>
     </row>
     <row r="592" spans="1:4">
@@ -28862,13 +28877,13 @@
         <v>591</v>
       </c>
       <c r="B592" s="5" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="C592" s="9" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="D592" s="1" t="s">
-        <v>3234</v>
+        <v>3233</v>
       </c>
     </row>
     <row r="593" spans="1:4">
@@ -28876,13 +28891,13 @@
         <v>592</v>
       </c>
       <c r="B593" s="5" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="C593" s="9" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="D593" s="1" t="s">
-        <v>3235</v>
+        <v>3234</v>
       </c>
     </row>
     <row r="594" spans="1:4">
@@ -28890,13 +28905,13 @@
         <v>593</v>
       </c>
       <c r="B594" s="5" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="C594" s="9" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="D594" s="1" t="s">
-        <v>3236</v>
+        <v>3235</v>
       </c>
     </row>
     <row r="595" spans="1:4">
@@ -28904,13 +28919,13 @@
         <v>594</v>
       </c>
       <c r="B595" s="5" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="C595" s="9" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="D595" s="1" t="s">
-        <v>3237</v>
+        <v>3236</v>
       </c>
     </row>
     <row r="596" spans="1:4">
@@ -28918,13 +28933,13 @@
         <v>595</v>
       </c>
       <c r="B596" s="5" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="C596" s="9" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="D596" s="1" t="s">
-        <v>3238</v>
+        <v>3237</v>
       </c>
     </row>
     <row r="597" spans="1:4">
@@ -28932,13 +28947,13 @@
         <v>596</v>
       </c>
       <c r="B597" s="5" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="C597" s="9" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="D597" s="1" t="s">
-        <v>3239</v>
+        <v>3238</v>
       </c>
     </row>
     <row r="598" spans="1:4">
@@ -28946,13 +28961,13 @@
         <v>597</v>
       </c>
       <c r="B598" s="5" t="s">
-        <v>918</v>
+        <v>909</v>
       </c>
       <c r="C598" s="9" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="D598" s="1" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="599" spans="1:4">
@@ -28960,13 +28975,13 @@
         <v>598</v>
       </c>
       <c r="B599" s="5" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="C599" s="9" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="D599" s="1" t="s">
-        <v>3241</v>
+        <v>3240</v>
       </c>
     </row>
     <row r="600" spans="1:4">
@@ -28974,13 +28989,13 @@
         <v>599</v>
       </c>
       <c r="B600" s="5" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="C600" s="9" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="D600" s="1" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="601" spans="1:4">
@@ -28988,13 +29003,13 @@
         <v>600</v>
       </c>
       <c r="B601" s="5" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="C601" s="9" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="D601" s="1" t="s">
-        <v>3243</v>
+        <v>3242</v>
       </c>
     </row>
     <row r="602" spans="1:4">
@@ -29002,13 +29017,13 @@
         <v>601</v>
       </c>
       <c r="B602" s="5" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C602" s="9" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="D602" s="1" t="s">
-        <v>3244</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="603" spans="1:4">
@@ -29016,13 +29031,13 @@
         <v>602</v>
       </c>
       <c r="B603" s="5" t="s">
-        <v>910</v>
+        <v>922</v>
       </c>
       <c r="C603" s="9" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="D603" s="1" t="s">
-        <v>3245</v>
+        <v>3244</v>
       </c>
     </row>
     <row r="604" spans="1:4">
@@ -29030,13 +29045,13 @@
         <v>603</v>
       </c>
       <c r="B604" s="5" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C604" s="9" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="D604" s="1" t="s">
-        <v>3246</v>
+        <v>3245</v>
       </c>
     </row>
     <row r="605" spans="1:4">
@@ -29044,13 +29059,13 @@
         <v>604</v>
       </c>
       <c r="B605" s="5" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="C605" s="9" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="D605" s="1" t="s">
-        <v>3247</v>
+        <v>3246</v>
       </c>
     </row>
     <row r="606" spans="1:4">
@@ -29058,13 +29073,13 @@
         <v>605</v>
       </c>
       <c r="B606" s="5" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C606" s="9" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="D606" s="1" t="s">
-        <v>3248</v>
+        <v>3247</v>
       </c>
     </row>
     <row r="607" spans="1:4">
@@ -29072,13 +29087,13 @@
         <v>606</v>
       </c>
       <c r="B607" s="5" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C607" s="9" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="D607" s="1" t="s">
-        <v>3249</v>
+        <v>3248</v>
       </c>
     </row>
     <row r="608" spans="1:4">
@@ -29086,13 +29101,13 @@
         <v>607</v>
       </c>
       <c r="B608" s="5" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C608" s="9" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="D608" s="1" t="s">
-        <v>3250</v>
+        <v>3249</v>
       </c>
     </row>
     <row r="609" spans="1:4">
@@ -29100,13 +29115,13 @@
         <v>608</v>
       </c>
       <c r="B609" s="5" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="C609" s="9" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="D609" s="1" t="s">
-        <v>3251</v>
+        <v>3250</v>
       </c>
     </row>
     <row r="610" spans="1:4">
@@ -29114,27 +29129,27 @@
         <v>609</v>
       </c>
       <c r="B610" s="5" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="C610" s="9" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="D610" s="1" t="s">
-        <v>3252</v>
+        <v>3251</v>
       </c>
     </row>
     <row r="611" spans="1:4">
       <c r="A611" s="15">
         <v>610</v>
       </c>
-      <c r="B611" s="6" t="s">
-        <v>930</v>
-      </c>
-      <c r="C611" s="13" t="s">
-        <v>1727</v>
-      </c>
-      <c r="D611" s="4" t="s">
-        <v>3253</v>
+      <c r="B611" s="5" t="s">
+        <v>917</v>
+      </c>
+      <c r="C611" s="9" t="s">
+        <v>1726</v>
+      </c>
+      <c r="D611" s="1" t="s">
+        <v>3252</v>
       </c>
     </row>
     <row r="612" spans="1:4">
@@ -29142,13 +29157,13 @@
         <v>611</v>
       </c>
       <c r="B612" s="6" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="C612" s="13" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="D612" s="4" t="s">
-        <v>3254</v>
+        <v>3253</v>
       </c>
     </row>
     <row r="613" spans="1:4">
@@ -29156,27 +29171,27 @@
         <v>612</v>
       </c>
       <c r="B613" s="6" t="s">
-        <v>932</v>
-      </c>
-      <c r="C613" s="9" t="s">
-        <v>1729</v>
-      </c>
-      <c r="D613" s="1" t="s">
-        <v>3255</v>
+        <v>931</v>
+      </c>
+      <c r="C613" s="13" t="s">
+        <v>1728</v>
+      </c>
+      <c r="D613" s="4" t="s">
+        <v>3254</v>
       </c>
     </row>
     <row r="614" spans="1:4">
       <c r="A614" s="15">
         <v>613</v>
       </c>
-      <c r="B614" s="5" t="s">
-        <v>933</v>
+      <c r="B614" s="6" t="s">
+        <v>932</v>
       </c>
       <c r="C614" s="9" t="s">
-        <v>3308</v>
+        <v>1729</v>
       </c>
       <c r="D614" s="1" t="s">
-        <v>3309</v>
+        <v>3255</v>
       </c>
     </row>
     <row r="615" spans="1:4">
@@ -29184,13 +29199,13 @@
         <v>614</v>
       </c>
       <c r="B615" s="5" t="s">
-        <v>1092</v>
+        <v>933</v>
       </c>
       <c r="C615" s="9" t="s">
-        <v>1730</v>
+        <v>3308</v>
       </c>
       <c r="D615" s="1" t="s">
-        <v>3256</v>
+        <v>3309</v>
       </c>
     </row>
     <row r="616" spans="1:4">
@@ -29198,13 +29213,13 @@
         <v>615</v>
       </c>
       <c r="B616" s="5" t="s">
-        <v>1095</v>
+        <v>1092</v>
       </c>
       <c r="C616" s="9" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="D616" s="1" t="s">
-        <v>3257</v>
+        <v>3256</v>
       </c>
     </row>
     <row r="617" spans="1:4">
@@ -29212,13 +29227,13 @@
         <v>616</v>
       </c>
       <c r="B617" s="5" t="s">
-        <v>1093</v>
+        <v>1095</v>
       </c>
       <c r="C617" s="9" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="D617" s="1" t="s">
-        <v>3258</v>
+        <v>3257</v>
       </c>
     </row>
     <row r="618" spans="1:4">
@@ -29226,13 +29241,13 @@
         <v>617</v>
       </c>
       <c r="B618" s="5" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="C618" s="9" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="D618" s="1" t="s">
-        <v>3259</v>
+        <v>3258</v>
       </c>
     </row>
     <row r="619" spans="1:4">
@@ -29240,13 +29255,13 @@
         <v>618</v>
       </c>
       <c r="B619" s="5" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
       <c r="C619" s="9" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="D619" s="1" t="s">
-        <v>3260</v>
+        <v>3259</v>
       </c>
     </row>
     <row r="620" spans="1:4">
@@ -29254,13 +29269,13 @@
         <v>619</v>
       </c>
       <c r="B620" s="5" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="C620" s="9" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="D620" s="1" t="s">
-        <v>3261</v>
+        <v>3260</v>
       </c>
     </row>
     <row r="621" spans="1:4">
@@ -29268,13 +29283,13 @@
         <v>620</v>
       </c>
       <c r="B621" s="5" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="C621" s="9" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="D621" s="1" t="s">
-        <v>3262</v>
+        <v>3261</v>
       </c>
     </row>
     <row r="622" spans="1:4">
@@ -29282,13 +29297,13 @@
         <v>621</v>
       </c>
       <c r="B622" s="5" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="C622" s="9" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="D622" s="1" t="s">
-        <v>3263</v>
+        <v>3262</v>
       </c>
     </row>
     <row r="623" spans="1:4">
@@ -29296,13 +29311,13 @@
         <v>622</v>
       </c>
       <c r="B623" s="5" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="C623" s="9" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="D623" s="1" t="s">
-        <v>3264</v>
+        <v>3263</v>
       </c>
     </row>
     <row r="624" spans="1:4">
@@ -29310,13 +29325,13 @@
         <v>623</v>
       </c>
       <c r="B624" s="5" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="C624" s="9" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="D624" s="1" t="s">
-        <v>3265</v>
+        <v>3264</v>
       </c>
     </row>
     <row r="625" spans="1:4">
@@ -29324,13 +29339,13 @@
         <v>624</v>
       </c>
       <c r="B625" s="5" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="C625" s="9" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="D625" s="1" t="s">
-        <v>3266</v>
+        <v>3265</v>
       </c>
     </row>
     <row r="626" spans="1:4">
@@ -29338,41 +29353,41 @@
         <v>625</v>
       </c>
       <c r="B626" s="5" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="C626" s="9" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="D626" s="1" t="s">
-        <v>3267</v>
-      </c>
-    </row>
-    <row r="627" spans="1:4" ht="15">
+        <v>3266</v>
+      </c>
+    </row>
+    <row r="627" spans="1:4">
       <c r="A627" s="15">
         <v>626</v>
       </c>
-      <c r="B627" s="24" t="s">
-        <v>3564</v>
-      </c>
-      <c r="C627" s="18" t="s">
-        <v>3528</v>
-      </c>
-      <c r="D627" s="24" t="s">
-        <v>3529</v>
-      </c>
-    </row>
-    <row r="628" spans="1:4">
+      <c r="B627" s="5" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C627" s="9" t="s">
+        <v>1741</v>
+      </c>
+      <c r="D627" s="1" t="s">
+        <v>3267</v>
+      </c>
+    </row>
+    <row r="628" spans="1:4" ht="15">
       <c r="A628" s="15">
         <v>627</v>
       </c>
-      <c r="B628" s="1" t="s">
-        <v>3565</v>
-      </c>
-      <c r="C628" s="9" t="s">
-        <v>3530</v>
-      </c>
-      <c r="D628" s="1" t="s">
-        <v>3531</v>
+      <c r="B628" s="24" t="s">
+        <v>3564</v>
+      </c>
+      <c r="C628" s="18" t="s">
+        <v>3528</v>
+      </c>
+      <c r="D628" s="24" t="s">
+        <v>3529</v>
       </c>
     </row>
     <row r="629" spans="1:4">
@@ -29380,13 +29395,13 @@
         <v>628</v>
       </c>
       <c r="B629" s="1" t="s">
-        <v>3535</v>
+        <v>3565</v>
       </c>
       <c r="C629" s="9" t="s">
-        <v>3532</v>
+        <v>3530</v>
       </c>
       <c r="D629" s="1" t="s">
-        <v>3535</v>
+        <v>3531</v>
       </c>
     </row>
     <row r="630" spans="1:4">
@@ -29394,13 +29409,13 @@
         <v>629</v>
       </c>
       <c r="B630" s="1" t="s">
-        <v>3534</v>
+        <v>3535</v>
       </c>
       <c r="C630" s="9" t="s">
-        <v>3533</v>
+        <v>3532</v>
       </c>
       <c r="D630" s="1" t="s">
-        <v>3534</v>
+        <v>3535</v>
       </c>
     </row>
     <row r="631" spans="1:4">
@@ -29408,13 +29423,13 @@
         <v>630</v>
       </c>
       <c r="B631" s="1" t="s">
-        <v>3539</v>
-      </c>
-      <c r="C631" s="1" t="s">
-        <v>3536</v>
+        <v>3534</v>
+      </c>
+      <c r="C631" s="9" t="s">
+        <v>3533</v>
       </c>
       <c r="D631" s="1" t="s">
-        <v>3539</v>
+        <v>3534</v>
       </c>
     </row>
     <row r="632" spans="1:4">
@@ -29422,13 +29437,13 @@
         <v>631</v>
       </c>
       <c r="B632" s="1" t="s">
-        <v>3540</v>
+        <v>3539</v>
       </c>
       <c r="C632" s="1" t="s">
-        <v>3537</v>
+        <v>3536</v>
       </c>
       <c r="D632" s="1" t="s">
-        <v>3540</v>
+        <v>3539</v>
       </c>
     </row>
     <row r="633" spans="1:4">
@@ -29436,13 +29451,13 @@
         <v>632</v>
       </c>
       <c r="B633" s="1" t="s">
-        <v>3541</v>
+        <v>3540</v>
       </c>
       <c r="C633" s="1" t="s">
-        <v>3538</v>
+        <v>3537</v>
       </c>
       <c r="D633" s="1" t="s">
-        <v>3541</v>
+        <v>3540</v>
       </c>
     </row>
     <row r="634" spans="1:4">
@@ -29450,13 +29465,13 @@
         <v>633</v>
       </c>
       <c r="B634" s="1" t="s">
-        <v>3563</v>
+        <v>3541</v>
       </c>
       <c r="C634" s="1" t="s">
-        <v>3562</v>
+        <v>3538</v>
       </c>
       <c r="D634" s="1" t="s">
-        <v>3563</v>
+        <v>3541</v>
       </c>
     </row>
     <row r="635" spans="1:4">
@@ -29464,13 +29479,13 @@
         <v>634</v>
       </c>
       <c r="B635" s="1" t="s">
-        <v>3566</v>
+        <v>3563</v>
       </c>
       <c r="C635" s="1" t="s">
-        <v>3544</v>
+        <v>3562</v>
       </c>
       <c r="D635" s="1" t="s">
-        <v>3545</v>
+        <v>3563</v>
       </c>
     </row>
     <row r="636" spans="1:4">
@@ -29478,13 +29493,13 @@
         <v>635</v>
       </c>
       <c r="B636" s="1" t="s">
-        <v>3567</v>
+        <v>3566</v>
       </c>
       <c r="C636" s="1" t="s">
-        <v>3546</v>
+        <v>3544</v>
       </c>
       <c r="D636" s="1" t="s">
-        <v>3547</v>
+        <v>3545</v>
       </c>
     </row>
     <row r="637" spans="1:4">
@@ -29492,13 +29507,13 @@
         <v>636</v>
       </c>
       <c r="B637" s="1" t="s">
-        <v>3568</v>
+        <v>3567</v>
       </c>
       <c r="C637" s="1" t="s">
-        <v>3548</v>
+        <v>3546</v>
       </c>
       <c r="D637" s="1" t="s">
-        <v>3549</v>
+        <v>3547</v>
       </c>
     </row>
     <row r="638" spans="1:4">
@@ -29506,13 +29521,13 @@
         <v>637</v>
       </c>
       <c r="B638" s="1" t="s">
-        <v>3569</v>
+        <v>3568</v>
       </c>
       <c r="C638" s="1" t="s">
-        <v>3550</v>
+        <v>3548</v>
       </c>
       <c r="D638" s="1" t="s">
-        <v>3551</v>
+        <v>3549</v>
       </c>
     </row>
     <row r="639" spans="1:4">
@@ -29520,13 +29535,13 @@
         <v>638</v>
       </c>
       <c r="B639" s="1" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C639" s="18" t="s">
-        <v>3552</v>
+        <v>3569</v>
+      </c>
+      <c r="C639" s="1" t="s">
+        <v>3550</v>
       </c>
       <c r="D639" s="1" t="s">
-        <v>3553</v>
+        <v>3551</v>
       </c>
     </row>
     <row r="640" spans="1:4">
@@ -29534,13 +29549,13 @@
         <v>639</v>
       </c>
       <c r="B640" s="1" t="s">
-        <v>3570</v>
-      </c>
-      <c r="C640" s="1" t="s">
-        <v>3554</v>
+        <v>3553</v>
+      </c>
+      <c r="C640" s="18" t="s">
+        <v>3552</v>
       </c>
       <c r="D640" s="1" t="s">
-        <v>3555</v>
+        <v>3553</v>
       </c>
     </row>
     <row r="641" spans="1:4">
@@ -29548,13 +29563,13 @@
         <v>640</v>
       </c>
       <c r="B641" s="1" t="s">
-        <v>3571</v>
+        <v>3570</v>
       </c>
       <c r="C641" s="1" t="s">
-        <v>3556</v>
+        <v>3554</v>
       </c>
       <c r="D641" s="1" t="s">
-        <v>3557</v>
+        <v>3555</v>
       </c>
     </row>
     <row r="642" spans="1:4">
@@ -29562,13 +29577,13 @@
         <v>641</v>
       </c>
       <c r="B642" s="1" t="s">
-        <v>3572</v>
+        <v>3571</v>
       </c>
       <c r="C642" s="1" t="s">
-        <v>3558</v>
+        <v>3556</v>
       </c>
       <c r="D642" s="1" t="s">
-        <v>3559</v>
+        <v>3557</v>
       </c>
     </row>
     <row r="643" spans="1:4">
@@ -29576,27 +29591,27 @@
         <v>642</v>
       </c>
       <c r="B643" s="1" t="s">
-        <v>3573</v>
+        <v>3572</v>
       </c>
       <c r="C643" s="1" t="s">
-        <v>3560</v>
+        <v>3558</v>
       </c>
       <c r="D643" s="1" t="s">
-        <v>3561</v>
+        <v>3559</v>
       </c>
     </row>
     <row r="644" spans="1:4">
       <c r="A644" s="15">
         <v>643</v>
       </c>
-      <c r="B644" s="5" t="s">
-        <v>3578</v>
-      </c>
-      <c r="C644" s="18" t="s">
-        <v>3579</v>
-      </c>
-      <c r="D644" s="9" t="s">
-        <v>480</v>
+      <c r="B644" s="1" t="s">
+        <v>3573</v>
+      </c>
+      <c r="C644" s="1" t="s">
+        <v>3560</v>
+      </c>
+      <c r="D644" s="1" t="s">
+        <v>3561</v>
       </c>
     </row>
     <row r="645" spans="1:4">
@@ -29604,13 +29619,13 @@
         <v>644</v>
       </c>
       <c r="B645" s="5" t="s">
-        <v>3580</v>
+        <v>3578</v>
       </c>
       <c r="C645" s="18" t="s">
-        <v>3581</v>
+        <v>3579</v>
       </c>
       <c r="D645" s="9" t="s">
-        <v>3582</v>
+        <v>480</v>
       </c>
     </row>
     <row r="646" spans="1:4">
@@ -29618,12 +29633,26 @@
         <v>645</v>
       </c>
       <c r="B646" s="5" t="s">
+        <v>3580</v>
+      </c>
+      <c r="C646" s="18" t="s">
+        <v>3581</v>
+      </c>
+      <c r="D646" s="9" t="s">
+        <v>3582</v>
+      </c>
+    </row>
+    <row r="647" spans="1:4">
+      <c r="A647" s="15">
+        <v>646</v>
+      </c>
+      <c r="B647" s="5" t="s">
         <v>3586</v>
       </c>
-      <c r="C646" s="18" t="s">
+      <c r="C647" s="18" t="s">
         <v>3587</v>
       </c>
-      <c r="D646" s="9" t="s">
+      <c r="D647" s="9" t="s">
         <v>3588</v>
       </c>
     </row>
@@ -29639,7 +29668,7 @@
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -30611,7 +30640,7 @@
         <v>3620</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>3621</v>
+        <v>3622</v>
       </c>
       <c r="E48" s="1">
         <v>0</v>
@@ -30628,10 +30657,10 @@
         <v>3619</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>1696</v>
+        <v>3621</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>867</v>
+        <v>3324</v>
       </c>
       <c r="E49" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Role management module adjustment
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnpc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnpc/locale/locale-en.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03447161-CD1E-4E4A-AFD5-0417C0A3BD03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AB8EFF-EEB7-47CB-B4D8-25005F4821FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3844" uniqueCount="3631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3847" uniqueCount="3634">
   <si>
     <t>myself</t>
   </si>
@@ -13562,6 +13562,18 @@
   </si>
   <si>
     <t>操作时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>languageLicense</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>语言授权</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Language Licensing</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -20605,10 +20617,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FBAC76-7507-496A-9947-9F636F0BCBC6}">
-  <dimension ref="A1:D651"/>
+  <dimension ref="A1:D652"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D145" sqref="D145"/>
+    <sheetView tabSelected="1" topLeftCell="A406" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B431" sqref="B431"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -26643,13 +26655,13 @@
         <v>430</v>
       </c>
       <c r="B431" s="5" t="s">
-        <v>377</v>
+        <v>3631</v>
       </c>
       <c r="C431" s="9" t="s">
-        <v>1597</v>
+        <v>3632</v>
       </c>
       <c r="D431" s="1" t="s">
-        <v>3100</v>
+        <v>3633</v>
       </c>
     </row>
     <row r="432" spans="1:4">
@@ -26657,13 +26669,13 @@
         <v>431</v>
       </c>
       <c r="B432" s="5" t="s">
-        <v>1058</v>
+        <v>377</v>
       </c>
       <c r="C432" s="9" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="D432" s="1" t="s">
-        <v>3101</v>
+        <v>3100</v>
       </c>
     </row>
     <row r="433" spans="1:4">
@@ -26671,13 +26683,13 @@
         <v>432</v>
       </c>
       <c r="B433" s="5" t="s">
-        <v>378</v>
+        <v>1058</v>
       </c>
       <c r="C433" s="9" t="s">
-        <v>3280</v>
+        <v>1598</v>
       </c>
       <c r="D433" s="1" t="s">
-        <v>3281</v>
+        <v>3101</v>
       </c>
     </row>
     <row r="434" spans="1:4">
@@ -26685,13 +26697,13 @@
         <v>433</v>
       </c>
       <c r="B434" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C434" s="9" t="s">
-        <v>3282</v>
+        <v>3280</v>
       </c>
       <c r="D434" s="1" t="s">
-        <v>863</v>
+        <v>3281</v>
       </c>
     </row>
     <row r="435" spans="1:4">
@@ -26699,13 +26711,13 @@
         <v>434</v>
       </c>
       <c r="B435" s="5" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C435" s="9" t="s">
-        <v>1115</v>
+        <v>3282</v>
       </c>
       <c r="D435" s="1" t="s">
-        <v>3102</v>
+        <v>863</v>
       </c>
     </row>
     <row r="436" spans="1:4">
@@ -26713,13 +26725,13 @@
         <v>435</v>
       </c>
       <c r="B436" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C436" s="9" t="s">
-        <v>1599</v>
+        <v>1115</v>
       </c>
       <c r="D436" s="1" t="s">
-        <v>3103</v>
+        <v>3102</v>
       </c>
     </row>
     <row r="437" spans="1:4">
@@ -26727,13 +26739,13 @@
         <v>436</v>
       </c>
       <c r="B437" s="5" t="s">
-        <v>715</v>
+        <v>383</v>
       </c>
       <c r="C437" s="9" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="D437" s="1" t="s">
-        <v>3104</v>
+        <v>3103</v>
       </c>
     </row>
     <row r="438" spans="1:4">
@@ -26741,13 +26753,13 @@
         <v>437</v>
       </c>
       <c r="B438" s="5" t="s">
-        <v>384</v>
+        <v>715</v>
       </c>
       <c r="C438" s="9" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="D438" s="1" t="s">
-        <v>3105</v>
+        <v>3104</v>
       </c>
     </row>
     <row r="439" spans="1:4">
@@ -26755,13 +26767,13 @@
         <v>438</v>
       </c>
       <c r="B439" s="5" t="s">
-        <v>1027</v>
+        <v>384</v>
       </c>
       <c r="C439" s="9" t="s">
-        <v>3283</v>
+        <v>1601</v>
       </c>
       <c r="D439" s="1" t="s">
-        <v>1028</v>
+        <v>3105</v>
       </c>
     </row>
     <row r="440" spans="1:4">
@@ -26769,13 +26781,13 @@
         <v>439</v>
       </c>
       <c r="B440" s="5" t="s">
-        <v>1054</v>
+        <v>1027</v>
       </c>
       <c r="C440" s="9" t="s">
-        <v>1602</v>
+        <v>3283</v>
       </c>
       <c r="D440" s="1" t="s">
-        <v>3106</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="441" spans="1:4">
@@ -26783,13 +26795,13 @@
         <v>440</v>
       </c>
       <c r="B441" s="5" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="C441" s="9" t="s">
-        <v>3284</v>
+        <v>1602</v>
       </c>
       <c r="D441" s="1" t="s">
-        <v>3285</v>
+        <v>3106</v>
       </c>
     </row>
     <row r="442" spans="1:4">
@@ -26797,13 +26809,13 @@
         <v>441</v>
       </c>
       <c r="B442" s="5" t="s">
-        <v>1049</v>
+        <v>1055</v>
       </c>
       <c r="C442" s="9" t="s">
-        <v>1603</v>
+        <v>3284</v>
       </c>
       <c r="D442" s="1" t="s">
-        <v>3107</v>
+        <v>3285</v>
       </c>
     </row>
     <row r="443" spans="1:4">
@@ -26811,13 +26823,13 @@
         <v>442</v>
       </c>
       <c r="B443" s="5" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="C443" s="9" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="D443" s="1" t="s">
-        <v>3108</v>
+        <v>3107</v>
       </c>
     </row>
     <row r="444" spans="1:4">
@@ -26825,13 +26837,13 @@
         <v>443</v>
       </c>
       <c r="B444" s="5" t="s">
-        <v>386</v>
+        <v>1052</v>
       </c>
       <c r="C444" s="9" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="D444" s="1" t="s">
-        <v>3109</v>
+        <v>3108</v>
       </c>
     </row>
     <row r="445" spans="1:4">
@@ -26839,13 +26851,13 @@
         <v>444</v>
       </c>
       <c r="B445" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C445" s="9" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
       <c r="D445" s="1" t="s">
-        <v>3110</v>
+        <v>3109</v>
       </c>
     </row>
     <row r="446" spans="1:4">
@@ -26853,13 +26865,13 @@
         <v>445</v>
       </c>
       <c r="B446" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C446" s="9" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="D446" s="1" t="s">
-        <v>3111</v>
+        <v>3110</v>
       </c>
     </row>
     <row r="447" spans="1:4">
@@ -26867,13 +26879,13 @@
         <v>446</v>
       </c>
       <c r="B447" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C447" s="9" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="D447" s="1" t="s">
-        <v>3112</v>
+        <v>3111</v>
       </c>
     </row>
     <row r="448" spans="1:4">
@@ -26881,13 +26893,13 @@
         <v>447</v>
       </c>
       <c r="B448" s="5" t="s">
-        <v>3399</v>
+        <v>389</v>
       </c>
       <c r="C448" s="9" t="s">
-        <v>3397</v>
+        <v>1608</v>
       </c>
       <c r="D448" s="1" t="s">
-        <v>3401</v>
+        <v>3112</v>
       </c>
     </row>
     <row r="449" spans="1:4">
@@ -26895,13 +26907,13 @@
         <v>448</v>
       </c>
       <c r="B449" s="5" t="s">
-        <v>3400</v>
+        <v>3399</v>
       </c>
       <c r="C449" s="9" t="s">
-        <v>3398</v>
+        <v>3397</v>
       </c>
       <c r="D449" s="1" t="s">
-        <v>3402</v>
+        <v>3401</v>
       </c>
     </row>
     <row r="450" spans="1:4">
@@ -26909,13 +26921,13 @@
         <v>449</v>
       </c>
       <c r="B450" s="5" t="s">
-        <v>390</v>
+        <v>3400</v>
       </c>
       <c r="C450" s="9" t="s">
-        <v>1609</v>
+        <v>3398</v>
       </c>
       <c r="D450" s="1" t="s">
-        <v>3113</v>
+        <v>3402</v>
       </c>
     </row>
     <row r="451" spans="1:4">
@@ -26923,27 +26935,27 @@
         <v>450</v>
       </c>
       <c r="B451" s="5" t="s">
-        <v>2069</v>
+        <v>390</v>
       </c>
       <c r="C451" s="9" t="s">
-        <v>2070</v>
-      </c>
-      <c r="D451" s="9" t="s">
-        <v>3114</v>
+        <v>1609</v>
+      </c>
+      <c r="D451" s="1" t="s">
+        <v>3113</v>
       </c>
     </row>
     <row r="452" spans="1:4">
       <c r="A452" s="15">
         <v>451</v>
       </c>
-      <c r="B452" s="1" t="s">
-        <v>2152</v>
-      </c>
-      <c r="C452" s="22" t="s">
-        <v>2153</v>
+      <c r="B452" s="5" t="s">
+        <v>2069</v>
+      </c>
+      <c r="C452" s="9" t="s">
+        <v>2070</v>
       </c>
       <c r="D452" s="9" t="s">
-        <v>3115</v>
+        <v>3114</v>
       </c>
     </row>
     <row r="453" spans="1:4">
@@ -26951,27 +26963,27 @@
         <v>452</v>
       </c>
       <c r="B453" s="1" t="s">
-        <v>2243</v>
+        <v>2152</v>
       </c>
       <c r="C453" s="22" t="s">
-        <v>2154</v>
+        <v>2153</v>
       </c>
       <c r="D453" s="9" t="s">
-        <v>3116</v>
+        <v>3115</v>
       </c>
     </row>
     <row r="454" spans="1:4">
       <c r="A454" s="15">
         <v>453</v>
       </c>
-      <c r="B454" s="5" t="s">
-        <v>2155</v>
+      <c r="B454" s="1" t="s">
+        <v>2243</v>
       </c>
       <c r="C454" s="22" t="s">
-        <v>2156</v>
+        <v>2154</v>
       </c>
       <c r="D454" s="9" t="s">
-        <v>3117</v>
+        <v>3116</v>
       </c>
     </row>
     <row r="455" spans="1:4">
@@ -26979,13 +26991,13 @@
         <v>454</v>
       </c>
       <c r="B455" s="5" t="s">
-        <v>2160</v>
+        <v>2155</v>
       </c>
       <c r="C455" s="22" t="s">
-        <v>2161</v>
+        <v>2156</v>
       </c>
       <c r="D455" s="9" t="s">
-        <v>3118</v>
+        <v>3117</v>
       </c>
     </row>
     <row r="456" spans="1:4">
@@ -26993,13 +27005,13 @@
         <v>455</v>
       </c>
       <c r="B456" s="5" t="s">
-        <v>2238</v>
-      </c>
-      <c r="C456" s="9" t="s">
-        <v>2239</v>
+        <v>2160</v>
+      </c>
+      <c r="C456" s="22" t="s">
+        <v>2161</v>
       </c>
       <c r="D456" s="9" t="s">
-        <v>3119</v>
+        <v>3118</v>
       </c>
     </row>
     <row r="457" spans="1:4">
@@ -27007,13 +27019,13 @@
         <v>456</v>
       </c>
       <c r="B457" s="5" t="s">
-        <v>2242</v>
+        <v>2238</v>
       </c>
       <c r="C457" s="9" t="s">
-        <v>2240</v>
+        <v>2239</v>
       </c>
       <c r="D457" s="9" t="s">
-        <v>2241</v>
+        <v>3119</v>
       </c>
     </row>
     <row r="458" spans="1:4">
@@ -27021,13 +27033,13 @@
         <v>457</v>
       </c>
       <c r="B458" s="5" t="s">
-        <v>2246</v>
+        <v>2242</v>
       </c>
       <c r="C458" s="9" t="s">
-        <v>2244</v>
+        <v>2240</v>
       </c>
       <c r="D458" s="9" t="s">
-        <v>2245</v>
+        <v>2241</v>
       </c>
     </row>
     <row r="459" spans="1:4">
@@ -27035,13 +27047,13 @@
         <v>458</v>
       </c>
       <c r="B459" s="5" t="s">
-        <v>3583</v>
-      </c>
-      <c r="C459" s="25" t="s">
-        <v>3584</v>
-      </c>
-      <c r="D459" s="25" t="s">
-        <v>3585</v>
+        <v>2246</v>
+      </c>
+      <c r="C459" s="9" t="s">
+        <v>2244</v>
+      </c>
+      <c r="D459" s="9" t="s">
+        <v>2245</v>
       </c>
     </row>
     <row r="460" spans="1:4">
@@ -27049,13 +27061,13 @@
         <v>459</v>
       </c>
       <c r="B460" s="5" t="s">
-        <v>2252</v>
-      </c>
-      <c r="C460" s="9" t="s">
-        <v>2253</v>
-      </c>
-      <c r="D460" s="9" t="s">
-        <v>3120</v>
+        <v>3583</v>
+      </c>
+      <c r="C460" s="25" t="s">
+        <v>3584</v>
+      </c>
+      <c r="D460" s="25" t="s">
+        <v>3585</v>
       </c>
     </row>
     <row r="461" spans="1:4">
@@ -27063,13 +27075,13 @@
         <v>460</v>
       </c>
       <c r="B461" s="5" t="s">
-        <v>391</v>
+        <v>2252</v>
       </c>
       <c r="C461" s="9" t="s">
-        <v>1610</v>
-      </c>
-      <c r="D461" s="1" t="s">
-        <v>3121</v>
+        <v>2253</v>
+      </c>
+      <c r="D461" s="9" t="s">
+        <v>3120</v>
       </c>
     </row>
     <row r="462" spans="1:4">
@@ -27077,13 +27089,13 @@
         <v>461</v>
       </c>
       <c r="B462" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C462" s="9" t="s">
-        <v>1116</v>
+        <v>1610</v>
       </c>
       <c r="D462" s="1" t="s">
-        <v>3122</v>
+        <v>3121</v>
       </c>
     </row>
     <row r="463" spans="1:4">
@@ -27091,13 +27103,13 @@
         <v>462</v>
       </c>
       <c r="B463" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C463" s="9" t="s">
-        <v>3286</v>
+        <v>1116</v>
       </c>
       <c r="D463" s="1" t="s">
-        <v>3291</v>
+        <v>3122</v>
       </c>
     </row>
     <row r="464" spans="1:4">
@@ -27105,13 +27117,13 @@
         <v>463</v>
       </c>
       <c r="B464" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C464" s="9" t="s">
-        <v>3287</v>
+        <v>3286</v>
       </c>
       <c r="D464" s="1" t="s">
-        <v>3292</v>
+        <v>3291</v>
       </c>
     </row>
     <row r="465" spans="1:4">
@@ -27119,13 +27131,13 @@
         <v>464</v>
       </c>
       <c r="B465" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C465" s="9" t="s">
-        <v>3288</v>
+        <v>3287</v>
       </c>
       <c r="D465" s="1" t="s">
-        <v>3293</v>
+        <v>3292</v>
       </c>
     </row>
     <row r="466" spans="1:4">
@@ -27133,13 +27145,13 @@
         <v>465</v>
       </c>
       <c r="B466" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C466" s="9" t="s">
-        <v>3289</v>
+        <v>3288</v>
       </c>
       <c r="D466" s="1" t="s">
-        <v>3294</v>
+        <v>3293</v>
       </c>
     </row>
     <row r="467" spans="1:4">
@@ -27147,13 +27159,13 @@
         <v>466</v>
       </c>
       <c r="B467" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C467" s="9" t="s">
-        <v>3290</v>
+        <v>3289</v>
       </c>
       <c r="D467" s="1" t="s">
-        <v>3123</v>
+        <v>3294</v>
       </c>
     </row>
     <row r="468" spans="1:4">
@@ -27161,13 +27173,13 @@
         <v>467</v>
       </c>
       <c r="B468" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C468" s="9" t="s">
-        <v>1117</v>
+        <v>3290</v>
       </c>
       <c r="D468" s="1" t="s">
-        <v>3463</v>
+        <v>3123</v>
       </c>
     </row>
     <row r="469" spans="1:4">
@@ -27175,13 +27187,13 @@
         <v>468</v>
       </c>
       <c r="B469" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C469" s="9" t="s">
-        <v>3295</v>
+        <v>1117</v>
       </c>
       <c r="D469" s="1" t="s">
-        <v>3296</v>
+        <v>3463</v>
       </c>
     </row>
     <row r="470" spans="1:4">
@@ -27189,13 +27201,13 @@
         <v>469</v>
       </c>
       <c r="B470" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C470" s="9" t="s">
-        <v>2011</v>
+        <v>3295</v>
       </c>
       <c r="D470" s="1" t="s">
-        <v>3125</v>
+        <v>3296</v>
       </c>
     </row>
     <row r="471" spans="1:4">
@@ -27203,13 +27215,13 @@
         <v>470</v>
       </c>
       <c r="B471" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C471" s="9" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D471" s="1" t="s">
-        <v>3464</v>
+        <v>3125</v>
       </c>
     </row>
     <row r="472" spans="1:4">
@@ -27217,13 +27229,13 @@
         <v>471</v>
       </c>
       <c r="B472" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C472" s="9" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D472" s="1" t="s">
-        <v>3465</v>
+        <v>3464</v>
       </c>
     </row>
     <row r="473" spans="1:4">
@@ -27231,13 +27243,13 @@
         <v>472</v>
       </c>
       <c r="B473" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C473" s="9" t="s">
-        <v>1611</v>
+        <v>2013</v>
       </c>
       <c r="D473" s="1" t="s">
-        <v>3466</v>
+        <v>3465</v>
       </c>
     </row>
     <row r="474" spans="1:4">
@@ -27245,13 +27257,13 @@
         <v>473</v>
       </c>
       <c r="B474" s="5" t="s">
-        <v>3611</v>
+        <v>403</v>
       </c>
       <c r="C474" s="9" t="s">
-        <v>3612</v>
-      </c>
-      <c r="D474" s="9" t="s">
-        <v>3615</v>
+        <v>1611</v>
+      </c>
+      <c r="D474" s="1" t="s">
+        <v>3466</v>
       </c>
     </row>
     <row r="475" spans="1:4">
@@ -27259,13 +27271,13 @@
         <v>474</v>
       </c>
       <c r="B475" s="5" t="s">
-        <v>3613</v>
+        <v>3611</v>
       </c>
       <c r="C475" s="9" t="s">
-        <v>3614</v>
+        <v>3612</v>
       </c>
       <c r="D475" s="9" t="s">
-        <v>3616</v>
+        <v>3615</v>
       </c>
     </row>
     <row r="476" spans="1:4">
@@ -27273,13 +27285,13 @@
         <v>475</v>
       </c>
       <c r="B476" s="5" t="s">
-        <v>404</v>
+        <v>3613</v>
       </c>
       <c r="C476" s="9" t="s">
-        <v>1612</v>
-      </c>
-      <c r="D476" s="1" t="s">
-        <v>3128</v>
+        <v>3614</v>
+      </c>
+      <c r="D476" s="9" t="s">
+        <v>3616</v>
       </c>
     </row>
     <row r="477" spans="1:4">
@@ -27287,13 +27299,13 @@
         <v>476</v>
       </c>
       <c r="B477" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C477" s="9" t="s">
-        <v>2217</v>
+        <v>1612</v>
       </c>
       <c r="D477" s="1" t="s">
-        <v>3129</v>
+        <v>3128</v>
       </c>
     </row>
     <row r="478" spans="1:4">
@@ -27301,13 +27313,13 @@
         <v>477</v>
       </c>
       <c r="B478" s="5" t="s">
-        <v>2194</v>
+        <v>405</v>
       </c>
       <c r="C478" s="9" t="s">
-        <v>2195</v>
-      </c>
-      <c r="D478" s="5" t="s">
-        <v>3130</v>
+        <v>2217</v>
+      </c>
+      <c r="D478" s="1" t="s">
+        <v>3129</v>
       </c>
     </row>
     <row r="479" spans="1:4">
@@ -27315,13 +27327,13 @@
         <v>478</v>
       </c>
       <c r="B479" s="5" t="s">
-        <v>2196</v>
+        <v>2194</v>
       </c>
       <c r="C479" s="9" t="s">
-        <v>2202</v>
+        <v>2195</v>
       </c>
       <c r="D479" s="5" t="s">
-        <v>3131</v>
+        <v>3130</v>
       </c>
     </row>
     <row r="480" spans="1:4">
@@ -27329,13 +27341,13 @@
         <v>479</v>
       </c>
       <c r="B480" s="5" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="C480" s="9" t="s">
-        <v>2198</v>
+        <v>2202</v>
       </c>
       <c r="D480" s="5" t="s">
-        <v>3132</v>
+        <v>3131</v>
       </c>
     </row>
     <row r="481" spans="1:4">
@@ -27343,13 +27355,13 @@
         <v>480</v>
       </c>
       <c r="B481" s="5" t="s">
-        <v>2199</v>
+        <v>2197</v>
       </c>
       <c r="C481" s="9" t="s">
-        <v>2200</v>
+        <v>2198</v>
       </c>
       <c r="D481" s="5" t="s">
-        <v>3133</v>
+        <v>3132</v>
       </c>
     </row>
     <row r="482" spans="1:4">
@@ -27357,13 +27369,13 @@
         <v>481</v>
       </c>
       <c r="B482" s="5" t="s">
-        <v>2201</v>
+        <v>2199</v>
       </c>
       <c r="C482" s="9" t="s">
-        <v>2203</v>
+        <v>2200</v>
       </c>
       <c r="D482" s="5" t="s">
-        <v>3134</v>
+        <v>3133</v>
       </c>
     </row>
     <row r="483" spans="1:4">
@@ -27371,13 +27383,13 @@
         <v>482</v>
       </c>
       <c r="B483" s="5" t="s">
-        <v>406</v>
+        <v>2201</v>
       </c>
       <c r="C483" s="9" t="s">
-        <v>1613</v>
-      </c>
-      <c r="D483" s="1" t="s">
-        <v>3135</v>
+        <v>2203</v>
+      </c>
+      <c r="D483" s="5" t="s">
+        <v>3134</v>
       </c>
     </row>
     <row r="484" spans="1:4">
@@ -27385,13 +27397,13 @@
         <v>483</v>
       </c>
       <c r="B484" s="5" t="s">
-        <v>771</v>
+        <v>406</v>
       </c>
       <c r="C484" s="9" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="D484" s="1" t="s">
-        <v>3136</v>
+        <v>3135</v>
       </c>
     </row>
     <row r="485" spans="1:4">
@@ -27399,13 +27411,13 @@
         <v>484</v>
       </c>
       <c r="B485" s="5" t="s">
-        <v>407</v>
+        <v>771</v>
       </c>
       <c r="C485" s="9" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="D485" s="1" t="s">
-        <v>3137</v>
+        <v>3136</v>
       </c>
     </row>
     <row r="486" spans="1:4">
@@ -27413,13 +27425,13 @@
         <v>485</v>
       </c>
       <c r="B486" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C486" s="9" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="D486" s="1" t="s">
-        <v>3138</v>
+        <v>3137</v>
       </c>
     </row>
     <row r="487" spans="1:4">
@@ -27427,13 +27439,13 @@
         <v>486</v>
       </c>
       <c r="B487" s="5" t="s">
-        <v>773</v>
+        <v>408</v>
       </c>
       <c r="C487" s="9" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="D487" s="1" t="s">
-        <v>3139</v>
+        <v>3138</v>
       </c>
     </row>
     <row r="488" spans="1:4">
@@ -27441,13 +27453,13 @@
         <v>487</v>
       </c>
       <c r="B488" s="5" t="s">
-        <v>2247</v>
+        <v>773</v>
       </c>
       <c r="C488" s="9" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="D488" s="1" t="s">
-        <v>3140</v>
+        <v>3139</v>
       </c>
     </row>
     <row r="489" spans="1:4">
@@ -27455,13 +27467,13 @@
         <v>488</v>
       </c>
       <c r="B489" s="5" t="s">
-        <v>409</v>
+        <v>2247</v>
       </c>
       <c r="C489" s="9" t="s">
-        <v>3297</v>
+        <v>1618</v>
       </c>
       <c r="D489" s="1" t="s">
-        <v>864</v>
+        <v>3140</v>
       </c>
     </row>
     <row r="490" spans="1:4">
@@ -27469,13 +27481,13 @@
         <v>489</v>
       </c>
       <c r="B490" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C490" s="9" t="s">
-        <v>3298</v>
+        <v>3297</v>
       </c>
       <c r="D490" s="1" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="491" spans="1:4">
@@ -27483,13 +27495,13 @@
         <v>490</v>
       </c>
       <c r="B491" s="5" t="s">
-        <v>528</v>
+        <v>410</v>
       </c>
       <c r="C491" s="9" t="s">
-        <v>1619</v>
+        <v>3298</v>
       </c>
       <c r="D491" s="1" t="s">
-        <v>3141</v>
+        <v>865</v>
       </c>
     </row>
     <row r="492" spans="1:4">
@@ -27497,13 +27509,13 @@
         <v>491</v>
       </c>
       <c r="B492" s="5" t="s">
-        <v>2163</v>
+        <v>528</v>
       </c>
       <c r="C492" s="9" t="s">
-        <v>2164</v>
-      </c>
-      <c r="D492" s="9" t="s">
-        <v>3142</v>
+        <v>1619</v>
+      </c>
+      <c r="D492" s="1" t="s">
+        <v>3141</v>
       </c>
     </row>
     <row r="493" spans="1:4">
@@ -27511,13 +27523,13 @@
         <v>492</v>
       </c>
       <c r="B493" s="5" t="s">
-        <v>2248</v>
-      </c>
-      <c r="C493" s="22" t="s">
-        <v>2249</v>
+        <v>2163</v>
+      </c>
+      <c r="C493" s="9" t="s">
+        <v>2164</v>
       </c>
       <c r="D493" s="9" t="s">
-        <v>3143</v>
+        <v>3142</v>
       </c>
     </row>
     <row r="494" spans="1:4">
@@ -27525,13 +27537,13 @@
         <v>493</v>
       </c>
       <c r="B494" s="5" t="s">
-        <v>2250</v>
+        <v>2248</v>
       </c>
       <c r="C494" s="22" t="s">
-        <v>2251</v>
+        <v>2249</v>
       </c>
       <c r="D494" s="9" t="s">
-        <v>3144</v>
+        <v>3143</v>
       </c>
     </row>
     <row r="495" spans="1:4">
@@ -27539,13 +27551,13 @@
         <v>494</v>
       </c>
       <c r="B495" s="5" t="s">
-        <v>421</v>
-      </c>
-      <c r="C495" s="9" t="s">
-        <v>1121</v>
-      </c>
-      <c r="D495" s="1" t="s">
-        <v>3145</v>
+        <v>2250</v>
+      </c>
+      <c r="C495" s="22" t="s">
+        <v>2251</v>
+      </c>
+      <c r="D495" s="9" t="s">
+        <v>3144</v>
       </c>
     </row>
     <row r="496" spans="1:4">
@@ -27553,13 +27565,13 @@
         <v>495</v>
       </c>
       <c r="B496" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C496" s="9" t="s">
-        <v>1620</v>
+        <v>1121</v>
       </c>
       <c r="D496" s="1" t="s">
-        <v>3146</v>
+        <v>3145</v>
       </c>
     </row>
     <row r="497" spans="1:4">
@@ -27567,13 +27579,13 @@
         <v>496</v>
       </c>
       <c r="B497" s="5" t="s">
-        <v>411</v>
+        <v>422</v>
       </c>
       <c r="C497" s="9" t="s">
-        <v>1122</v>
+        <v>1620</v>
       </c>
       <c r="D497" s="1" t="s">
-        <v>3477</v>
+        <v>3146</v>
       </c>
     </row>
     <row r="498" spans="1:4">
@@ -27581,13 +27593,13 @@
         <v>497</v>
       </c>
       <c r="B498" s="5" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C498" s="9" t="s">
-        <v>3299</v>
+        <v>1122</v>
       </c>
       <c r="D498" s="1" t="s">
-        <v>3300</v>
+        <v>3477</v>
       </c>
     </row>
     <row r="499" spans="1:4">
@@ -27595,13 +27607,13 @@
         <v>498</v>
       </c>
       <c r="B499" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C499" s="9" t="s">
-        <v>1621</v>
+        <v>3299</v>
       </c>
       <c r="D499" s="1" t="s">
-        <v>3148</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="500" spans="1:4">
@@ -27609,13 +27621,13 @@
         <v>499</v>
       </c>
       <c r="B500" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C500" s="9" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="D500" s="1" t="s">
-        <v>3149</v>
+        <v>3148</v>
       </c>
     </row>
     <row r="501" spans="1:4">
@@ -27623,13 +27635,13 @@
         <v>500</v>
       </c>
       <c r="B501" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C501" s="9" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="D501" s="1" t="s">
-        <v>3478</v>
+        <v>3149</v>
       </c>
     </row>
     <row r="502" spans="1:4">
@@ -27637,13 +27649,13 @@
         <v>501</v>
       </c>
       <c r="B502" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C502" s="9" t="s">
-        <v>3301</v>
+        <v>1623</v>
       </c>
       <c r="D502" s="1" t="s">
-        <v>3302</v>
+        <v>3478</v>
       </c>
     </row>
     <row r="503" spans="1:4">
@@ -27651,13 +27663,13 @@
         <v>502</v>
       </c>
       <c r="B503" s="5" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C503" s="9" t="s">
-        <v>3303</v>
+        <v>3301</v>
       </c>
       <c r="D503" s="1" t="s">
-        <v>3306</v>
+        <v>3302</v>
       </c>
     </row>
     <row r="504" spans="1:4">
@@ -27665,13 +27677,13 @@
         <v>503</v>
       </c>
       <c r="B504" s="5" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="C504" s="9" t="s">
-        <v>3304</v>
+        <v>3303</v>
       </c>
       <c r="D504" s="1" t="s">
-        <v>3305</v>
+        <v>3306</v>
       </c>
     </row>
     <row r="505" spans="1:4">
@@ -27679,13 +27691,13 @@
         <v>504</v>
       </c>
       <c r="B505" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C505" s="9" t="s">
-        <v>1624</v>
+        <v>3304</v>
       </c>
       <c r="D505" s="1" t="s">
-        <v>3151</v>
+        <v>3305</v>
       </c>
     </row>
     <row r="506" spans="1:4">
@@ -27693,13 +27705,13 @@
         <v>505</v>
       </c>
       <c r="B506" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C506" s="9" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="D506" s="1" t="s">
-        <v>3152</v>
+        <v>3151</v>
       </c>
     </row>
     <row r="507" spans="1:4">
@@ -27707,13 +27719,13 @@
         <v>506</v>
       </c>
       <c r="B507" s="5" t="s">
-        <v>1053</v>
+        <v>419</v>
       </c>
       <c r="C507" s="9" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="D507" s="1" t="s">
-        <v>3153</v>
+        <v>3152</v>
       </c>
     </row>
     <row r="508" spans="1:4">
@@ -27721,13 +27733,13 @@
         <v>507</v>
       </c>
       <c r="B508" s="5" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="C508" s="9" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="D508" s="1" t="s">
-        <v>3154</v>
+        <v>3153</v>
       </c>
     </row>
     <row r="509" spans="1:4">
@@ -27735,13 +27747,13 @@
         <v>508</v>
       </c>
       <c r="B509" s="5" t="s">
-        <v>423</v>
+        <v>1056</v>
       </c>
       <c r="C509" s="9" t="s">
-        <v>1120</v>
+        <v>1627</v>
       </c>
       <c r="D509" s="1" t="s">
-        <v>423</v>
+        <v>3154</v>
       </c>
     </row>
     <row r="510" spans="1:4">
@@ -27749,13 +27761,13 @@
         <v>509</v>
       </c>
       <c r="B510" s="5" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="C510" s="9" t="s">
-        <v>1628</v>
+        <v>1120</v>
       </c>
       <c r="D510" s="1" t="s">
-        <v>3156</v>
+        <v>423</v>
       </c>
     </row>
     <row r="511" spans="1:4">
@@ -27763,13 +27775,13 @@
         <v>510</v>
       </c>
       <c r="B511" s="5" t="s">
-        <v>1015</v>
+        <v>430</v>
       </c>
       <c r="C511" s="9" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="D511" s="1" t="s">
-        <v>3157</v>
+        <v>3156</v>
       </c>
     </row>
     <row r="512" spans="1:4">
@@ -27777,13 +27789,13 @@
         <v>511</v>
       </c>
       <c r="B512" s="5" t="s">
-        <v>424</v>
+        <v>1015</v>
       </c>
       <c r="C512" s="9" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="D512" s="1" t="s">
-        <v>3158</v>
+        <v>3157</v>
       </c>
     </row>
     <row r="513" spans="1:4">
@@ -27791,13 +27803,13 @@
         <v>512</v>
       </c>
       <c r="B513" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C513" s="9" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="D513" s="1" t="s">
-        <v>3159</v>
+        <v>3158</v>
       </c>
     </row>
     <row r="514" spans="1:4">
@@ -27805,13 +27817,13 @@
         <v>513</v>
       </c>
       <c r="B514" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C514" s="9" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="D514" s="1" t="s">
-        <v>429</v>
+        <v>3159</v>
       </c>
     </row>
     <row r="515" spans="1:4">
@@ -27819,13 +27831,13 @@
         <v>514</v>
       </c>
       <c r="B515" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C515" s="9" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="D515" s="1" t="s">
-        <v>3160</v>
+        <v>429</v>
       </c>
     </row>
     <row r="516" spans="1:4">
@@ -27833,13 +27845,13 @@
         <v>515</v>
       </c>
       <c r="B516" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C516" s="9" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="D516" s="1" t="s">
-        <v>3161</v>
+        <v>3160</v>
       </c>
     </row>
     <row r="517" spans="1:4">
@@ -27847,13 +27859,13 @@
         <v>516</v>
       </c>
       <c r="B517" s="5" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C517" s="9" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="D517" s="1" t="s">
-        <v>3162</v>
+        <v>3161</v>
       </c>
     </row>
     <row r="518" spans="1:4">
@@ -27861,13 +27873,13 @@
         <v>517</v>
       </c>
       <c r="B518" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C518" s="9" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="D518" s="1" t="s">
-        <v>3163</v>
+        <v>3162</v>
       </c>
     </row>
     <row r="519" spans="1:4">
@@ -27875,13 +27887,13 @@
         <v>518</v>
       </c>
       <c r="B519" s="5" t="s">
-        <v>468</v>
+        <v>432</v>
       </c>
       <c r="C519" s="9" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="D519" s="1" t="s">
-        <v>3164</v>
+        <v>3163</v>
       </c>
     </row>
     <row r="520" spans="1:4">
@@ -27889,13 +27901,13 @@
         <v>519</v>
       </c>
       <c r="B520" s="5" t="s">
-        <v>433</v>
+        <v>468</v>
       </c>
       <c r="C520" s="9" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="D520" s="1" t="s">
-        <v>3165</v>
+        <v>3164</v>
       </c>
     </row>
     <row r="521" spans="1:4">
@@ -27903,13 +27915,13 @@
         <v>520</v>
       </c>
       <c r="B521" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C521" s="9" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="D521" s="1" t="s">
-        <v>3166</v>
+        <v>3165</v>
       </c>
     </row>
     <row r="522" spans="1:4">
@@ -27917,13 +27929,13 @@
         <v>521</v>
       </c>
       <c r="B522" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C522" s="9" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="D522" s="1" t="s">
-        <v>3167</v>
+        <v>3166</v>
       </c>
     </row>
     <row r="523" spans="1:4">
@@ -27931,13 +27943,13 @@
         <v>522</v>
       </c>
       <c r="B523" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C523" s="9" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="D523" s="1" t="s">
-        <v>3168</v>
+        <v>3167</v>
       </c>
     </row>
     <row r="524" spans="1:4">
@@ -27945,13 +27957,13 @@
         <v>523</v>
       </c>
       <c r="B524" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C524" s="9" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="D524" s="1" t="s">
-        <v>3169</v>
+        <v>3168</v>
       </c>
     </row>
     <row r="525" spans="1:4">
@@ -27959,13 +27971,13 @@
         <v>524</v>
       </c>
       <c r="B525" s="5" t="s">
-        <v>469</v>
+        <v>437</v>
       </c>
       <c r="C525" s="9" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="D525" s="1" t="s">
-        <v>3170</v>
+        <v>3169</v>
       </c>
     </row>
     <row r="526" spans="1:4">
@@ -27973,13 +27985,13 @@
         <v>525</v>
       </c>
       <c r="B526" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C526" s="9" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="D526" s="1" t="s">
-        <v>3171</v>
+        <v>3170</v>
       </c>
     </row>
     <row r="527" spans="1:4">
@@ -27987,13 +27999,13 @@
         <v>526</v>
       </c>
       <c r="B527" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C527" s="9" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="D527" s="1" t="s">
-        <v>3172</v>
+        <v>3171</v>
       </c>
     </row>
     <row r="528" spans="1:4">
@@ -28001,13 +28013,13 @@
         <v>527</v>
       </c>
       <c r="B528" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C528" s="9" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="D528" s="1" t="s">
-        <v>3173</v>
+        <v>3172</v>
       </c>
     </row>
     <row r="529" spans="1:4">
@@ -28015,13 +28027,13 @@
         <v>528</v>
       </c>
       <c r="B529" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C529" s="9" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="D529" s="1" t="s">
-        <v>3174</v>
+        <v>3173</v>
       </c>
     </row>
     <row r="530" spans="1:4">
@@ -28029,13 +28041,13 @@
         <v>529</v>
       </c>
       <c r="B530" s="5" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C530" s="9" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="D530" s="1" t="s">
-        <v>3175</v>
+        <v>3174</v>
       </c>
     </row>
     <row r="531" spans="1:4">
@@ -28043,13 +28055,13 @@
         <v>530</v>
       </c>
       <c r="B531" s="5" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C531" s="9" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="D531" s="1" t="s">
-        <v>3176</v>
+        <v>3175</v>
       </c>
     </row>
     <row r="532" spans="1:4">
@@ -28057,13 +28069,13 @@
         <v>531</v>
       </c>
       <c r="B532" s="5" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C532" s="9" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="D532" s="1" t="s">
-        <v>3177</v>
+        <v>3176</v>
       </c>
     </row>
     <row r="533" spans="1:4">
@@ -28071,13 +28083,13 @@
         <v>532</v>
       </c>
       <c r="B533" s="5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C533" s="9" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="D533" s="1" t="s">
-        <v>3178</v>
+        <v>3177</v>
       </c>
     </row>
     <row r="534" spans="1:4">
@@ -28085,13 +28097,13 @@
         <v>533</v>
       </c>
       <c r="B534" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C534" s="9" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="D534" s="1" t="s">
-        <v>3179</v>
+        <v>3178</v>
       </c>
     </row>
     <row r="535" spans="1:4">
@@ -28099,13 +28111,13 @@
         <v>534</v>
       </c>
       <c r="B535" s="5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C535" s="9" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="D535" s="1" t="s">
-        <v>3180</v>
+        <v>3179</v>
       </c>
     </row>
     <row r="536" spans="1:4">
@@ -28113,13 +28125,13 @@
         <v>535</v>
       </c>
       <c r="B536" s="5" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C536" s="9" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="D536" s="1" t="s">
-        <v>3181</v>
+        <v>3180</v>
       </c>
     </row>
     <row r="537" spans="1:4">
@@ -28127,13 +28139,13 @@
         <v>536</v>
       </c>
       <c r="B537" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C537" s="9" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="D537" s="1" t="s">
-        <v>3182</v>
+        <v>3181</v>
       </c>
     </row>
     <row r="538" spans="1:4">
@@ -28141,13 +28153,13 @@
         <v>537</v>
       </c>
       <c r="B538" s="5" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C538" s="9" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="D538" s="1" t="s">
-        <v>3183</v>
+        <v>3182</v>
       </c>
     </row>
     <row r="539" spans="1:4">
@@ -28155,13 +28167,13 @@
         <v>538</v>
       </c>
       <c r="B539" s="5" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="C539" s="9" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="D539" s="1" t="s">
-        <v>3184</v>
+        <v>3183</v>
       </c>
     </row>
     <row r="540" spans="1:4">
@@ -28169,13 +28181,13 @@
         <v>539</v>
       </c>
       <c r="B540" s="5" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="C540" s="9" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="D540" s="1" t="s">
-        <v>3185</v>
+        <v>3184</v>
       </c>
     </row>
     <row r="541" spans="1:4">
@@ -28183,13 +28195,13 @@
         <v>540</v>
       </c>
       <c r="B541" s="5" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C541" s="9" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="D541" s="1" t="s">
-        <v>3186</v>
+        <v>3185</v>
       </c>
     </row>
     <row r="542" spans="1:4">
@@ -28197,13 +28209,13 @@
         <v>541</v>
       </c>
       <c r="B542" s="5" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C542" s="9" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="D542" s="1" t="s">
-        <v>3187</v>
+        <v>3186</v>
       </c>
     </row>
     <row r="543" spans="1:4">
@@ -28211,13 +28223,13 @@
         <v>542</v>
       </c>
       <c r="B543" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C543" s="9" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="D543" s="1" t="s">
-        <v>3188</v>
+        <v>3187</v>
       </c>
     </row>
     <row r="544" spans="1:4">
@@ -28225,13 +28237,13 @@
         <v>543</v>
       </c>
       <c r="B544" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C544" s="9" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="D544" s="1" t="s">
-        <v>3189</v>
+        <v>3188</v>
       </c>
     </row>
     <row r="545" spans="1:4">
@@ -28239,13 +28251,13 @@
         <v>544</v>
       </c>
       <c r="B545" s="5" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C545" s="9" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="D545" s="1" t="s">
-        <v>3190</v>
+        <v>3189</v>
       </c>
     </row>
     <row r="546" spans="1:4">
@@ -28253,13 +28265,13 @@
         <v>545</v>
       </c>
       <c r="B546" s="5" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C546" s="9" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="D546" s="1" t="s">
-        <v>3191</v>
+        <v>3190</v>
       </c>
     </row>
     <row r="547" spans="1:4">
@@ -28267,13 +28279,13 @@
         <v>546</v>
       </c>
       <c r="B547" s="5" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C547" s="9" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="D547" s="1" t="s">
-        <v>3192</v>
+        <v>3191</v>
       </c>
     </row>
     <row r="548" spans="1:4">
@@ -28281,13 +28293,13 @@
         <v>547</v>
       </c>
       <c r="B548" s="5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C548" s="9" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="D548" s="1" t="s">
-        <v>3193</v>
+        <v>3192</v>
       </c>
     </row>
     <row r="549" spans="1:4">
@@ -28295,13 +28307,13 @@
         <v>548</v>
       </c>
       <c r="B549" s="5" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C549" s="9" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="D549" s="1" t="s">
-        <v>3194</v>
+        <v>3193</v>
       </c>
     </row>
     <row r="550" spans="1:4">
@@ -28309,13 +28321,13 @@
         <v>549</v>
       </c>
       <c r="B550" s="5" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C550" s="9" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="D550" s="1" t="s">
-        <v>3195</v>
+        <v>3194</v>
       </c>
     </row>
     <row r="551" spans="1:4">
@@ -28323,13 +28335,13 @@
         <v>550</v>
       </c>
       <c r="B551" s="5" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C551" s="9" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="D551" s="1" t="s">
-        <v>3196</v>
+        <v>3195</v>
       </c>
     </row>
     <row r="552" spans="1:4">
@@ -28337,13 +28349,13 @@
         <v>551</v>
       </c>
       <c r="B552" s="5" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C552" s="9" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="D552" s="1" t="s">
-        <v>3197</v>
+        <v>3196</v>
       </c>
     </row>
     <row r="553" spans="1:4">
@@ -28351,13 +28363,13 @@
         <v>552</v>
       </c>
       <c r="B553" s="5" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C553" s="9" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="D553" s="1" t="s">
-        <v>3198</v>
+        <v>3197</v>
       </c>
     </row>
     <row r="554" spans="1:4">
@@ -28365,13 +28377,13 @@
         <v>553</v>
       </c>
       <c r="B554" s="5" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C554" s="9" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="D554" s="1" t="s">
-        <v>3493</v>
+        <v>3198</v>
       </c>
     </row>
     <row r="555" spans="1:4">
@@ -28379,13 +28391,13 @@
         <v>554</v>
       </c>
       <c r="B555" s="5" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C555" s="9" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="D555" s="1" t="s">
-        <v>3199</v>
+        <v>3493</v>
       </c>
     </row>
     <row r="556" spans="1:4">
@@ -28393,13 +28405,13 @@
         <v>555</v>
       </c>
       <c r="B556" s="5" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C556" s="9" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="D556" s="1" t="s">
-        <v>3200</v>
+        <v>3199</v>
       </c>
     </row>
     <row r="557" spans="1:4">
@@ -28407,13 +28419,13 @@
         <v>556</v>
       </c>
       <c r="B557" s="5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C557" s="9" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D557" s="1" t="s">
-        <v>3201</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="558" spans="1:4">
@@ -28421,13 +28433,13 @@
         <v>557</v>
       </c>
       <c r="B558" s="5" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C558" s="9" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="D558" s="1" t="s">
-        <v>3202</v>
+        <v>3201</v>
       </c>
     </row>
     <row r="559" spans="1:4">
@@ -28435,13 +28447,13 @@
         <v>558</v>
       </c>
       <c r="B559" s="5" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C559" s="9" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="D559" s="1" t="s">
-        <v>3203</v>
+        <v>3202</v>
       </c>
     </row>
     <row r="560" spans="1:4">
@@ -28449,13 +28461,13 @@
         <v>559</v>
       </c>
       <c r="B560" s="5" t="s">
-        <v>3625</v>
-      </c>
-      <c r="C560" s="18" t="s">
-        <v>3623</v>
-      </c>
-      <c r="D560" s="9" t="s">
-        <v>3624</v>
+        <v>505</v>
+      </c>
+      <c r="C560" s="9" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D560" s="1" t="s">
+        <v>3203</v>
       </c>
     </row>
     <row r="561" spans="1:4">
@@ -28463,13 +28475,13 @@
         <v>560</v>
       </c>
       <c r="B561" s="5" t="s">
-        <v>506</v>
-      </c>
-      <c r="C561" s="9" t="s">
-        <v>1678</v>
-      </c>
-      <c r="D561" s="1" t="s">
-        <v>3204</v>
+        <v>3625</v>
+      </c>
+      <c r="C561" s="18" t="s">
+        <v>3623</v>
+      </c>
+      <c r="D561" s="9" t="s">
+        <v>3624</v>
       </c>
     </row>
     <row r="562" spans="1:4">
@@ -28477,13 +28489,13 @@
         <v>561</v>
       </c>
       <c r="B562" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C562" s="9" t="s">
-        <v>3307</v>
+        <v>1678</v>
       </c>
       <c r="D562" s="1" t="s">
-        <v>866</v>
+        <v>3204</v>
       </c>
     </row>
     <row r="563" spans="1:4">
@@ -28491,13 +28503,13 @@
         <v>562</v>
       </c>
       <c r="B563" s="5" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C563" s="9" t="s">
-        <v>1680</v>
+        <v>3307</v>
       </c>
       <c r="D563" s="1" t="s">
-        <v>3205</v>
+        <v>866</v>
       </c>
     </row>
     <row r="564" spans="1:4">
@@ -28505,13 +28517,13 @@
         <v>563</v>
       </c>
       <c r="B564" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C564" s="9" t="s">
-        <v>1679</v>
+        <v>1680</v>
       </c>
       <c r="D564" s="1" t="s">
-        <v>3206</v>
+        <v>3205</v>
       </c>
     </row>
     <row r="565" spans="1:4">
@@ -28519,13 +28531,13 @@
         <v>564</v>
       </c>
       <c r="B565" s="5" t="s">
-        <v>548</v>
+        <v>509</v>
       </c>
       <c r="C565" s="9" t="s">
-        <v>1517</v>
+        <v>1679</v>
       </c>
       <c r="D565" s="1" t="s">
-        <v>3020</v>
+        <v>3206</v>
       </c>
     </row>
     <row r="566" spans="1:4">
@@ -28533,13 +28545,13 @@
         <v>565</v>
       </c>
       <c r="B566" s="5" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C566" s="9" t="s">
-        <v>1680</v>
+        <v>1517</v>
       </c>
       <c r="D566" s="1" t="s">
-        <v>3207</v>
+        <v>3020</v>
       </c>
     </row>
     <row r="567" spans="1:4">
@@ -28547,13 +28559,13 @@
         <v>566</v>
       </c>
       <c r="B567" s="5" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C567" s="9" t="s">
-        <v>1518</v>
+        <v>1680</v>
       </c>
       <c r="D567" s="1" t="s">
-        <v>2776</v>
+        <v>3207</v>
       </c>
     </row>
     <row r="568" spans="1:4">
@@ -28561,13 +28573,13 @@
         <v>567</v>
       </c>
       <c r="B568" s="5" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C568" s="9" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="D568" s="1" t="s">
-        <v>2777</v>
+        <v>2776</v>
       </c>
     </row>
     <row r="569" spans="1:4">
@@ -28575,13 +28587,13 @@
         <v>568</v>
       </c>
       <c r="B569" s="5" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C569" s="9" t="s">
-        <v>1681</v>
+        <v>1519</v>
       </c>
       <c r="D569" s="1" t="s">
-        <v>3208</v>
+        <v>2777</v>
       </c>
     </row>
     <row r="570" spans="1:4">
@@ -28589,13 +28601,13 @@
         <v>569</v>
       </c>
       <c r="B570" s="5" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C570" s="9" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="D570" s="1" t="s">
-        <v>3209</v>
+        <v>3208</v>
       </c>
     </row>
     <row r="571" spans="1:4">
@@ -28603,13 +28615,13 @@
         <v>570</v>
       </c>
       <c r="B571" s="5" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C571" s="9" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="D571" s="1" t="s">
-        <v>3210</v>
+        <v>3209</v>
       </c>
     </row>
     <row r="572" spans="1:4">
@@ -28617,13 +28629,13 @@
         <v>571</v>
       </c>
       <c r="B572" s="5" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C572" s="9" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="D572" s="1" t="s">
-        <v>3211</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="573" spans="1:4">
@@ -28631,13 +28643,13 @@
         <v>572</v>
       </c>
       <c r="B573" s="5" t="s">
-        <v>588</v>
+        <v>556</v>
       </c>
       <c r="C573" s="9" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="D573" s="1" t="s">
-        <v>3212</v>
+        <v>3211</v>
       </c>
     </row>
     <row r="574" spans="1:4">
@@ -28645,13 +28657,13 @@
         <v>573</v>
       </c>
       <c r="B574" s="5" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="C574" s="9" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="D574" s="1" t="s">
-        <v>3213</v>
+        <v>3212</v>
       </c>
     </row>
     <row r="575" spans="1:4">
@@ -28659,13 +28671,13 @@
         <v>574</v>
       </c>
       <c r="B575" s="5" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C575" s="9" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
       <c r="D575" s="1" t="s">
-        <v>3214</v>
+        <v>3213</v>
       </c>
     </row>
     <row r="576" spans="1:4">
@@ -28673,13 +28685,13 @@
         <v>575</v>
       </c>
       <c r="B576" s="5" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C576" s="9" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="D576" s="1" t="s">
-        <v>3215</v>
+        <v>3214</v>
       </c>
     </row>
     <row r="577" spans="1:4">
@@ -28687,13 +28699,13 @@
         <v>576</v>
       </c>
       <c r="B577" s="5" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="C577" s="9" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="D577" s="1" t="s">
-        <v>3216</v>
+        <v>3215</v>
       </c>
     </row>
     <row r="578" spans="1:4">
@@ -28701,13 +28713,13 @@
         <v>577</v>
       </c>
       <c r="B578" s="5" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C578" s="9" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="D578" s="1" t="s">
-        <v>3217</v>
+        <v>3216</v>
       </c>
     </row>
     <row r="579" spans="1:4">
@@ -28715,13 +28727,13 @@
         <v>578</v>
       </c>
       <c r="B579" s="5" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C579" s="9" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="D579" s="1" t="s">
-        <v>3218</v>
+        <v>3217</v>
       </c>
     </row>
     <row r="580" spans="1:4">
@@ -28729,13 +28741,13 @@
         <v>579</v>
       </c>
       <c r="B580" s="5" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C580" s="9" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="D580" s="1" t="s">
-        <v>3219</v>
+        <v>3218</v>
       </c>
     </row>
     <row r="581" spans="1:4">
@@ -28743,13 +28755,13 @@
         <v>580</v>
       </c>
       <c r="B581" s="5" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C581" s="9" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="D581" s="1" t="s">
-        <v>3220</v>
+        <v>3219</v>
       </c>
     </row>
     <row r="582" spans="1:4">
@@ -28757,13 +28769,13 @@
         <v>581</v>
       </c>
       <c r="B582" s="5" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C582" s="9" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="D582" s="1" t="s">
-        <v>3221</v>
+        <v>3220</v>
       </c>
     </row>
     <row r="583" spans="1:4">
@@ -28771,13 +28783,13 @@
         <v>582</v>
       </c>
       <c r="B583" s="5" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C583" s="9" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="D583" s="1" t="s">
-        <v>3222</v>
+        <v>3221</v>
       </c>
     </row>
     <row r="584" spans="1:4">
@@ -28785,13 +28797,13 @@
         <v>583</v>
       </c>
       <c r="B584" s="5" t="s">
-        <v>680</v>
+        <v>595</v>
       </c>
       <c r="C584" s="9" t="s">
-        <v>1697</v>
+        <v>1695</v>
       </c>
       <c r="D584" s="1" t="s">
-        <v>3410</v>
+        <v>3222</v>
       </c>
     </row>
     <row r="585" spans="1:4">
@@ -28799,13 +28811,13 @@
         <v>584</v>
       </c>
       <c r="B585" s="5" t="s">
-        <v>935</v>
+        <v>680</v>
       </c>
       <c r="C585" s="9" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="D585" s="1" t="s">
-        <v>3224</v>
+        <v>3410</v>
       </c>
     </row>
     <row r="586" spans="1:4">
@@ -28813,13 +28825,13 @@
         <v>585</v>
       </c>
       <c r="B586" s="5" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="C586" s="9" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="D586" s="1" t="s">
-        <v>3225</v>
+        <v>3224</v>
       </c>
     </row>
     <row r="587" spans="1:4">
@@ -28827,13 +28839,13 @@
         <v>586</v>
       </c>
       <c r="B587" s="5" t="s">
-        <v>756</v>
-      </c>
-      <c r="C587" s="13" t="s">
-        <v>3406</v>
-      </c>
-      <c r="D587" s="4" t="s">
-        <v>3408</v>
+        <v>934</v>
+      </c>
+      <c r="C587" s="9" t="s">
+        <v>1699</v>
+      </c>
+      <c r="D587" s="1" t="s">
+        <v>3225</v>
       </c>
     </row>
     <row r="588" spans="1:4">
@@ -28841,13 +28853,13 @@
         <v>587</v>
       </c>
       <c r="B588" s="5" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="C588" s="13" t="s">
-        <v>3405</v>
+        <v>3406</v>
       </c>
       <c r="D588" s="4" t="s">
-        <v>3407</v>
+        <v>3408</v>
       </c>
     </row>
     <row r="589" spans="1:4">
@@ -28855,13 +28867,13 @@
         <v>588</v>
       </c>
       <c r="B589" s="5" t="s">
-        <v>880</v>
-      </c>
-      <c r="C589" s="9" t="s">
-        <v>1700</v>
-      </c>
-      <c r="D589" s="1" t="s">
-        <v>3226</v>
+        <v>757</v>
+      </c>
+      <c r="C589" s="13" t="s">
+        <v>3405</v>
+      </c>
+      <c r="D589" s="4" t="s">
+        <v>3407</v>
       </c>
     </row>
     <row r="590" spans="1:4">
@@ -28869,13 +28881,13 @@
         <v>589</v>
       </c>
       <c r="B590" s="5" t="s">
-        <v>876</v>
+        <v>880</v>
       </c>
       <c r="C590" s="9" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="D590" s="1" t="s">
-        <v>3227</v>
+        <v>3226</v>
       </c>
     </row>
     <row r="591" spans="1:4">
@@ -28883,13 +28895,13 @@
         <v>590</v>
       </c>
       <c r="B591" s="5" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="C591" s="9" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="D591" s="1" t="s">
-        <v>3228</v>
+        <v>3227</v>
       </c>
     </row>
     <row r="592" spans="1:4">
@@ -28897,13 +28909,13 @@
         <v>591</v>
       </c>
       <c r="B592" s="5" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C592" s="9" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="D592" s="1" t="s">
-        <v>3229</v>
+        <v>3228</v>
       </c>
     </row>
     <row r="593" spans="1:4">
@@ -28911,13 +28923,13 @@
         <v>592</v>
       </c>
       <c r="B593" s="5" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="C593" s="9" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="D593" s="1" t="s">
-        <v>3230</v>
+        <v>3229</v>
       </c>
     </row>
     <row r="594" spans="1:4">
@@ -28925,13 +28937,13 @@
         <v>593</v>
       </c>
       <c r="B594" s="5" t="s">
-        <v>901</v>
+        <v>879</v>
       </c>
       <c r="C594" s="9" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="D594" s="1" t="s">
-        <v>3231</v>
+        <v>3230</v>
       </c>
     </row>
     <row r="595" spans="1:4">
@@ -28939,13 +28951,13 @@
         <v>594</v>
       </c>
       <c r="B595" s="5" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="C595" s="9" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="D595" s="1" t="s">
-        <v>3232</v>
+        <v>3231</v>
       </c>
     </row>
     <row r="596" spans="1:4">
@@ -28953,13 +28965,13 @@
         <v>595</v>
       </c>
       <c r="B596" s="5" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="C596" s="9" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="D596" s="1" t="s">
-        <v>3233</v>
+        <v>3232</v>
       </c>
     </row>
     <row r="597" spans="1:4">
@@ -28967,13 +28979,13 @@
         <v>596</v>
       </c>
       <c r="B597" s="5" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="C597" s="9" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="D597" s="1" t="s">
-        <v>3234</v>
+        <v>3233</v>
       </c>
     </row>
     <row r="598" spans="1:4">
@@ -28981,13 +28993,13 @@
         <v>597</v>
       </c>
       <c r="B598" s="5" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="C598" s="9" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="D598" s="1" t="s">
-        <v>3235</v>
+        <v>3234</v>
       </c>
     </row>
     <row r="599" spans="1:4">
@@ -28995,13 +29007,13 @@
         <v>598</v>
       </c>
       <c r="B599" s="5" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="C599" s="9" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="D599" s="1" t="s">
-        <v>3236</v>
+        <v>3235</v>
       </c>
     </row>
     <row r="600" spans="1:4">
@@ -29009,13 +29021,13 @@
         <v>599</v>
       </c>
       <c r="B600" s="5" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="C600" s="9" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="D600" s="1" t="s">
-        <v>3237</v>
+        <v>3236</v>
       </c>
     </row>
     <row r="601" spans="1:4">
@@ -29023,13 +29035,13 @@
         <v>600</v>
       </c>
       <c r="B601" s="5" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="C601" s="9" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="D601" s="1" t="s">
-        <v>3238</v>
+        <v>3237</v>
       </c>
     </row>
     <row r="602" spans="1:4">
@@ -29037,13 +29049,13 @@
         <v>601</v>
       </c>
       <c r="B602" s="5" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="C602" s="9" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="D602" s="1" t="s">
-        <v>3239</v>
+        <v>3238</v>
       </c>
     </row>
     <row r="603" spans="1:4">
@@ -29051,13 +29063,13 @@
         <v>602</v>
       </c>
       <c r="B603" s="5" t="s">
-        <v>918</v>
+        <v>909</v>
       </c>
       <c r="C603" s="9" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="D603" s="1" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="604" spans="1:4">
@@ -29065,13 +29077,13 @@
         <v>603</v>
       </c>
       <c r="B604" s="5" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="C604" s="9" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="D604" s="1" t="s">
-        <v>3241</v>
+        <v>3240</v>
       </c>
     </row>
     <row r="605" spans="1:4">
@@ -29079,13 +29091,13 @@
         <v>604</v>
       </c>
       <c r="B605" s="5" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="C605" s="9" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="D605" s="1" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="606" spans="1:4">
@@ -29093,13 +29105,13 @@
         <v>605</v>
       </c>
       <c r="B606" s="5" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="C606" s="9" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="D606" s="1" t="s">
-        <v>3243</v>
+        <v>3242</v>
       </c>
     </row>
     <row r="607" spans="1:4">
@@ -29107,13 +29119,13 @@
         <v>606</v>
       </c>
       <c r="B607" s="5" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C607" s="9" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="D607" s="1" t="s">
-        <v>3244</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="608" spans="1:4">
@@ -29121,13 +29133,13 @@
         <v>607</v>
       </c>
       <c r="B608" s="5" t="s">
-        <v>910</v>
+        <v>922</v>
       </c>
       <c r="C608" s="9" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="D608" s="1" t="s">
-        <v>3245</v>
+        <v>3244</v>
       </c>
     </row>
     <row r="609" spans="1:4">
@@ -29135,13 +29147,13 @@
         <v>608</v>
       </c>
       <c r="B609" s="5" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C609" s="9" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="D609" s="1" t="s">
-        <v>3246</v>
+        <v>3245</v>
       </c>
     </row>
     <row r="610" spans="1:4">
@@ -29149,13 +29161,13 @@
         <v>609</v>
       </c>
       <c r="B610" s="5" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="C610" s="9" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="D610" s="1" t="s">
-        <v>3247</v>
+        <v>3246</v>
       </c>
     </row>
     <row r="611" spans="1:4">
@@ -29163,13 +29175,13 @@
         <v>610</v>
       </c>
       <c r="B611" s="5" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C611" s="9" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="D611" s="1" t="s">
-        <v>3248</v>
+        <v>3247</v>
       </c>
     </row>
     <row r="612" spans="1:4">
@@ -29177,13 +29189,13 @@
         <v>611</v>
       </c>
       <c r="B612" s="5" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C612" s="9" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="D612" s="1" t="s">
-        <v>3249</v>
+        <v>3248</v>
       </c>
     </row>
     <row r="613" spans="1:4">
@@ -29191,13 +29203,13 @@
         <v>612</v>
       </c>
       <c r="B613" s="5" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C613" s="9" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="D613" s="1" t="s">
-        <v>3250</v>
+        <v>3249</v>
       </c>
     </row>
     <row r="614" spans="1:4">
@@ -29205,13 +29217,13 @@
         <v>613</v>
       </c>
       <c r="B614" s="5" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="C614" s="9" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="D614" s="1" t="s">
-        <v>3251</v>
+        <v>3250</v>
       </c>
     </row>
     <row r="615" spans="1:4">
@@ -29219,27 +29231,27 @@
         <v>614</v>
       </c>
       <c r="B615" s="5" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="C615" s="9" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="D615" s="1" t="s">
-        <v>3252</v>
+        <v>3251</v>
       </c>
     </row>
     <row r="616" spans="1:4">
       <c r="A616" s="15">
         <v>615</v>
       </c>
-      <c r="B616" s="6" t="s">
-        <v>930</v>
-      </c>
-      <c r="C616" s="13" t="s">
-        <v>1727</v>
-      </c>
-      <c r="D616" s="4" t="s">
-        <v>3253</v>
+      <c r="B616" s="5" t="s">
+        <v>917</v>
+      </c>
+      <c r="C616" s="9" t="s">
+        <v>1726</v>
+      </c>
+      <c r="D616" s="1" t="s">
+        <v>3252</v>
       </c>
     </row>
     <row r="617" spans="1:4">
@@ -29247,13 +29259,13 @@
         <v>616</v>
       </c>
       <c r="B617" s="6" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="C617" s="13" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="D617" s="4" t="s">
-        <v>3254</v>
+        <v>3253</v>
       </c>
     </row>
     <row r="618" spans="1:4">
@@ -29261,27 +29273,27 @@
         <v>617</v>
       </c>
       <c r="B618" s="6" t="s">
-        <v>932</v>
-      </c>
-      <c r="C618" s="9" t="s">
-        <v>1729</v>
-      </c>
-      <c r="D618" s="1" t="s">
-        <v>3255</v>
+        <v>931</v>
+      </c>
+      <c r="C618" s="13" t="s">
+        <v>1728</v>
+      </c>
+      <c r="D618" s="4" t="s">
+        <v>3254</v>
       </c>
     </row>
     <row r="619" spans="1:4">
       <c r="A619" s="15">
         <v>618</v>
       </c>
-      <c r="B619" s="5" t="s">
-        <v>933</v>
+      <c r="B619" s="6" t="s">
+        <v>932</v>
       </c>
       <c r="C619" s="9" t="s">
-        <v>3308</v>
+        <v>1729</v>
       </c>
       <c r="D619" s="1" t="s">
-        <v>3309</v>
+        <v>3255</v>
       </c>
     </row>
     <row r="620" spans="1:4">
@@ -29289,13 +29301,13 @@
         <v>619</v>
       </c>
       <c r="B620" s="5" t="s">
-        <v>1092</v>
+        <v>933</v>
       </c>
       <c r="C620" s="9" t="s">
-        <v>1730</v>
+        <v>3308</v>
       </c>
       <c r="D620" s="1" t="s">
-        <v>3256</v>
+        <v>3309</v>
       </c>
     </row>
     <row r="621" spans="1:4">
@@ -29303,13 +29315,13 @@
         <v>620</v>
       </c>
       <c r="B621" s="5" t="s">
-        <v>1095</v>
+        <v>1092</v>
       </c>
       <c r="C621" s="9" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="D621" s="1" t="s">
-        <v>3257</v>
+        <v>3256</v>
       </c>
     </row>
     <row r="622" spans="1:4">
@@ -29317,13 +29329,13 @@
         <v>621</v>
       </c>
       <c r="B622" s="5" t="s">
-        <v>1093</v>
+        <v>1095</v>
       </c>
       <c r="C622" s="9" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="D622" s="1" t="s">
-        <v>3258</v>
+        <v>3257</v>
       </c>
     </row>
     <row r="623" spans="1:4">
@@ -29331,13 +29343,13 @@
         <v>622</v>
       </c>
       <c r="B623" s="5" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="C623" s="9" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="D623" s="1" t="s">
-        <v>3259</v>
+        <v>3258</v>
       </c>
     </row>
     <row r="624" spans="1:4">
@@ -29345,13 +29357,13 @@
         <v>623</v>
       </c>
       <c r="B624" s="5" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
       <c r="C624" s="9" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="D624" s="1" t="s">
-        <v>3260</v>
+        <v>3259</v>
       </c>
     </row>
     <row r="625" spans="1:4">
@@ -29359,13 +29371,13 @@
         <v>624</v>
       </c>
       <c r="B625" s="5" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="C625" s="9" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="D625" s="1" t="s">
-        <v>3261</v>
+        <v>3260</v>
       </c>
     </row>
     <row r="626" spans="1:4">
@@ -29373,13 +29385,13 @@
         <v>625</v>
       </c>
       <c r="B626" s="5" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="C626" s="9" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="D626" s="1" t="s">
-        <v>3262</v>
+        <v>3261</v>
       </c>
     </row>
     <row r="627" spans="1:4">
@@ -29387,13 +29399,13 @@
         <v>626</v>
       </c>
       <c r="B627" s="5" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="C627" s="9" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="D627" s="1" t="s">
-        <v>3263</v>
+        <v>3262</v>
       </c>
     </row>
     <row r="628" spans="1:4">
@@ -29401,13 +29413,13 @@
         <v>627</v>
       </c>
       <c r="B628" s="5" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="C628" s="9" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="D628" s="1" t="s">
-        <v>3264</v>
+        <v>3263</v>
       </c>
     </row>
     <row r="629" spans="1:4">
@@ -29415,13 +29427,13 @@
         <v>628</v>
       </c>
       <c r="B629" s="5" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="C629" s="9" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="D629" s="1" t="s">
-        <v>3265</v>
+        <v>3264</v>
       </c>
     </row>
     <row r="630" spans="1:4">
@@ -29429,13 +29441,13 @@
         <v>629</v>
       </c>
       <c r="B630" s="5" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="C630" s="9" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="D630" s="1" t="s">
-        <v>3266</v>
+        <v>3265</v>
       </c>
     </row>
     <row r="631" spans="1:4">
@@ -29443,41 +29455,41 @@
         <v>630</v>
       </c>
       <c r="B631" s="5" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="C631" s="9" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="D631" s="1" t="s">
-        <v>3267</v>
-      </c>
-    </row>
-    <row r="632" spans="1:4" ht="15">
+        <v>3266</v>
+      </c>
+    </row>
+    <row r="632" spans="1:4">
       <c r="A632" s="15">
         <v>631</v>
       </c>
-      <c r="B632" s="24" t="s">
-        <v>3564</v>
-      </c>
-      <c r="C632" s="18" t="s">
-        <v>3528</v>
-      </c>
-      <c r="D632" s="24" t="s">
-        <v>3529</v>
-      </c>
-    </row>
-    <row r="633" spans="1:4">
+      <c r="B632" s="5" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C632" s="9" t="s">
+        <v>1741</v>
+      </c>
+      <c r="D632" s="1" t="s">
+        <v>3267</v>
+      </c>
+    </row>
+    <row r="633" spans="1:4" ht="15">
       <c r="A633" s="15">
         <v>632</v>
       </c>
-      <c r="B633" s="1" t="s">
-        <v>3565</v>
-      </c>
-      <c r="C633" s="9" t="s">
-        <v>3530</v>
-      </c>
-      <c r="D633" s="1" t="s">
-        <v>3531</v>
+      <c r="B633" s="24" t="s">
+        <v>3564</v>
+      </c>
+      <c r="C633" s="18" t="s">
+        <v>3528</v>
+      </c>
+      <c r="D633" s="24" t="s">
+        <v>3529</v>
       </c>
     </row>
     <row r="634" spans="1:4">
@@ -29485,13 +29497,13 @@
         <v>633</v>
       </c>
       <c r="B634" s="1" t="s">
-        <v>3535</v>
+        <v>3565</v>
       </c>
       <c r="C634" s="9" t="s">
-        <v>3532</v>
+        <v>3530</v>
       </c>
       <c r="D634" s="1" t="s">
-        <v>3535</v>
+        <v>3531</v>
       </c>
     </row>
     <row r="635" spans="1:4">
@@ -29499,13 +29511,13 @@
         <v>634</v>
       </c>
       <c r="B635" s="1" t="s">
-        <v>3534</v>
+        <v>3535</v>
       </c>
       <c r="C635" s="9" t="s">
-        <v>3533</v>
+        <v>3532</v>
       </c>
       <c r="D635" s="1" t="s">
-        <v>3534</v>
+        <v>3535</v>
       </c>
     </row>
     <row r="636" spans="1:4">
@@ -29513,13 +29525,13 @@
         <v>635</v>
       </c>
       <c r="B636" s="1" t="s">
-        <v>3539</v>
-      </c>
-      <c r="C636" s="1" t="s">
-        <v>3536</v>
+        <v>3534</v>
+      </c>
+      <c r="C636" s="9" t="s">
+        <v>3533</v>
       </c>
       <c r="D636" s="1" t="s">
-        <v>3539</v>
+        <v>3534</v>
       </c>
     </row>
     <row r="637" spans="1:4">
@@ -29527,13 +29539,13 @@
         <v>636</v>
       </c>
       <c r="B637" s="1" t="s">
-        <v>3540</v>
+        <v>3539</v>
       </c>
       <c r="C637" s="1" t="s">
-        <v>3537</v>
+        <v>3536</v>
       </c>
       <c r="D637" s="1" t="s">
-        <v>3540</v>
+        <v>3539</v>
       </c>
     </row>
     <row r="638" spans="1:4">
@@ -29541,13 +29553,13 @@
         <v>637</v>
       </c>
       <c r="B638" s="1" t="s">
-        <v>3541</v>
+        <v>3540</v>
       </c>
       <c r="C638" s="1" t="s">
-        <v>3538</v>
+        <v>3537</v>
       </c>
       <c r="D638" s="1" t="s">
-        <v>3541</v>
+        <v>3540</v>
       </c>
     </row>
     <row r="639" spans="1:4">
@@ -29555,13 +29567,13 @@
         <v>638</v>
       </c>
       <c r="B639" s="1" t="s">
-        <v>3563</v>
+        <v>3541</v>
       </c>
       <c r="C639" s="1" t="s">
-        <v>3562</v>
+        <v>3538</v>
       </c>
       <c r="D639" s="1" t="s">
-        <v>3563</v>
+        <v>3541</v>
       </c>
     </row>
     <row r="640" spans="1:4">
@@ -29569,13 +29581,13 @@
         <v>639</v>
       </c>
       <c r="B640" s="1" t="s">
-        <v>3566</v>
+        <v>3563</v>
       </c>
       <c r="C640" s="1" t="s">
-        <v>3544</v>
+        <v>3562</v>
       </c>
       <c r="D640" s="1" t="s">
-        <v>3545</v>
+        <v>3563</v>
       </c>
     </row>
     <row r="641" spans="1:4">
@@ -29583,13 +29595,13 @@
         <v>640</v>
       </c>
       <c r="B641" s="1" t="s">
-        <v>3567</v>
+        <v>3566</v>
       </c>
       <c r="C641" s="1" t="s">
-        <v>3546</v>
+        <v>3544</v>
       </c>
       <c r="D641" s="1" t="s">
-        <v>3547</v>
+        <v>3545</v>
       </c>
     </row>
     <row r="642" spans="1:4">
@@ -29597,13 +29609,13 @@
         <v>641</v>
       </c>
       <c r="B642" s="1" t="s">
-        <v>3568</v>
+        <v>3567</v>
       </c>
       <c r="C642" s="1" t="s">
-        <v>3548</v>
+        <v>3546</v>
       </c>
       <c r="D642" s="1" t="s">
-        <v>3549</v>
+        <v>3547</v>
       </c>
     </row>
     <row r="643" spans="1:4">
@@ -29611,13 +29623,13 @@
         <v>642</v>
       </c>
       <c r="B643" s="1" t="s">
-        <v>3569</v>
+        <v>3568</v>
       </c>
       <c r="C643" s="1" t="s">
-        <v>3550</v>
+        <v>3548</v>
       </c>
       <c r="D643" s="1" t="s">
-        <v>3551</v>
+        <v>3549</v>
       </c>
     </row>
     <row r="644" spans="1:4">
@@ -29625,13 +29637,13 @@
         <v>643</v>
       </c>
       <c r="B644" s="1" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C644" s="18" t="s">
-        <v>3552</v>
+        <v>3569</v>
+      </c>
+      <c r="C644" s="1" t="s">
+        <v>3550</v>
       </c>
       <c r="D644" s="1" t="s">
-        <v>3553</v>
+        <v>3551</v>
       </c>
     </row>
     <row r="645" spans="1:4">
@@ -29639,13 +29651,13 @@
         <v>644</v>
       </c>
       <c r="B645" s="1" t="s">
-        <v>3570</v>
-      </c>
-      <c r="C645" s="1" t="s">
-        <v>3554</v>
+        <v>3553</v>
+      </c>
+      <c r="C645" s="18" t="s">
+        <v>3552</v>
       </c>
       <c r="D645" s="1" t="s">
-        <v>3555</v>
+        <v>3553</v>
       </c>
     </row>
     <row r="646" spans="1:4">
@@ -29653,13 +29665,13 @@
         <v>645</v>
       </c>
       <c r="B646" s="1" t="s">
-        <v>3571</v>
+        <v>3570</v>
       </c>
       <c r="C646" s="1" t="s">
-        <v>3556</v>
+        <v>3554</v>
       </c>
       <c r="D646" s="1" t="s">
-        <v>3557</v>
+        <v>3555</v>
       </c>
     </row>
     <row r="647" spans="1:4">
@@ -29667,13 +29679,13 @@
         <v>646</v>
       </c>
       <c r="B647" s="1" t="s">
-        <v>3572</v>
+        <v>3571</v>
       </c>
       <c r="C647" s="1" t="s">
-        <v>3558</v>
+        <v>3556</v>
       </c>
       <c r="D647" s="1" t="s">
-        <v>3559</v>
+        <v>3557</v>
       </c>
     </row>
     <row r="648" spans="1:4">
@@ -29681,27 +29693,27 @@
         <v>647</v>
       </c>
       <c r="B648" s="1" t="s">
-        <v>3573</v>
+        <v>3572</v>
       </c>
       <c r="C648" s="1" t="s">
-        <v>3560</v>
+        <v>3558</v>
       </c>
       <c r="D648" s="1" t="s">
-        <v>3561</v>
+        <v>3559</v>
       </c>
     </row>
     <row r="649" spans="1:4">
       <c r="A649" s="15">
         <v>648</v>
       </c>
-      <c r="B649" s="5" t="s">
-        <v>3578</v>
-      </c>
-      <c r="C649" s="18" t="s">
-        <v>3579</v>
-      </c>
-      <c r="D649" s="9" t="s">
-        <v>480</v>
+      <c r="B649" s="1" t="s">
+        <v>3573</v>
+      </c>
+      <c r="C649" s="1" t="s">
+        <v>3560</v>
+      </c>
+      <c r="D649" s="1" t="s">
+        <v>3561</v>
       </c>
     </row>
     <row r="650" spans="1:4">
@@ -29709,13 +29721,13 @@
         <v>649</v>
       </c>
       <c r="B650" s="5" t="s">
-        <v>3580</v>
+        <v>3578</v>
       </c>
       <c r="C650" s="18" t="s">
-        <v>3581</v>
+        <v>3579</v>
       </c>
       <c r="D650" s="9" t="s">
-        <v>3582</v>
+        <v>480</v>
       </c>
     </row>
     <row r="651" spans="1:4">
@@ -29723,12 +29735,26 @@
         <v>650</v>
       </c>
       <c r="B651" s="5" t="s">
+        <v>3580</v>
+      </c>
+      <c r="C651" s="18" t="s">
+        <v>3581</v>
+      </c>
+      <c r="D651" s="9" t="s">
+        <v>3582</v>
+      </c>
+    </row>
+    <row r="652" spans="1:4">
+      <c r="A652" s="15">
+        <v>651</v>
+      </c>
+      <c r="B652" s="5" t="s">
         <v>3586</v>
       </c>
-      <c r="C651" s="18" t="s">
+      <c r="C652" s="18" t="s">
         <v>3587</v>
       </c>
-      <c r="D651" s="9" t="s">
+      <c r="D652" s="9" t="s">
         <v>3588</v>
       </c>
     </row>

</xml_diff>

<commit_message>
The protocol configuration adds extended fields.
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnpc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnpc/locale/locale-en.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7518B970-27BE-4418-8C2D-891816A825D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB019847-57AD-4632-9FE1-6B52EF8D65C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3973" uniqueCount="3756">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3988" uniqueCount="3769">
   <si>
     <t>myself</t>
   </si>
@@ -13206,14 +13206,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>油气生产智能监控系统 V9.6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>《油气生产智能监控系统 V9.6》主要在采集、控制的基础上，侧重油井智能分析。模块主要包括实时监控、历史查询、生产报表、故障查询、日志查询、计算维护、驱动配置、权限管理、设备管理、系统配置等。系统应用大数据分析方法，对工况、产量、液面、平衡、能耗等生产关键指标进行统计分析，及时发现生产不正常井，挖掘生产潜力井，提升对目标区块和单井的管控能力。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Intelligent monitoring system V9.6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -14180,6 +14172,62 @@
   </si>
   <si>
     <t>Dynamometer construction data-ground efficiency</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>智能监控系统 V9.6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>《智能监控系统 V9.6》主要在采集、控制的基础上，侧重油井智能分析。模块主要包括实时监控、历史查询、生产报表、故障查询、日志查询、计算维护、驱动配置、权限管理、设备管理、系统配置等。系统应用大数据分析方法，对工况、产量、液面、平衡、能耗等生产关键指标进行统计分析，及时发现生产不正常井，挖掘生产潜力井，提升对目标区块和单井的管控能力。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拓展字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Extended fields</t>
+  </si>
+  <si>
+    <t>Extended fields</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>extendedField</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FOUROPERATION</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>加法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>减法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>乘法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>除法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>subtraction</t>
+  </si>
+  <si>
+    <t>multiplication</t>
+  </si>
+  <si>
+    <t>division</t>
+  </si>
+  <si>
+    <t>addition</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -16390,7 +16438,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -16423,10 +16471,10 @@
         <v>15</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>3754</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>3509</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3511</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -16437,10 +16485,10 @@
         <v>16</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>3755</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>3510</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3512</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -16610,7 +16658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D370"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -17566,13 +17614,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>3672</v>
+        <v>3670</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>3667</v>
+        <v>3665</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>3677</v>
+        <v>3675</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -17580,13 +17628,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>3673</v>
+        <v>3671</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>3668</v>
+        <v>3666</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>3678</v>
+        <v>3676</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -17594,13 +17642,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>3674</v>
+        <v>3672</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>3669</v>
+        <v>3667</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>3679</v>
+        <v>3677</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -17608,13 +17656,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>3675</v>
+        <v>3673</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>3670</v>
+        <v>3668</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>3680</v>
+        <v>3678</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -17622,13 +17670,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>3676</v>
+        <v>3674</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>3671</v>
+        <v>3669</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>3681</v>
+        <v>3679</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -19518,7 +19566,7 @@
         <v>1281</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>3516</v>
+        <v>3514</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -19532,7 +19580,7 @@
         <v>1282</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>3517</v>
+        <v>3515</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -19546,7 +19594,7 @@
         <v>1283</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>3518</v>
+        <v>3516</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -19560,7 +19608,7 @@
         <v>1284</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>3519</v>
+        <v>3517</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -19574,7 +19622,7 @@
         <v>1285</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>3520</v>
+        <v>3518</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -19588,7 +19636,7 @@
         <v>1286</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>3521</v>
+        <v>3519</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -19602,7 +19650,7 @@
         <v>1287</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>3522</v>
+        <v>3520</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -19616,7 +19664,7 @@
         <v>1288</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>3523</v>
+        <v>3521</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -19644,7 +19692,7 @@
         <v>1289</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>3524</v>
+        <v>3522</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -19658,7 +19706,7 @@
         <v>1290</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>3525</v>
+        <v>3523</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -19756,7 +19804,7 @@
         <v>1846</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>3526</v>
+        <v>3524</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -19770,7 +19818,7 @@
         <v>1847</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>3527</v>
+        <v>3525</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -19798,7 +19846,7 @@
         <v>1849</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>3528</v>
+        <v>3526</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -19806,13 +19854,13 @@
         <v>227</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>3534</v>
+        <v>3532</v>
       </c>
       <c r="C228" s="9" t="s">
-        <v>3529</v>
+        <v>3527</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>3532</v>
+        <v>3530</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -19820,13 +19868,13 @@
         <v>228</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>3535</v>
+        <v>3533</v>
       </c>
       <c r="C229" s="9" t="s">
-        <v>3530</v>
+        <v>3528</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>3571</v>
+        <v>3569</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -19834,13 +19882,13 @@
         <v>229</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>3533</v>
+        <v>3531</v>
       </c>
       <c r="C230" s="9" t="s">
-        <v>3627</v>
+        <v>3625</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>3628</v>
+        <v>3626</v>
       </c>
     </row>
     <row r="231" spans="1:4">
@@ -19848,13 +19896,13 @@
         <v>230</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>3536</v>
+        <v>3534</v>
       </c>
       <c r="C231" s="9" t="s">
-        <v>3627</v>
+        <v>3625</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>3628</v>
+        <v>3626</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -19862,13 +19910,13 @@
         <v>231</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>3537</v>
+        <v>3535</v>
       </c>
       <c r="C232" s="9" t="s">
-        <v>3531</v>
+        <v>3529</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>3572</v>
+        <v>3570</v>
       </c>
     </row>
     <row r="233" spans="1:4" ht="15" customHeight="1">
@@ -19876,13 +19924,13 @@
         <v>232</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>3538</v>
+        <v>3536</v>
       </c>
       <c r="C233" s="9" t="s">
-        <v>3569</v>
+        <v>3567</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>3573</v>
+        <v>3571</v>
       </c>
     </row>
     <row r="234" spans="1:4">
@@ -19890,13 +19938,13 @@
         <v>233</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>3540</v>
+        <v>3538</v>
       </c>
       <c r="C234" s="9" t="s">
-        <v>3574</v>
+        <v>3572</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>3575</v>
+        <v>3573</v>
       </c>
     </row>
     <row r="235" spans="1:4">
@@ -19904,13 +19952,13 @@
         <v>234</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>3539</v>
+        <v>3537</v>
       </c>
       <c r="C235" s="9" t="s">
-        <v>3576</v>
+        <v>3574</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>3577</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="236" spans="1:4">
@@ -19918,13 +19966,13 @@
         <v>235</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>3541</v>
+        <v>3539</v>
       </c>
       <c r="C236" s="9" t="s">
-        <v>3578</v>
+        <v>3576</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>3579</v>
+        <v>3577</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -19932,13 +19980,13 @@
         <v>236</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>3542</v>
+        <v>3540</v>
       </c>
       <c r="C237" s="9" t="s">
-        <v>3580</v>
+        <v>3578</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>3581</v>
+        <v>3579</v>
       </c>
     </row>
     <row r="238" spans="1:4">
@@ -19946,13 +19994,13 @@
         <v>237</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>3543</v>
+        <v>3541</v>
       </c>
       <c r="C238" s="9" t="s">
-        <v>3582</v>
+        <v>3580</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>3583</v>
+        <v>3581</v>
       </c>
     </row>
     <row r="239" spans="1:4">
@@ -19960,13 +20008,13 @@
         <v>238</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>3544</v>
+        <v>3542</v>
       </c>
       <c r="C239" s="9" t="s">
-        <v>3584</v>
+        <v>3582</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>3585</v>
+        <v>3583</v>
       </c>
     </row>
     <row r="240" spans="1:4">
@@ -19974,13 +20022,13 @@
         <v>239</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>3545</v>
+        <v>3543</v>
       </c>
       <c r="C240" s="9" t="s">
-        <v>3586</v>
+        <v>3584</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>3587</v>
+        <v>3585</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -19988,13 +20036,13 @@
         <v>240</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>3546</v>
+        <v>3544</v>
       </c>
       <c r="C241" s="9" t="s">
-        <v>3588</v>
+        <v>3586</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>3589</v>
+        <v>3587</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -20002,13 +20050,13 @@
         <v>241</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>3547</v>
+        <v>3545</v>
       </c>
       <c r="C242" s="9" t="s">
-        <v>3570</v>
+        <v>3568</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>3590</v>
+        <v>3588</v>
       </c>
     </row>
     <row r="243" spans="1:4">
@@ -20016,13 +20064,13 @@
         <v>242</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>3548</v>
+        <v>3546</v>
       </c>
       <c r="C243" s="9" t="s">
-        <v>3591</v>
+        <v>3589</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>3592</v>
+        <v>3590</v>
       </c>
     </row>
     <row r="244" spans="1:4">
@@ -20030,13 +20078,13 @@
         <v>243</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>3549</v>
+        <v>3547</v>
       </c>
       <c r="C244" s="9" t="s">
-        <v>3593</v>
+        <v>3591</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>3594</v>
+        <v>3592</v>
       </c>
     </row>
     <row r="245" spans="1:4">
@@ -20044,13 +20092,13 @@
         <v>244</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>3550</v>
+        <v>3548</v>
       </c>
       <c r="C245" s="9" t="s">
-        <v>3551</v>
+        <v>3549</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>3595</v>
+        <v>3593</v>
       </c>
     </row>
     <row r="246" spans="1:4">
@@ -20058,13 +20106,13 @@
         <v>245</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>3552</v>
+        <v>3550</v>
       </c>
       <c r="C246" s="9" t="s">
-        <v>3596</v>
+        <v>3594</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>3597</v>
+        <v>3595</v>
       </c>
     </row>
     <row r="247" spans="1:4">
@@ -20072,13 +20120,13 @@
         <v>246</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>3553</v>
+        <v>3551</v>
       </c>
       <c r="C247" s="9" t="s">
-        <v>3598</v>
+        <v>3596</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>3599</v>
+        <v>3597</v>
       </c>
     </row>
     <row r="248" spans="1:4">
@@ -20086,13 +20134,13 @@
         <v>247</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>3554</v>
+        <v>3552</v>
       </c>
       <c r="C248" s="9" t="s">
-        <v>3600</v>
+        <v>3598</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>3601</v>
+        <v>3599</v>
       </c>
     </row>
     <row r="249" spans="1:4">
@@ -20100,13 +20148,13 @@
         <v>248</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>3555</v>
+        <v>3553</v>
       </c>
       <c r="C249" s="9" t="s">
-        <v>3602</v>
+        <v>3600</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>3603</v>
+        <v>3601</v>
       </c>
     </row>
     <row r="250" spans="1:4">
@@ -20114,13 +20162,13 @@
         <v>249</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>3556</v>
+        <v>3554</v>
       </c>
       <c r="C250" s="9" t="s">
-        <v>3604</v>
+        <v>3602</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>3605</v>
+        <v>3603</v>
       </c>
     </row>
     <row r="251" spans="1:4">
@@ -20128,13 +20176,13 @@
         <v>250</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>3557</v>
+        <v>3555</v>
       </c>
       <c r="C251" s="9" t="s">
-        <v>3606</v>
+        <v>3604</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>3607</v>
+        <v>3605</v>
       </c>
     </row>
     <row r="252" spans="1:4">
@@ -20142,13 +20190,13 @@
         <v>251</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>3558</v>
+        <v>3556</v>
       </c>
       <c r="C252" s="9" t="s">
-        <v>3608</v>
+        <v>3606</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>3609</v>
+        <v>3607</v>
       </c>
     </row>
     <row r="253" spans="1:4">
@@ -20156,13 +20204,13 @@
         <v>252</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>3559</v>
+        <v>3557</v>
       </c>
       <c r="C253" s="9" t="s">
-        <v>3610</v>
+        <v>3608</v>
       </c>
       <c r="D253" s="1" t="s">
-        <v>3611</v>
+        <v>3609</v>
       </c>
     </row>
     <row r="254" spans="1:4">
@@ -20170,13 +20218,13 @@
         <v>253</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>3560</v>
+        <v>3558</v>
       </c>
       <c r="C254" s="9" t="s">
-        <v>3612</v>
+        <v>3610</v>
       </c>
       <c r="D254" s="1" t="s">
-        <v>3613</v>
+        <v>3611</v>
       </c>
     </row>
     <row r="255" spans="1:4">
@@ -20184,13 +20232,13 @@
         <v>254</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>3561</v>
+        <v>3559</v>
       </c>
       <c r="C255" s="9" t="s">
-        <v>3614</v>
+        <v>3612</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>3615</v>
+        <v>3613</v>
       </c>
     </row>
     <row r="256" spans="1:4">
@@ -20198,13 +20246,13 @@
         <v>255</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>3562</v>
+        <v>3560</v>
       </c>
       <c r="C256" s="9" t="s">
-        <v>3563</v>
+        <v>3561</v>
       </c>
       <c r="D256" s="1" t="s">
-        <v>3616</v>
+        <v>3614</v>
       </c>
     </row>
     <row r="257" spans="1:4">
@@ -20212,13 +20260,13 @@
         <v>256</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>3564</v>
+        <v>3562</v>
       </c>
       <c r="C257" s="9" t="s">
-        <v>3617</v>
+        <v>3615</v>
       </c>
       <c r="D257" s="1" t="s">
-        <v>3618</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="258" spans="1:4">
@@ -20226,13 +20274,13 @@
         <v>257</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>3565</v>
+        <v>3563</v>
       </c>
       <c r="C258" s="9" t="s">
-        <v>3619</v>
+        <v>3617</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>3620</v>
+        <v>3618</v>
       </c>
     </row>
     <row r="259" spans="1:4">
@@ -20240,13 +20288,13 @@
         <v>258</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>3566</v>
+        <v>3564</v>
       </c>
       <c r="C259" s="9" t="s">
-        <v>3621</v>
+        <v>3619</v>
       </c>
       <c r="D259" s="1" t="s">
-        <v>3622</v>
+        <v>3620</v>
       </c>
     </row>
     <row r="260" spans="1:4">
@@ -20254,13 +20302,13 @@
         <v>259</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>3567</v>
+        <v>3565</v>
       </c>
       <c r="C260" s="9" t="s">
-        <v>3623</v>
+        <v>3621</v>
       </c>
       <c r="D260" s="1" t="s">
-        <v>3624</v>
+        <v>3622</v>
       </c>
     </row>
     <row r="261" spans="1:4">
@@ -20268,13 +20316,13 @@
         <v>260</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>3568</v>
+        <v>3566</v>
       </c>
       <c r="C261" s="9" t="s">
-        <v>3625</v>
+        <v>3623</v>
       </c>
       <c r="D261" s="1" t="s">
-        <v>3626</v>
+        <v>3624</v>
       </c>
     </row>
     <row r="262" spans="1:4">
@@ -20288,7 +20336,7 @@
         <v>2486</v>
       </c>
       <c r="D262" s="1" t="s">
-        <v>3657</v>
+        <v>3655</v>
       </c>
     </row>
     <row r="263" spans="1:4">
@@ -20316,7 +20364,7 @@
         <v>2487</v>
       </c>
       <c r="D264" s="1" t="s">
-        <v>3658</v>
+        <v>3656</v>
       </c>
     </row>
     <row r="265" spans="1:4">
@@ -20330,7 +20378,7 @@
         <v>2488</v>
       </c>
       <c r="D265" s="1" t="s">
-        <v>3659</v>
+        <v>3657</v>
       </c>
     </row>
     <row r="266" spans="1:4">
@@ -20400,7 +20448,7 @@
         <v>2489</v>
       </c>
       <c r="D270" s="1" t="s">
-        <v>3660</v>
+        <v>3658</v>
       </c>
     </row>
     <row r="271" spans="1:4">
@@ -20428,7 +20476,7 @@
         <v>2491</v>
       </c>
       <c r="D272" s="1" t="s">
-        <v>3661</v>
+        <v>3659</v>
       </c>
     </row>
     <row r="273" spans="1:4">
@@ -20442,7 +20490,7 @@
         <v>2492</v>
       </c>
       <c r="D273" s="1" t="s">
-        <v>3662</v>
+        <v>3660</v>
       </c>
     </row>
     <row r="274" spans="1:4">
@@ -20456,7 +20504,7 @@
         <v>2493</v>
       </c>
       <c r="D274" s="1" t="s">
-        <v>3663</v>
+        <v>3661</v>
       </c>
     </row>
     <row r="275" spans="1:4">
@@ -20470,7 +20518,7 @@
         <v>2494</v>
       </c>
       <c r="D275" s="1" t="s">
-        <v>3664</v>
+        <v>3662</v>
       </c>
     </row>
     <row r="276" spans="1:4">
@@ -20512,7 +20560,7 @@
         <v>2495</v>
       </c>
       <c r="D278" s="1" t="s">
-        <v>3665</v>
+        <v>3663</v>
       </c>
     </row>
     <row r="279" spans="1:4">
@@ -20526,7 +20574,7 @@
         <v>2496</v>
       </c>
       <c r="D279" s="1" t="s">
-        <v>3666</v>
+        <v>3664</v>
       </c>
     </row>
     <row r="280" spans="1:4">
@@ -20554,7 +20602,7 @@
         <v>2497</v>
       </c>
       <c r="D281" s="1" t="s">
-        <v>3682</v>
+        <v>3680</v>
       </c>
     </row>
     <row r="282" spans="1:4">
@@ -20568,7 +20616,7 @@
         <v>2498</v>
       </c>
       <c r="D282" s="1" t="s">
-        <v>3683</v>
+        <v>3681</v>
       </c>
     </row>
     <row r="283" spans="1:4">
@@ -20582,7 +20630,7 @@
         <v>2499</v>
       </c>
       <c r="D283" s="1" t="s">
-        <v>3684</v>
+        <v>3682</v>
       </c>
     </row>
     <row r="284" spans="1:4">
@@ -20596,7 +20644,7 @@
         <v>2563</v>
       </c>
       <c r="D284" s="1" t="s">
-        <v>3685</v>
+        <v>3683</v>
       </c>
     </row>
     <row r="285" spans="1:4">
@@ -20610,7 +20658,7 @@
         <v>2564</v>
       </c>
       <c r="D285" s="1" t="s">
-        <v>3686</v>
+        <v>3684</v>
       </c>
     </row>
     <row r="286" spans="1:4">
@@ -20624,7 +20672,7 @@
         <v>2565</v>
       </c>
       <c r="D286" s="1" t="s">
-        <v>3687</v>
+        <v>3685</v>
       </c>
     </row>
     <row r="287" spans="1:4">
@@ -20638,7 +20686,7 @@
         <v>2566</v>
       </c>
       <c r="D287" s="1" t="s">
-        <v>3688</v>
+        <v>3686</v>
       </c>
     </row>
     <row r="288" spans="1:4">
@@ -20652,7 +20700,7 @@
         <v>2567</v>
       </c>
       <c r="D288" s="1" t="s">
-        <v>3689</v>
+        <v>3687</v>
       </c>
     </row>
     <row r="289" spans="1:4">
@@ -20666,7 +20714,7 @@
         <v>2568</v>
       </c>
       <c r="D289" s="1" t="s">
-        <v>3690</v>
+        <v>3688</v>
       </c>
     </row>
     <row r="290" spans="1:4">
@@ -20680,7 +20728,7 @@
         <v>2569</v>
       </c>
       <c r="D290" s="1" t="s">
-        <v>3691</v>
+        <v>3689</v>
       </c>
     </row>
     <row r="291" spans="1:4">
@@ -20694,7 +20742,7 @@
         <v>2570</v>
       </c>
       <c r="D291" s="1" t="s">
-        <v>3692</v>
+        <v>3690</v>
       </c>
     </row>
     <row r="292" spans="1:4">
@@ -20708,7 +20756,7 @@
         <v>2571</v>
       </c>
       <c r="D292" s="1" t="s">
-        <v>3693</v>
+        <v>3691</v>
       </c>
     </row>
     <row r="293" spans="1:4">
@@ -20722,7 +20770,7 @@
         <v>2572</v>
       </c>
       <c r="D293" s="1" t="s">
-        <v>3694</v>
+        <v>3692</v>
       </c>
     </row>
     <row r="294" spans="1:4">
@@ -20736,7 +20784,7 @@
         <v>2573</v>
       </c>
       <c r="D294" s="1" t="s">
-        <v>3695</v>
+        <v>3693</v>
       </c>
     </row>
     <row r="295" spans="1:4">
@@ -20750,7 +20798,7 @@
         <v>2574</v>
       </c>
       <c r="D295" s="1" t="s">
-        <v>3696</v>
+        <v>3694</v>
       </c>
     </row>
     <row r="296" spans="1:4">
@@ -20764,7 +20812,7 @@
         <v>2575</v>
       </c>
       <c r="D296" s="1" t="s">
-        <v>3697</v>
+        <v>3695</v>
       </c>
     </row>
     <row r="297" spans="1:4">
@@ -20778,7 +20826,7 @@
         <v>2576</v>
       </c>
       <c r="D297" s="1" t="s">
-        <v>3698</v>
+        <v>3696</v>
       </c>
     </row>
     <row r="298" spans="1:4">
@@ -20792,7 +20840,7 @@
         <v>2577</v>
       </c>
       <c r="D298" s="1" t="s">
-        <v>3699</v>
+        <v>3697</v>
       </c>
     </row>
     <row r="299" spans="1:4">
@@ -20806,7 +20854,7 @@
         <v>2578</v>
       </c>
       <c r="D299" s="1" t="s">
-        <v>3700</v>
+        <v>3698</v>
       </c>
     </row>
     <row r="300" spans="1:4">
@@ -20820,7 +20868,7 @@
         <v>2579</v>
       </c>
       <c r="D300" s="1" t="s">
-        <v>3701</v>
+        <v>3699</v>
       </c>
     </row>
     <row r="301" spans="1:4">
@@ -20834,7 +20882,7 @@
         <v>2580</v>
       </c>
       <c r="D301" s="1" t="s">
-        <v>3702</v>
+        <v>3700</v>
       </c>
     </row>
     <row r="302" spans="1:4">
@@ -20848,7 +20896,7 @@
         <v>2581</v>
       </c>
       <c r="D302" s="1" t="s">
-        <v>3703</v>
+        <v>3701</v>
       </c>
     </row>
     <row r="303" spans="1:4">
@@ -20862,7 +20910,7 @@
         <v>2582</v>
       </c>
       <c r="D303" s="1" t="s">
-        <v>3704</v>
+        <v>3702</v>
       </c>
     </row>
     <row r="304" spans="1:4">
@@ -20890,7 +20938,7 @@
         <v>2500</v>
       </c>
       <c r="D305" s="1" t="s">
-        <v>3705</v>
+        <v>3703</v>
       </c>
     </row>
     <row r="306" spans="1:4">
@@ -20904,7 +20952,7 @@
         <v>2501</v>
       </c>
       <c r="D306" s="1" t="s">
-        <v>3706</v>
+        <v>3704</v>
       </c>
     </row>
     <row r="307" spans="1:4">
@@ -20918,7 +20966,7 @@
         <v>2502</v>
       </c>
       <c r="D307" s="1" t="s">
-        <v>3707</v>
+        <v>3705</v>
       </c>
     </row>
     <row r="308" spans="1:4">
@@ -20932,7 +20980,7 @@
         <v>2503</v>
       </c>
       <c r="D308" s="1" t="s">
-        <v>3708</v>
+        <v>3706</v>
       </c>
     </row>
     <row r="309" spans="1:4">
@@ -20946,7 +20994,7 @@
         <v>2504</v>
       </c>
       <c r="D309" s="1" t="s">
-        <v>3709</v>
+        <v>3707</v>
       </c>
     </row>
     <row r="310" spans="1:4">
@@ -20960,7 +21008,7 @@
         <v>2505</v>
       </c>
       <c r="D310" s="1" t="s">
-        <v>3710</v>
+        <v>3708</v>
       </c>
     </row>
     <row r="311" spans="1:4">
@@ -20974,7 +21022,7 @@
         <v>2506</v>
       </c>
       <c r="D311" s="1" t="s">
-        <v>3711</v>
+        <v>3709</v>
       </c>
     </row>
     <row r="312" spans="1:4">
@@ -20988,7 +21036,7 @@
         <v>2507</v>
       </c>
       <c r="D312" s="1" t="s">
-        <v>3712</v>
+        <v>3710</v>
       </c>
     </row>
     <row r="313" spans="1:4">
@@ -21002,7 +21050,7 @@
         <v>2508</v>
       </c>
       <c r="D313" s="1" t="s">
-        <v>3713</v>
+        <v>3711</v>
       </c>
     </row>
     <row r="314" spans="1:4">
@@ -21016,7 +21064,7 @@
         <v>2509</v>
       </c>
       <c r="D314" s="1" t="s">
-        <v>3714</v>
+        <v>3712</v>
       </c>
     </row>
     <row r="315" spans="1:4">
@@ -21030,7 +21078,7 @@
         <v>2510</v>
       </c>
       <c r="D315" s="1" t="s">
-        <v>3715</v>
+        <v>3713</v>
       </c>
     </row>
     <row r="316" spans="1:4">
@@ -21044,7 +21092,7 @@
         <v>2511</v>
       </c>
       <c r="D316" s="1" t="s">
-        <v>3716</v>
+        <v>3714</v>
       </c>
     </row>
     <row r="317" spans="1:4">
@@ -21156,7 +21204,7 @@
         <v>2519</v>
       </c>
       <c r="D324" s="1" t="s">
-        <v>3717</v>
+        <v>3715</v>
       </c>
     </row>
     <row r="325" spans="1:4">
@@ -21268,7 +21316,7 @@
         <v>2527</v>
       </c>
       <c r="D332" s="1" t="s">
-        <v>3718</v>
+        <v>3716</v>
       </c>
     </row>
     <row r="333" spans="1:4">
@@ -21282,7 +21330,7 @@
         <v>2528</v>
       </c>
       <c r="D333" s="1" t="s">
-        <v>3719</v>
+        <v>3717</v>
       </c>
     </row>
     <row r="334" spans="1:4">
@@ -21296,7 +21344,7 @@
         <v>2529</v>
       </c>
       <c r="D334" s="1" t="s">
-        <v>3720</v>
+        <v>3718</v>
       </c>
     </row>
     <row r="335" spans="1:4">
@@ -21310,7 +21358,7 @@
         <v>2530</v>
       </c>
       <c r="D335" s="1" t="s">
-        <v>3721</v>
+        <v>3719</v>
       </c>
     </row>
     <row r="336" spans="1:4">
@@ -21324,7 +21372,7 @@
         <v>2531</v>
       </c>
       <c r="D336" s="1" t="s">
-        <v>3722</v>
+        <v>3720</v>
       </c>
     </row>
     <row r="337" spans="1:4">
@@ -21335,10 +21383,10 @@
         <v>2104</v>
       </c>
       <c r="C337" s="22" t="s">
-        <v>3723</v>
+        <v>3721</v>
       </c>
       <c r="D337" s="1" t="s">
-        <v>3735</v>
+        <v>3733</v>
       </c>
     </row>
     <row r="338" spans="1:4">
@@ -21349,10 +21397,10 @@
         <v>2105</v>
       </c>
       <c r="C338" s="22" t="s">
-        <v>3736</v>
+        <v>3734</v>
       </c>
       <c r="D338" s="1" t="s">
-        <v>3737</v>
+        <v>3735</v>
       </c>
     </row>
     <row r="339" spans="1:4">
@@ -21363,10 +21411,10 @@
         <v>2106</v>
       </c>
       <c r="C339" s="22" t="s">
-        <v>3754</v>
+        <v>3752</v>
       </c>
       <c r="D339" s="1" t="s">
-        <v>3755</v>
+        <v>3753</v>
       </c>
     </row>
     <row r="340" spans="1:4">
@@ -21377,10 +21425,10 @@
         <v>2107</v>
       </c>
       <c r="C340" s="22" t="s">
-        <v>3724</v>
+        <v>3722</v>
       </c>
       <c r="D340" s="1" t="s">
-        <v>3738</v>
+        <v>3736</v>
       </c>
     </row>
     <row r="341" spans="1:4">
@@ -21391,10 +21439,10 @@
         <v>2118</v>
       </c>
       <c r="C341" s="22" t="s">
-        <v>3725</v>
+        <v>3723</v>
       </c>
       <c r="D341" s="1" t="s">
-        <v>3739</v>
+        <v>3737</v>
       </c>
     </row>
     <row r="342" spans="1:4">
@@ -21405,10 +21453,10 @@
         <v>2108</v>
       </c>
       <c r="C342" s="22" t="s">
-        <v>3730</v>
+        <v>3728</v>
       </c>
       <c r="D342" s="1" t="s">
-        <v>3740</v>
+        <v>3738</v>
       </c>
     </row>
     <row r="343" spans="1:4">
@@ -21419,10 +21467,10 @@
         <v>2109</v>
       </c>
       <c r="C343" s="22" t="s">
-        <v>3731</v>
+        <v>3729</v>
       </c>
       <c r="D343" s="1" t="s">
-        <v>3741</v>
+        <v>3739</v>
       </c>
     </row>
     <row r="344" spans="1:4">
@@ -21433,10 +21481,10 @@
         <v>2110</v>
       </c>
       <c r="C344" s="22" t="s">
-        <v>3732</v>
+        <v>3730</v>
       </c>
       <c r="D344" s="1" t="s">
-        <v>3742</v>
+        <v>3740</v>
       </c>
     </row>
     <row r="345" spans="1:4">
@@ -21447,10 +21495,10 @@
         <v>2111</v>
       </c>
       <c r="C345" s="22" t="s">
-        <v>3733</v>
+        <v>3731</v>
       </c>
       <c r="D345" s="1" t="s">
-        <v>3743</v>
+        <v>3741</v>
       </c>
     </row>
     <row r="346" spans="1:4">
@@ -21461,10 +21509,10 @@
         <v>2112</v>
       </c>
       <c r="C346" s="22" t="s">
-        <v>3734</v>
+        <v>3732</v>
       </c>
       <c r="D346" s="1" t="s">
-        <v>3744</v>
+        <v>3742</v>
       </c>
     </row>
     <row r="347" spans="1:4">
@@ -21475,10 +21523,10 @@
         <v>2124</v>
       </c>
       <c r="C347" s="22" t="s">
-        <v>3726</v>
+        <v>3724</v>
       </c>
       <c r="D347" s="1" t="s">
-        <v>3745</v>
+        <v>3743</v>
       </c>
     </row>
     <row r="348" spans="1:4">
@@ -21489,10 +21537,10 @@
         <v>2125</v>
       </c>
       <c r="C348" s="22" t="s">
-        <v>3727</v>
+        <v>3725</v>
       </c>
       <c r="D348" s="1" t="s">
-        <v>3746</v>
+        <v>3744</v>
       </c>
     </row>
     <row r="349" spans="1:4">
@@ -21503,10 +21551,10 @@
         <v>2113</v>
       </c>
       <c r="C349" s="22" t="s">
-        <v>3728</v>
+        <v>3726</v>
       </c>
       <c r="D349" s="1" t="s">
-        <v>3747</v>
+        <v>3745</v>
       </c>
     </row>
     <row r="350" spans="1:4">
@@ -21517,10 +21565,10 @@
         <v>2171</v>
       </c>
       <c r="C350" s="22" t="s">
-        <v>3729</v>
+        <v>3727</v>
       </c>
       <c r="D350" s="22" t="s">
-        <v>3750</v>
+        <v>3748</v>
       </c>
     </row>
     <row r="351" spans="1:4">
@@ -21534,7 +21582,7 @@
         <v>2181</v>
       </c>
       <c r="D351" s="22" t="s">
-        <v>3514</v>
+        <v>3512</v>
       </c>
     </row>
     <row r="352" spans="1:4">
@@ -21548,7 +21596,7 @@
         <v>2183</v>
       </c>
       <c r="D352" s="22" t="s">
-        <v>3515</v>
+        <v>3513</v>
       </c>
     </row>
     <row r="353" spans="1:4">
@@ -21730,7 +21778,7 @@
         <v>2175</v>
       </c>
       <c r="D365" s="22" t="s">
-        <v>3751</v>
+        <v>3749</v>
       </c>
     </row>
     <row r="366" spans="1:4">
@@ -21744,7 +21792,7 @@
         <v>2177</v>
       </c>
       <c r="D366" s="22" t="s">
-        <v>3752</v>
+        <v>3750</v>
       </c>
     </row>
     <row r="367" spans="1:4">
@@ -21758,7 +21806,7 @@
         <v>2179</v>
       </c>
       <c r="D367" s="22" t="s">
-        <v>3753</v>
+        <v>3751</v>
       </c>
     </row>
     <row r="368" spans="1:4">
@@ -21786,7 +21834,7 @@
         <v>2188</v>
       </c>
       <c r="D369" s="9" t="s">
-        <v>3748</v>
+        <v>3746</v>
       </c>
     </row>
     <row r="370" spans="1:4">
@@ -21800,7 +21848,7 @@
         <v>2190</v>
       </c>
       <c r="D370" s="9" t="s">
-        <v>3749</v>
+        <v>3747</v>
       </c>
     </row>
   </sheetData>
@@ -21812,10 +21860,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FBAC76-7507-496A-9947-9F636F0BCBC6}">
-  <dimension ref="A1:D652"/>
+  <dimension ref="A1:D653"/>
   <sheetViews>
-    <sheetView topLeftCell="A566" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D585" sqref="D585"/>
+    <sheetView topLeftCell="A624" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A653" sqref="A653:XFD653"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -21830,7 +21878,7 @@
         <v>1742</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>1743</v>
+        <v>3757</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>1744</v>
@@ -25868,7 +25916,7 @@
         <v>1474</v>
       </c>
       <c r="D289" s="1" t="s">
-        <v>3513</v>
+        <v>3511</v>
       </c>
     </row>
     <row r="290" spans="1:4">
@@ -30951,6 +30999,20 @@
       </c>
       <c r="D652" s="9" t="s">
         <v>3454</v>
+      </c>
+    </row>
+    <row r="653" spans="1:4">
+      <c r="A653" s="15">
+        <v>652</v>
+      </c>
+      <c r="B653" s="5" t="s">
+        <v>3759</v>
+      </c>
+      <c r="C653" s="18" t="s">
+        <v>3756</v>
+      </c>
+      <c r="D653" s="9" t="s">
+        <v>3758</v>
       </c>
     </row>
   </sheetData>
@@ -30962,10 +31024,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -31985,6 +32047,86 @@
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="15">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>3760</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>3761</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>3768</v>
+      </c>
+      <c r="E51" s="1">
+        <v>1</v>
+      </c>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="15">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>3760</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>3765</v>
+      </c>
+      <c r="E52" s="1">
+        <v>2</v>
+      </c>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="15">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>3760</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>3766</v>
+      </c>
+      <c r="E53" s="1">
+        <v>3</v>
+      </c>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="15">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>3760</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>3764</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>3767</v>
+      </c>
+      <c r="E54" s="1">
+        <v>4</v>
+      </c>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -32058,7 +32200,7 @@
         <v>1838</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3629</v>
+        <v>3627</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>1887</v>
@@ -32110,7 +32252,7 @@
         <v>1819</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>3630</v>
+        <v>3628</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>1889</v>
@@ -32136,7 +32278,7 @@
         <v>1820</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>3631</v>
+        <v>3629</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>1890</v>
@@ -32164,7 +32306,7 @@
         <v>1821</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>3632</v>
+        <v>3630</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>1891</v>
@@ -32192,7 +32334,7 @@
         <v>1839</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>3633</v>
+        <v>3631</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>1892</v>
@@ -32220,7 +32362,7 @@
         <v>1822</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>3634</v>
+        <v>3632</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>1893</v>
@@ -32248,7 +32390,7 @@
         <v>1823</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>3635</v>
+        <v>3633</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>1894</v>
@@ -32304,7 +32446,7 @@
         <v>1824</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>3636</v>
+        <v>3634</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>1896</v>
@@ -32332,7 +32474,7 @@
         <v>1825</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>3637</v>
+        <v>3635</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>1897</v>
@@ -32360,7 +32502,7 @@
         <v>1826</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>3638</v>
+        <v>3636</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>1898</v>
@@ -32388,7 +32530,7 @@
         <v>1827</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>3639</v>
+        <v>3637</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>1899</v>
@@ -32416,7 +32558,7 @@
         <v>1828</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>3640</v>
+        <v>3638</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>1900</v>
@@ -32444,7 +32586,7 @@
         <v>1829</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>3641</v>
+        <v>3639</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>1901</v>
@@ -32472,7 +32614,7 @@
         <v>1830</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>3642</v>
+        <v>3640</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>1902</v>
@@ -32500,7 +32642,7 @@
         <v>1831</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>3643</v>
+        <v>3641</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>1903</v>
@@ -32528,7 +32670,7 @@
         <v>1841</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>3644</v>
+        <v>3642</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>1904</v>
@@ -32556,7 +32698,7 @@
         <v>1832</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>3645</v>
+        <v>3643</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>1905</v>
@@ -32584,7 +32726,7 @@
         <v>1842</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>3646</v>
+        <v>3644</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>1901</v>
@@ -32612,7 +32754,7 @@
         <v>1833</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>3647</v>
+        <v>3645</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>1906</v>
@@ -32640,7 +32782,7 @@
         <v>1834</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>3648</v>
+        <v>3646</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>1907</v>
@@ -32668,7 +32810,7 @@
         <v>1844</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>3649</v>
+        <v>3647</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>1908</v>
@@ -32696,7 +32838,7 @@
         <v>1995</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>3650</v>
+        <v>3648</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>1909</v>
@@ -32724,7 +32866,7 @@
         <v>1994</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>3651</v>
+        <v>3649</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="1"/>
@@ -32748,7 +32890,7 @@
         <v>1992</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>3652</v>
+        <v>3650</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>1910</v>
@@ -32776,7 +32918,7 @@
         <v>1993</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>3653</v>
+        <v>3651</v>
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="1"/>
@@ -32800,7 +32942,7 @@
         <v>1835</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>3654</v>
+        <v>3652</v>
       </c>
       <c r="E29" s="9" t="s">
         <v>1911</v>
@@ -32828,7 +32970,7 @@
         <v>1836</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>3655</v>
+        <v>3653</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="1"/>
@@ -32852,7 +32994,7 @@
         <v>1837</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>3656</v>
+        <v>3654</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="1"/>

</xml_diff>

<commit_message>
Organize data import and improve it
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnpc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnpc/locale/locale-en.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9157C01F-44CC-427F-BD2D-806B38C41F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46D06B2-9867-44F4-8BD4-66010B871635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4034" uniqueCount="3809">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4049" uniqueCount="3824">
   <si>
     <t>myself</t>
   </si>
@@ -14388,6 +14388,63 @@
   </si>
   <si>
     <t>Role export data</t>
+  </si>
+  <si>
+    <t>dataDictionaryExportFileName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据字典导出数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data dictionary exports data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>importOrganization</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>导入组织</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Import organization</t>
+  </si>
+  <si>
+    <t>organizationList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>组织列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>List of organizations</t>
+  </si>
+  <si>
+    <t>uploadingFile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文件上传中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>File uploading</t>
+  </si>
+  <si>
+    <t>parentNodeNoExist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>父节点不存在</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The parent node does not exist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -22033,10 +22090,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FBAC76-7507-496A-9947-9F636F0BCBC6}">
-  <dimension ref="A1:D664"/>
+  <dimension ref="A1:D669"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A646" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C670" sqref="C670"/>
+    <sheetView tabSelected="1" topLeftCell="C646" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C672" sqref="C672"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -31340,6 +31397,76 @@
       </c>
       <c r="D664" s="18" t="s">
         <v>3808</v>
+      </c>
+    </row>
+    <row r="665" spans="1:4">
+      <c r="A665" s="15">
+        <v>664</v>
+      </c>
+      <c r="B665" s="5" t="s">
+        <v>3809</v>
+      </c>
+      <c r="C665" s="18" t="s">
+        <v>3810</v>
+      </c>
+      <c r="D665" s="18" t="s">
+        <v>3811</v>
+      </c>
+    </row>
+    <row r="666" spans="1:4">
+      <c r="A666" s="15">
+        <v>665</v>
+      </c>
+      <c r="B666" s="5" t="s">
+        <v>3812</v>
+      </c>
+      <c r="C666" s="18" t="s">
+        <v>3813</v>
+      </c>
+      <c r="D666" s="9" t="s">
+        <v>3814</v>
+      </c>
+    </row>
+    <row r="667" spans="1:4">
+      <c r="A667" s="15">
+        <v>666</v>
+      </c>
+      <c r="B667" s="5" t="s">
+        <v>3815</v>
+      </c>
+      <c r="C667" s="18" t="s">
+        <v>3816</v>
+      </c>
+      <c r="D667" s="9" t="s">
+        <v>3817</v>
+      </c>
+    </row>
+    <row r="668" spans="1:4">
+      <c r="A668" s="15">
+        <v>667</v>
+      </c>
+      <c r="B668" s="5" t="s">
+        <v>3818</v>
+      </c>
+      <c r="C668" s="18" t="s">
+        <v>3819</v>
+      </c>
+      <c r="D668" s="9" t="s">
+        <v>3820</v>
+      </c>
+    </row>
+    <row r="669" spans="1:4">
+      <c r="A669" s="15">
+        <v>668</v>
+      </c>
+      <c r="B669" s="5" t="s">
+        <v>3821</v>
+      </c>
+      <c r="C669" s="18" t="s">
+        <v>3822</v>
+      </c>
+      <c r="D669" s="9" t="s">
+        <v>3823</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
When maintaining historical data, add statistical information.
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnpc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnpc/locale/locale-en.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D950FC45-8C48-4A36-8D03-61917A769DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B58211-A18F-4C7E-8C52-90CE92955A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="300" windowWidth="23256" windowHeight="12576" tabRatio="732" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4073" uniqueCount="3848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4075" uniqueCount="3850">
   <si>
     <t>myself</t>
   </si>
@@ -14597,6 +14597,14 @@
   </si>
   <si>
     <t>Import modules</t>
+  </si>
+  <si>
+    <t>运维配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O&amp;M configuration</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -22270,7 +22278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FBAC76-7507-496A-9947-9F636F0BCBC6}">
   <dimension ref="A1:D683"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D657" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A657" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="I679" sqref="I679"/>
     </sheetView>
   </sheetViews>
@@ -33878,10 +33886,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -34109,6 +34117,17 @@
       </c>
       <c r="C20" s="24" t="s">
         <v>3217</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="14">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>3848</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>3849</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Switch quantity data display adjustment
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnpc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnpc/locale/locale-en.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F3456E-461D-49DC-8DBD-9A3B09BDBA70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC70507A-73CE-424B-BF2E-E5314C519506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4261" uniqueCount="4032">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4264" uniqueCount="4035">
   <si>
     <t>myself</t>
   </si>
@@ -15277,6 +15277,18 @@
   </si>
   <si>
     <t>generalCaclualteConfig</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>showName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Display Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -22951,8 +22963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FBAC76-7507-496A-9947-9F636F0BCBC6}">
   <dimension ref="A1:D740"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B198" sqref="B198"/>
+    <sheetView tabSelected="1" topLeftCell="A714" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D740" sqref="D740"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -33309,10 +33321,18 @@
       </c>
     </row>
     <row r="740" spans="1:4">
-      <c r="A740" s="14"/>
-      <c r="B740" s="4"/>
-      <c r="C740" s="17"/>
-      <c r="D740" s="24"/>
+      <c r="A740" s="14">
+        <v>739</v>
+      </c>
+      <c r="B740" s="4" t="s">
+        <v>4032</v>
+      </c>
+      <c r="C740" s="17" t="s">
+        <v>4033</v>
+      </c>
+      <c r="D740" s="24" t="s">
+        <v>4034</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Adjustment of Switch Quantity Meaning
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnpc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnpc/locale/locale-en.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D862E867-2FB4-45F0-A650-4D890D561BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8291AA-5D03-4D6D-97B8-BA50DD0BDF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4267" uniqueCount="4038">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4273" uniqueCount="4044">
   <si>
     <t>myself</t>
   </si>
@@ -15302,6 +15302,30 @@
   </si>
   <si>
     <t>Add control group</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>switchingValueBitStatusConfig</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>位状态配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bit state configuration</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>switchingValuStatus</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -22974,10 +22998,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FBAC76-7507-496A-9947-9F636F0BCBC6}">
-  <dimension ref="A1:D741"/>
+  <dimension ref="A1:D761"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A216" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C238" sqref="C238"/>
+    <sheetView tabSelected="1" topLeftCell="A723" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B748" activeCellId="1" sqref="B743 B748"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -33360,6 +33384,142 @@
       <c r="D741" s="24" t="s">
         <v>4032</v>
       </c>
+    </row>
+    <row r="742" spans="1:4">
+      <c r="A742" s="14">
+        <v>741</v>
+      </c>
+      <c r="B742" s="4" t="s">
+        <v>4038</v>
+      </c>
+      <c r="C742" s="17" t="s">
+        <v>4039</v>
+      </c>
+      <c r="D742" s="24" t="s">
+        <v>4040</v>
+      </c>
+    </row>
+    <row r="743" spans="1:4">
+      <c r="A743" s="14">
+        <v>742</v>
+      </c>
+      <c r="B743" s="4" t="s">
+        <v>4043</v>
+      </c>
+      <c r="C743" s="17" t="s">
+        <v>4041</v>
+      </c>
+      <c r="D743" s="24" t="s">
+        <v>4042</v>
+      </c>
+    </row>
+    <row r="744" spans="1:4">
+      <c r="A744" s="14"/>
+      <c r="B744" s="4"/>
+      <c r="C744" s="17"/>
+      <c r="D744" s="24"/>
+    </row>
+    <row r="745" spans="1:4">
+      <c r="A745" s="14"/>
+      <c r="B745" s="4"/>
+      <c r="C745" s="17"/>
+      <c r="D745" s="24"/>
+    </row>
+    <row r="746" spans="1:4">
+      <c r="A746" s="14"/>
+      <c r="B746" s="4"/>
+      <c r="C746" s="17"/>
+      <c r="D746" s="24"/>
+    </row>
+    <row r="747" spans="1:4">
+      <c r="A747" s="14"/>
+      <c r="B747" s="4"/>
+      <c r="C747" s="17"/>
+      <c r="D747" s="24"/>
+    </row>
+    <row r="748" spans="1:4">
+      <c r="A748" s="14"/>
+      <c r="B748" s="4"/>
+      <c r="C748" s="17"/>
+      <c r="D748" s="24"/>
+    </row>
+    <row r="749" spans="1:4">
+      <c r="A749" s="14"/>
+      <c r="B749" s="4"/>
+      <c r="C749" s="17"/>
+      <c r="D749" s="24"/>
+    </row>
+    <row r="750" spans="1:4">
+      <c r="A750" s="14"/>
+      <c r="B750" s="4"/>
+      <c r="C750" s="17"/>
+      <c r="D750" s="24"/>
+    </row>
+    <row r="751" spans="1:4">
+      <c r="A751" s="14"/>
+      <c r="B751" s="4"/>
+      <c r="C751" s="17"/>
+      <c r="D751" s="24"/>
+    </row>
+    <row r="752" spans="1:4">
+      <c r="A752" s="14"/>
+      <c r="B752" s="4"/>
+      <c r="C752" s="17"/>
+      <c r="D752" s="24"/>
+    </row>
+    <row r="753" spans="1:4">
+      <c r="A753" s="14"/>
+      <c r="B753" s="4"/>
+      <c r="C753" s="17"/>
+      <c r="D753" s="24"/>
+    </row>
+    <row r="754" spans="1:4">
+      <c r="A754" s="14"/>
+      <c r="B754" s="4"/>
+      <c r="C754" s="17"/>
+      <c r="D754" s="24"/>
+    </row>
+    <row r="755" spans="1:4">
+      <c r="A755" s="14"/>
+      <c r="B755" s="4"/>
+      <c r="C755" s="17"/>
+      <c r="D755" s="24"/>
+    </row>
+    <row r="756" spans="1:4">
+      <c r="A756" s="14"/>
+      <c r="B756" s="4"/>
+      <c r="C756" s="17"/>
+      <c r="D756" s="24"/>
+    </row>
+    <row r="757" spans="1:4">
+      <c r="A757" s="14"/>
+      <c r="B757" s="4"/>
+      <c r="C757" s="17"/>
+      <c r="D757" s="24"/>
+    </row>
+    <row r="758" spans="1:4">
+      <c r="A758" s="14"/>
+      <c r="B758" s="4"/>
+      <c r="C758" s="17"/>
+      <c r="D758" s="24"/>
+    </row>
+    <row r="759" spans="1:4">
+      <c r="A759" s="14"/>
+      <c r="B759" s="4"/>
+      <c r="C759" s="17"/>
+      <c r="D759" s="24"/>
+    </row>
+    <row r="760" spans="1:4">
+      <c r="A760" s="14"/>
+      <c r="B760" s="4"/>
+      <c r="C760" s="17"/>
+      <c r="D760" s="24"/>
+    </row>
+    <row r="761" spans="1:4">
+      <c r="A761" s="14"/>
+      <c r="B761" s="4"/>
+      <c r="C761" s="17"/>
+      <c r="D761" s="24"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Adjustment of drive configuration
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnpc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnpc/locale/locale-en.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8291AA-5D03-4D6D-97B8-BA50DD0BDF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7192CE64-51EF-4726-AF04-FC289F7F7415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4273" uniqueCount="4044">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4282" uniqueCount="4053">
   <si>
     <t>myself</t>
   </si>
@@ -15326,6 +15326,42 @@
   </si>
   <si>
     <t>switchingValuStatus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高或低字节</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>High or low bytes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>highOrLowByte</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高字节</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>High bytes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>highByte</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lowByte</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>低字节</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Low bytes</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -23001,7 +23037,7 @@
   <dimension ref="A1:D761"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A723" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B748" activeCellId="1" sqref="B743 B748"/>
+      <selection activeCell="B749" sqref="B749"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -33414,22 +33450,46 @@
       </c>
     </row>
     <row r="744" spans="1:4">
-      <c r="A744" s="14"/>
-      <c r="B744" s="4"/>
-      <c r="C744" s="17"/>
-      <c r="D744" s="24"/>
+      <c r="A744" s="14">
+        <v>743</v>
+      </c>
+      <c r="B744" s="4" t="s">
+        <v>4046</v>
+      </c>
+      <c r="C744" s="17" t="s">
+        <v>4044</v>
+      </c>
+      <c r="D744" s="24" t="s">
+        <v>4045</v>
+      </c>
     </row>
     <row r="745" spans="1:4">
-      <c r="A745" s="14"/>
-      <c r="B745" s="4"/>
-      <c r="C745" s="17"/>
-      <c r="D745" s="24"/>
+      <c r="A745" s="14">
+        <v>744</v>
+      </c>
+      <c r="B745" s="4" t="s">
+        <v>4049</v>
+      </c>
+      <c r="C745" s="17" t="s">
+        <v>4047</v>
+      </c>
+      <c r="D745" s="24" t="s">
+        <v>4048</v>
+      </c>
     </row>
     <row r="746" spans="1:4">
-      <c r="A746" s="14"/>
-      <c r="B746" s="4"/>
-      <c r="C746" s="17"/>
-      <c r="D746" s="24"/>
+      <c r="A746" s="14">
+        <v>745</v>
+      </c>
+      <c r="B746" s="4" t="s">
+        <v>4050</v>
+      </c>
+      <c r="C746" s="17" t="s">
+        <v>4051</v>
+      </c>
+      <c r="D746" s="24" t="s">
+        <v>4052</v>
+      </c>
     </row>
     <row r="747" spans="1:4">
       <c r="A747" s="14"/>

</xml_diff>

<commit_message>
AD initialization and data processing
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnpc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnpc/locale/locale-en.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7192CE64-51EF-4726-AF04-FC289F7F7415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19B4463-0B6E-4EAC-82F0-EFEB8A715C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15337,10 +15337,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>highOrLowByte</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>高字节</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -15362,6 +15358,10 @@
   </si>
   <si>
     <t>Low bytes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>highLowByte</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -23037,7 +23037,7 @@
   <dimension ref="A1:D761"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A723" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B749" sqref="B749"/>
+      <selection activeCell="B751" sqref="B751"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -33454,7 +33454,7 @@
         <v>743</v>
       </c>
       <c r="B744" s="4" t="s">
-        <v>4046</v>
+        <v>4052</v>
       </c>
       <c r="C744" s="17" t="s">
         <v>4044</v>
@@ -33468,13 +33468,13 @@
         <v>744</v>
       </c>
       <c r="B745" s="4" t="s">
-        <v>4049</v>
+        <v>4048</v>
       </c>
       <c r="C745" s="17" t="s">
+        <v>4046</v>
+      </c>
+      <c r="D745" s="24" t="s">
         <v>4047</v>
-      </c>
-      <c r="D745" s="24" t="s">
-        <v>4048</v>
       </c>
     </row>
     <row r="746" spans="1:4">
@@ -33482,13 +33482,13 @@
         <v>745</v>
       </c>
       <c r="B746" s="4" t="s">
+        <v>4049</v>
+      </c>
+      <c r="C746" s="17" t="s">
         <v>4050</v>
       </c>
-      <c r="C746" s="17" t="s">
+      <c r="D746" s="24" t="s">
         <v>4051</v>
-      </c>
-      <c r="D746" s="24" t="s">
-        <v>4052</v>
       </c>
     </row>
     <row r="747" spans="1:4">

</xml_diff>

<commit_message>
Switch quantity data display and control adjustment
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnpc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnpc/locale/locale-en.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5E9706-E931-48B1-855A-7096005F211D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965D7226-36AC-4A4A-B3ED-EA5960607D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23050,7 +23050,7 @@
   <dimension ref="A1:D761"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A180" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D198" sqref="D198"/>
+      <selection activeCell="C198" sqref="C198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Improve the alarm function
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnpc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnpc/locale/locale-en.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B09BEB0-AF2D-4769-9598-E5986131DD80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6F658E-9975-4471-904F-AAC35B8A1398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4342" uniqueCount="4113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4348" uniqueCount="4119">
   <si>
     <t>myself</t>
   </si>
@@ -15596,6 +15596,28 @@
   <si>
     <t>alarmCount</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reportConfig</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>报表配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>offsetTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>偏移时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Report configuration</t>
+  </si>
+  <si>
+    <t>Offset time</t>
   </si>
 </sst>
 </file>
@@ -23270,7 +23292,7 @@
   <dimension ref="A1:D785"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A741" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B769" sqref="B769"/>
+      <selection activeCell="C772" sqref="C772"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -34005,16 +34027,32 @@
       </c>
     </row>
     <row r="767" spans="1:4">
-      <c r="A767" s="14"/>
-      <c r="B767" s="4"/>
-      <c r="C767" s="17"/>
-      <c r="D767" s="24"/>
+      <c r="A767" s="14">
+        <v>766</v>
+      </c>
+      <c r="B767" s="4" t="s">
+        <v>4113</v>
+      </c>
+      <c r="C767" s="17" t="s">
+        <v>4114</v>
+      </c>
+      <c r="D767" s="24" t="s">
+        <v>4117</v>
+      </c>
     </row>
     <row r="768" spans="1:4">
-      <c r="A768" s="14"/>
-      <c r="B768" s="4"/>
-      <c r="C768" s="17"/>
-      <c r="D768" s="24"/>
+      <c r="A768" s="14">
+        <v>767</v>
+      </c>
+      <c r="B768" s="4" t="s">
+        <v>4115</v>
+      </c>
+      <c r="C768" s="17" t="s">
+        <v>4116</v>
+      </c>
+      <c r="D768" s="24" t="s">
+        <v>4118</v>
+      </c>
     </row>
     <row r="769" spans="1:4">
       <c r="A769" s="14"/>

</xml_diff>

<commit_message>
Optimization of the primary device module
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnpc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnpc/locale/locale-en.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6F658E-9975-4471-904F-AAC35B8A1398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA0E955-3C19-4F0D-8D43-7476FF9AF670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4348" uniqueCount="4119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4351" uniqueCount="4122">
   <si>
     <t>myself</t>
   </si>
@@ -15610,14 +15610,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>偏移时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Report configuration</t>
   </si>
   <si>
-    <t>Offset time</t>
+    <t>一天起始时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Start time of the day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>班报表记录间隔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shift report record interval</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deviceHourlyReportInterval</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -23291,8 +23304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FBAC76-7507-496A-9947-9F636F0BCBC6}">
   <dimension ref="A1:D785"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A741" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C772" sqref="C772"/>
+    <sheetView tabSelected="1" topLeftCell="A751" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B774" sqref="B774"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -34037,7 +34050,7 @@
         <v>4114</v>
       </c>
       <c r="D767" s="24" t="s">
-        <v>4117</v>
+        <v>4116</v>
       </c>
     </row>
     <row r="768" spans="1:4">
@@ -34048,17 +34061,25 @@
         <v>4115</v>
       </c>
       <c r="C768" s="17" t="s">
-        <v>4116</v>
+        <v>4117</v>
       </c>
       <c r="D768" s="24" t="s">
         <v>4118</v>
       </c>
     </row>
     <row r="769" spans="1:4">
-      <c r="A769" s="14"/>
-      <c r="B769" s="4"/>
-      <c r="C769" s="17"/>
-      <c r="D769" s="24"/>
+      <c r="A769" s="14">
+        <v>768</v>
+      </c>
+      <c r="B769" s="4" t="s">
+        <v>4121</v>
+      </c>
+      <c r="C769" s="17" t="s">
+        <v>4119</v>
+      </c>
+      <c r="D769" s="24" t="s">
+        <v>4120</v>
+      </c>
     </row>
     <row r="770" spans="1:4">
       <c r="A770" s="14"/>

</xml_diff>

<commit_message>
System optimization and improvement
</commit_message>
<xml_diff>
--- a/WebRoot/oem/cnpc/locale/locale-en.xlsx
+++ b/WebRoot/oem/cnpc/locale/locale-en.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA0E955-3C19-4F0D-8D43-7476FF9AF670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC986DC9-71FE-4B9E-9AEC-E5B6FBAB417E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15566,26 +15566,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>数值状态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Numerical state</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>numStatusStatisticsPieChart</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>数值状态统计饼图</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Numerical state statistics pie chart</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>报警数</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -15630,6 +15614,22 @@
   </si>
   <si>
     <t>deviceHourlyReportInterval</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>报警状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alarm status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>报警状态统计饼图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alarm status statistics pie chart</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -23304,8 +23304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FBAC76-7507-496A-9947-9F636F0BCBC6}">
   <dimension ref="A1:D785"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A751" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B774" sqref="B774"/>
+    <sheetView tabSelected="1" topLeftCell="A745" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C762" sqref="C762"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -23519,10 +23519,10 @@
         <v>4104</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>4105</v>
+        <v>4118</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>4106</v>
+        <v>4119</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -33974,13 +33974,13 @@
         <v>761</v>
       </c>
       <c r="B762" s="4" t="s">
-        <v>4107</v>
+        <v>4105</v>
       </c>
       <c r="C762" s="17" t="s">
-        <v>4108</v>
+        <v>4120</v>
       </c>
       <c r="D762" s="24" t="s">
-        <v>4109</v>
+        <v>4121</v>
       </c>
     </row>
     <row r="763" spans="1:4">
@@ -34030,13 +34030,13 @@
         <v>765</v>
       </c>
       <c r="B766" s="4" t="s">
-        <v>4112</v>
+        <v>4108</v>
       </c>
       <c r="C766" s="17" t="s">
-        <v>4110</v>
+        <v>4106</v>
       </c>
       <c r="D766" s="24" t="s">
-        <v>4111</v>
+        <v>4107</v>
       </c>
     </row>
     <row r="767" spans="1:4">
@@ -34044,13 +34044,13 @@
         <v>766</v>
       </c>
       <c r="B767" s="4" t="s">
-        <v>4113</v>
+        <v>4109</v>
       </c>
       <c r="C767" s="17" t="s">
-        <v>4114</v>
+        <v>4110</v>
       </c>
       <c r="D767" s="24" t="s">
-        <v>4116</v>
+        <v>4112</v>
       </c>
     </row>
     <row r="768" spans="1:4">
@@ -34058,13 +34058,13 @@
         <v>767</v>
       </c>
       <c r="B768" s="4" t="s">
-        <v>4115</v>
+        <v>4111</v>
       </c>
       <c r="C768" s="17" t="s">
-        <v>4117</v>
+        <v>4113</v>
       </c>
       <c r="D768" s="24" t="s">
-        <v>4118</v>
+        <v>4114</v>
       </c>
     </row>
     <row r="769" spans="1:4">
@@ -34072,13 +34072,13 @@
         <v>768</v>
       </c>
       <c r="B769" s="4" t="s">
-        <v>4121</v>
+        <v>4117</v>
       </c>
       <c r="C769" s="17" t="s">
-        <v>4119</v>
+        <v>4115</v>
       </c>
       <c r="D769" s="24" t="s">
-        <v>4120</v>
+        <v>4116</v>
       </c>
     </row>
     <row r="770" spans="1:4">

</xml_diff>